<commit_message>
Revised document naming rules to be consistent
</commit_message>
<xml_diff>
--- a/en/Sample_Project/Design_Document/B1_Client_Management_System/030_Application_Design/010_System_Functional_Design/System_Function_List_B1_Client_Management_System.xlsx
+++ b/en/Sample_Project/Design_Document/B1_Client_Management_System/030_Application_Design/010_System_Functional_Design/System_Function_List_B1_Client_Management_System.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0853D7-356A-46B1-A8C8-E661A5E56073}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676C98C8-7980-44F9-BA49-3DB4728EA6CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="360" windowWidth="27090" windowHeight="10830" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="17" r:id="rId1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -794,257 +792,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1065,6 +814,58 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1074,6 +875,15 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1092,49 +902,165 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1144,14 +1070,86 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1894,12 +1892,12 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="68">
+      <c r="I25" s="78">
         <f ca="1">IF(INDIRECT("'Revision history'!D8")="","",MAX(INDIRECT("'Revision history'!D8"):INDIRECT("'Revision history'!F33")))</f>
         <v>43404</v>
       </c>
-      <c r="J25" s="68"/>
-      <c r="K25" s="68"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
     </row>
     <row r="26" spans="6:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F26" s="6"/>
@@ -2496,55 +2494,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="72" t="s">
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="78" t="s">
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="119" t="s">
+      <c r="P1" s="124"/>
+      <c r="Q1" s="124"/>
+      <c r="R1" s="125"/>
+      <c r="S1" s="132" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="120"/>
-      <c r="U1" s="120"/>
-      <c r="V1" s="120"/>
-      <c r="W1" s="120"/>
-      <c r="X1" s="120"/>
-      <c r="Y1" s="120"/>
-      <c r="Z1" s="121"/>
-      <c r="AA1" s="75" t="s">
+      <c r="T1" s="133"/>
+      <c r="U1" s="133"/>
+      <c r="V1" s="133"/>
+      <c r="W1" s="133"/>
+      <c r="X1" s="133"/>
+      <c r="Y1" s="133"/>
+      <c r="Z1" s="134"/>
+      <c r="AA1" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="69" t="s">
+      <c r="AB1" s="116"/>
+      <c r="AC1" s="141" t="s">
         <v>2</v>
       </c>
-      <c r="AD1" s="70"/>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="71"/>
-      <c r="AG1" s="146">
+      <c r="AD1" s="142"/>
+      <c r="AE1" s="142"/>
+      <c r="AF1" s="143"/>
+      <c r="AG1" s="106">
         <v>43404</v>
       </c>
-      <c r="AH1" s="147"/>
-      <c r="AI1" s="148"/>
+      <c r="AH1" s="107"/>
+      <c r="AI1" s="108"/>
       <c r="AJ1" s="17"/>
       <c r="AK1" s="17"/>
       <c r="AL1" s="17"/>
@@ -2552,53 +2550,53 @@
       <c r="AN1" s="26"/>
     </row>
     <row r="2" spans="1:40" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="72" t="s">
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="134"/>
-      <c r="Q2" s="134"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="127"/>
-      <c r="AA2" s="75" t="s">
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="126"/>
+      <c r="P2" s="127"/>
+      <c r="Q2" s="127"/>
+      <c r="R2" s="128"/>
+      <c r="S2" s="135"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="136"/>
+      <c r="V2" s="136"/>
+      <c r="W2" s="136"/>
+      <c r="X2" s="136"/>
+      <c r="Y2" s="136"/>
+      <c r="Z2" s="137"/>
+      <c r="AA2" s="114" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="149" t="str">
+      <c r="AB2" s="116"/>
+      <c r="AC2" s="120" t="str">
         <f ca="1">IF(COUNTA(AF9:AF33)&lt;&gt;0,INDIRECT("AF"&amp;(COUNTA(AF9:AF33)+8)),"")</f>
         <v/>
       </c>
-      <c r="AD2" s="150"/>
-      <c r="AE2" s="150"/>
-      <c r="AF2" s="151"/>
-      <c r="AG2" s="146" t="str">
+      <c r="AD2" s="121"/>
+      <c r="AE2" s="121"/>
+      <c r="AF2" s="122"/>
+      <c r="AG2" s="106" t="str">
         <f>IF(D9="","",MAX(D9:F33))</f>
         <v/>
       </c>
-      <c r="AH2" s="147"/>
-      <c r="AI2" s="148"/>
+      <c r="AH2" s="107"/>
+      <c r="AI2" s="108"/>
       <c r="AJ2" s="17"/>
       <c r="AK2" s="17"/>
       <c r="AL2" s="17"/>
@@ -2606,1265 +2604,1109 @@
       <c r="AN2" s="17"/>
     </row>
     <row r="3" spans="1:40" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="114" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="72" t="s">
+      <c r="B3" s="115"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="131"/>
-      <c r="T3" s="132"/>
-      <c r="U3" s="132"/>
-      <c r="V3" s="132"/>
-      <c r="W3" s="132"/>
-      <c r="X3" s="132"/>
-      <c r="Y3" s="132"/>
-      <c r="Z3" s="133"/>
-      <c r="AA3" s="75"/>
-      <c r="AB3" s="77"/>
-      <c r="AC3" s="69"/>
-      <c r="AD3" s="70"/>
-      <c r="AE3" s="70"/>
-      <c r="AF3" s="71"/>
-      <c r="AG3" s="146"/>
-      <c r="AH3" s="147"/>
-      <c r="AI3" s="148"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="129"/>
+      <c r="P3" s="130"/>
+      <c r="Q3" s="130"/>
+      <c r="R3" s="131"/>
+      <c r="S3" s="138"/>
+      <c r="T3" s="139"/>
+      <c r="U3" s="139"/>
+      <c r="V3" s="139"/>
+      <c r="W3" s="139"/>
+      <c r="X3" s="139"/>
+      <c r="Y3" s="139"/>
+      <c r="Z3" s="140"/>
+      <c r="AA3" s="114"/>
+      <c r="AB3" s="116"/>
+      <c r="AC3" s="141"/>
+      <c r="AD3" s="142"/>
+      <c r="AE3" s="142"/>
+      <c r="AF3" s="143"/>
+      <c r="AG3" s="106"/>
+      <c r="AH3" s="107"/>
+      <c r="AI3" s="108"/>
       <c r="AJ3" s="17"/>
       <c r="AK3" s="17"/>
       <c r="AL3" s="17"/>
       <c r="AM3" s="17"/>
       <c r="AN3" s="17"/>
     </row>
-    <row r="5" spans="1:40" s="152" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N5" s="153" t="s">
+    <row r="5" spans="1:40" s="69" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="AA5" s="154"/>
-      <c r="AB5" s="154"/>
-      <c r="AC5" s="155"/>
-      <c r="AD5" s="156"/>
-      <c r="AE5" s="156"/>
-      <c r="AF5" s="156"/>
-      <c r="AG5" s="154"/>
-      <c r="AH5" s="154"/>
-      <c r="AI5" s="154"/>
-    </row>
-    <row r="6" spans="1:40" s="152" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N6" s="153"/>
-      <c r="AA6" s="154"/>
-      <c r="AB6" s="154"/>
-      <c r="AC6" s="155"/>
-      <c r="AD6" s="156"/>
-      <c r="AE6" s="156"/>
-      <c r="AF6" s="156"/>
-      <c r="AG6" s="154"/>
-      <c r="AH6" s="154"/>
-      <c r="AI6" s="154"/>
-    </row>
-    <row r="7" spans="1:40" s="157" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="135" t="s">
+      <c r="AA5" s="71"/>
+      <c r="AB5" s="71"/>
+      <c r="AC5" s="72"/>
+      <c r="AD5" s="73"/>
+      <c r="AE5" s="73"/>
+      <c r="AF5" s="73"/>
+      <c r="AG5" s="71"/>
+      <c r="AH5" s="71"/>
+      <c r="AI5" s="71"/>
+    </row>
+    <row r="6" spans="1:40" s="69" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="70"/>
+      <c r="AA6" s="71"/>
+      <c r="AB6" s="71"/>
+      <c r="AC6" s="72"/>
+      <c r="AD6" s="73"/>
+      <c r="AE6" s="73"/>
+      <c r="AF6" s="73"/>
+      <c r="AG6" s="71"/>
+      <c r="AH6" s="71"/>
+      <c r="AI6" s="71"/>
+    </row>
+    <row r="7" spans="1:40" s="74" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="136" t="s">
+      <c r="B7" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="137"/>
-      <c r="D7" s="138" t="s">
+      <c r="C7" s="110"/>
+      <c r="D7" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="139"/>
-      <c r="F7" s="140"/>
-      <c r="G7" s="138" t="s">
+      <c r="E7" s="112"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="139"/>
-      <c r="I7" s="140"/>
-      <c r="J7" s="138" t="s">
+      <c r="H7" s="112"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="139"/>
-      <c r="L7" s="139"/>
-      <c r="M7" s="139"/>
-      <c r="N7" s="139"/>
-      <c r="O7" s="139"/>
-      <c r="P7" s="140"/>
-      <c r="Q7" s="138" t="s">
+      <c r="K7" s="112"/>
+      <c r="L7" s="112"/>
+      <c r="M7" s="112"/>
+      <c r="N7" s="112"/>
+      <c r="O7" s="112"/>
+      <c r="P7" s="113"/>
+      <c r="Q7" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="R7" s="139"/>
-      <c r="S7" s="139"/>
-      <c r="T7" s="139"/>
-      <c r="U7" s="139"/>
-      <c r="V7" s="139"/>
-      <c r="W7" s="139"/>
-      <c r="X7" s="139"/>
-      <c r="Y7" s="139"/>
-      <c r="Z7" s="139"/>
-      <c r="AA7" s="139"/>
-      <c r="AB7" s="139"/>
-      <c r="AC7" s="139"/>
-      <c r="AD7" s="139"/>
-      <c r="AE7" s="140"/>
-      <c r="AF7" s="138" t="s">
+      <c r="R7" s="112"/>
+      <c r="S7" s="112"/>
+      <c r="T7" s="112"/>
+      <c r="U7" s="112"/>
+      <c r="V7" s="112"/>
+      <c r="W7" s="112"/>
+      <c r="X7" s="112"/>
+      <c r="Y7" s="112"/>
+      <c r="Z7" s="112"/>
+      <c r="AA7" s="112"/>
+      <c r="AB7" s="112"/>
+      <c r="AC7" s="112"/>
+      <c r="AD7" s="112"/>
+      <c r="AE7" s="113"/>
+      <c r="AF7" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="AG7" s="139"/>
-      <c r="AH7" s="139"/>
-      <c r="AI7" s="140"/>
-    </row>
-    <row r="8" spans="1:40" s="157" customFormat="1" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="158">
+      <c r="AG7" s="112"/>
+      <c r="AH7" s="112"/>
+      <c r="AI7" s="113"/>
+    </row>
+    <row r="8" spans="1:40" s="74" customFormat="1" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="75">
         <v>1</v>
       </c>
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="142"/>
-      <c r="D8" s="159">
+      <c r="C8" s="93"/>
+      <c r="D8" s="94">
         <v>43404</v>
       </c>
-      <c r="E8" s="160"/>
-      <c r="F8" s="161"/>
-      <c r="G8" s="143" t="s">
+      <c r="E8" s="95"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="144"/>
-      <c r="I8" s="145"/>
-      <c r="J8" s="162" t="s">
+      <c r="H8" s="98"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="163"/>
-      <c r="L8" s="163"/>
-      <c r="M8" s="163"/>
-      <c r="N8" s="163"/>
-      <c r="O8" s="163"/>
-      <c r="P8" s="164"/>
-      <c r="Q8" s="165" t="s">
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
+      <c r="M8" s="101"/>
+      <c r="N8" s="101"/>
+      <c r="O8" s="101"/>
+      <c r="P8" s="102"/>
+      <c r="Q8" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="R8" s="166"/>
-      <c r="S8" s="166"/>
-      <c r="T8" s="166"/>
-      <c r="U8" s="166"/>
-      <c r="V8" s="166"/>
-      <c r="W8" s="166"/>
-      <c r="X8" s="166"/>
-      <c r="Y8" s="166"/>
-      <c r="Z8" s="166"/>
-      <c r="AA8" s="166"/>
-      <c r="AB8" s="166"/>
-      <c r="AC8" s="166"/>
-      <c r="AD8" s="166"/>
-      <c r="AE8" s="167"/>
-      <c r="AF8" s="162" t="s">
+      <c r="R8" s="104"/>
+      <c r="S8" s="104"/>
+      <c r="T8" s="104"/>
+      <c r="U8" s="104"/>
+      <c r="V8" s="104"/>
+      <c r="W8" s="104"/>
+      <c r="X8" s="104"/>
+      <c r="Y8" s="104"/>
+      <c r="Z8" s="104"/>
+      <c r="AA8" s="104"/>
+      <c r="AB8" s="104"/>
+      <c r="AC8" s="104"/>
+      <c r="AD8" s="104"/>
+      <c r="AE8" s="105"/>
+      <c r="AF8" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="AG8" s="163"/>
-      <c r="AH8" s="163"/>
-      <c r="AI8" s="164"/>
-    </row>
-    <row r="9" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="168"/>
-      <c r="B9" s="169"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="171"/>
-      <c r="E9" s="172"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="174"/>
-      <c r="I9" s="170"/>
-      <c r="J9" s="175"/>
-      <c r="K9" s="176"/>
-      <c r="L9" s="176"/>
-      <c r="M9" s="176"/>
-      <c r="N9" s="176"/>
-      <c r="O9" s="176"/>
-      <c r="P9" s="177"/>
-      <c r="Q9" s="178"/>
-      <c r="R9" s="179"/>
-      <c r="S9" s="179"/>
-      <c r="T9" s="179"/>
-      <c r="U9" s="179"/>
-      <c r="V9" s="179"/>
-      <c r="W9" s="179"/>
-      <c r="X9" s="179"/>
-      <c r="Y9" s="179"/>
-      <c r="Z9" s="179"/>
-      <c r="AA9" s="179"/>
-      <c r="AB9" s="179"/>
-      <c r="AC9" s="179"/>
-      <c r="AD9" s="179"/>
-      <c r="AE9" s="180"/>
-      <c r="AF9" s="175"/>
-      <c r="AG9" s="176"/>
-      <c r="AH9" s="176"/>
-      <c r="AI9" s="177"/>
-    </row>
-    <row r="10" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="168"/>
-      <c r="B10" s="169"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="171"/>
-      <c r="E10" s="172"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="169"/>
-      <c r="H10" s="174"/>
-      <c r="I10" s="170"/>
-      <c r="J10" s="175"/>
-      <c r="K10" s="176"/>
-      <c r="L10" s="176"/>
-      <c r="M10" s="176"/>
-      <c r="N10" s="176"/>
-      <c r="O10" s="176"/>
-      <c r="P10" s="177"/>
-      <c r="Q10" s="178"/>
-      <c r="R10" s="179"/>
-      <c r="S10" s="179"/>
-      <c r="T10" s="179"/>
-      <c r="U10" s="179"/>
-      <c r="V10" s="179"/>
-      <c r="W10" s="179"/>
-      <c r="X10" s="179"/>
-      <c r="Y10" s="179"/>
-      <c r="Z10" s="179"/>
-      <c r="AA10" s="179"/>
-      <c r="AB10" s="179"/>
-      <c r="AC10" s="179"/>
-      <c r="AD10" s="179"/>
-      <c r="AE10" s="180"/>
-      <c r="AF10" s="175"/>
-      <c r="AG10" s="176"/>
-      <c r="AH10" s="176"/>
-      <c r="AI10" s="177"/>
-    </row>
-    <row r="11" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="168"/>
-      <c r="B11" s="169"/>
-      <c r="C11" s="170"/>
-      <c r="D11" s="171"/>
-      <c r="E11" s="172"/>
-      <c r="F11" s="173"/>
-      <c r="G11" s="169"/>
-      <c r="H11" s="174"/>
-      <c r="I11" s="170"/>
-      <c r="J11" s="175"/>
-      <c r="K11" s="176"/>
-      <c r="L11" s="176"/>
-      <c r="M11" s="176"/>
-      <c r="N11" s="176"/>
-      <c r="O11" s="176"/>
-      <c r="P11" s="177"/>
-      <c r="Q11" s="178"/>
-      <c r="R11" s="179"/>
-      <c r="S11" s="179"/>
-      <c r="T11" s="179"/>
-      <c r="U11" s="179"/>
-      <c r="V11" s="179"/>
-      <c r="W11" s="179"/>
-      <c r="X11" s="179"/>
-      <c r="Y11" s="179"/>
-      <c r="Z11" s="179"/>
-      <c r="AA11" s="179"/>
-      <c r="AB11" s="179"/>
-      <c r="AC11" s="179"/>
-      <c r="AD11" s="179"/>
-      <c r="AE11" s="180"/>
-      <c r="AF11" s="175"/>
-      <c r="AG11" s="176"/>
-      <c r="AH11" s="176"/>
-      <c r="AI11" s="177"/>
-    </row>
-    <row r="12" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="168"/>
-      <c r="B12" s="169"/>
-      <c r="C12" s="170"/>
-      <c r="D12" s="171"/>
-      <c r="E12" s="172"/>
-      <c r="F12" s="173"/>
-      <c r="G12" s="169"/>
-      <c r="H12" s="174"/>
-      <c r="I12" s="170"/>
-      <c r="J12" s="175"/>
-      <c r="K12" s="176"/>
-      <c r="L12" s="176"/>
-      <c r="M12" s="176"/>
-      <c r="N12" s="176"/>
-      <c r="O12" s="176"/>
-      <c r="P12" s="177"/>
-      <c r="Q12" s="178"/>
-      <c r="R12" s="179"/>
-      <c r="S12" s="179"/>
-      <c r="T12" s="179"/>
-      <c r="U12" s="179"/>
-      <c r="V12" s="179"/>
-      <c r="W12" s="179"/>
-      <c r="X12" s="179"/>
-      <c r="Y12" s="179"/>
-      <c r="Z12" s="179"/>
-      <c r="AA12" s="179"/>
-      <c r="AB12" s="179"/>
-      <c r="AC12" s="179"/>
-      <c r="AD12" s="179"/>
-      <c r="AE12" s="180"/>
-      <c r="AF12" s="175"/>
-      <c r="AG12" s="176"/>
-      <c r="AH12" s="176"/>
-      <c r="AI12" s="177"/>
-    </row>
-    <row r="13" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="168"/>
-      <c r="B13" s="169"/>
-      <c r="C13" s="170"/>
-      <c r="D13" s="171"/>
-      <c r="E13" s="172"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="169"/>
-      <c r="H13" s="174"/>
-      <c r="I13" s="170"/>
-      <c r="J13" s="175"/>
-      <c r="K13" s="176"/>
-      <c r="L13" s="176"/>
-      <c r="M13" s="176"/>
-      <c r="N13" s="176"/>
-      <c r="O13" s="176"/>
-      <c r="P13" s="177"/>
-      <c r="Q13" s="178"/>
-      <c r="R13" s="179"/>
-      <c r="S13" s="179"/>
-      <c r="T13" s="179"/>
-      <c r="U13" s="179"/>
-      <c r="V13" s="179"/>
-      <c r="W13" s="179"/>
-      <c r="X13" s="179"/>
-      <c r="Y13" s="179"/>
-      <c r="Z13" s="179"/>
-      <c r="AA13" s="179"/>
-      <c r="AB13" s="179"/>
-      <c r="AC13" s="179"/>
-      <c r="AD13" s="179"/>
-      <c r="AE13" s="180"/>
-      <c r="AF13" s="175"/>
-      <c r="AG13" s="176"/>
-      <c r="AH13" s="176"/>
-      <c r="AI13" s="177"/>
-    </row>
-    <row r="14" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="168"/>
-      <c r="B14" s="169"/>
-      <c r="C14" s="170"/>
-      <c r="D14" s="171"/>
-      <c r="E14" s="172"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="169"/>
-      <c r="H14" s="174"/>
-      <c r="I14" s="170"/>
-      <c r="J14" s="175"/>
-      <c r="K14" s="176"/>
-      <c r="L14" s="176"/>
-      <c r="M14" s="176"/>
-      <c r="N14" s="176"/>
-      <c r="O14" s="176"/>
-      <c r="P14" s="177"/>
-      <c r="Q14" s="178"/>
-      <c r="R14" s="179"/>
-      <c r="S14" s="179"/>
-      <c r="T14" s="179"/>
-      <c r="U14" s="179"/>
-      <c r="V14" s="179"/>
-      <c r="W14" s="179"/>
-      <c r="X14" s="179"/>
-      <c r="Y14" s="179"/>
-      <c r="Z14" s="179"/>
-      <c r="AA14" s="179"/>
-      <c r="AB14" s="179"/>
-      <c r="AC14" s="179"/>
-      <c r="AD14" s="179"/>
-      <c r="AE14" s="180"/>
-      <c r="AF14" s="175"/>
-      <c r="AG14" s="176"/>
-      <c r="AH14" s="176"/>
-      <c r="AI14" s="177"/>
-    </row>
-    <row r="15" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="168"/>
-      <c r="B15" s="169"/>
-      <c r="C15" s="170"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="169"/>
-      <c r="H15" s="174"/>
-      <c r="I15" s="170"/>
-      <c r="J15" s="175"/>
-      <c r="K15" s="176"/>
-      <c r="L15" s="176"/>
-      <c r="M15" s="176"/>
-      <c r="N15" s="176"/>
-      <c r="O15" s="176"/>
-      <c r="P15" s="177"/>
-      <c r="Q15" s="178"/>
-      <c r="R15" s="179"/>
-      <c r="S15" s="179"/>
-      <c r="T15" s="179"/>
-      <c r="U15" s="179"/>
-      <c r="V15" s="179"/>
-      <c r="W15" s="179"/>
-      <c r="X15" s="179"/>
-      <c r="Y15" s="179"/>
-      <c r="Z15" s="179"/>
-      <c r="AA15" s="179"/>
-      <c r="AB15" s="179"/>
-      <c r="AC15" s="179"/>
-      <c r="AD15" s="179"/>
-      <c r="AE15" s="180"/>
-      <c r="AF15" s="175"/>
-      <c r="AG15" s="176"/>
-      <c r="AH15" s="176"/>
-      <c r="AI15" s="177"/>
-    </row>
-    <row r="16" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="168"/>
-      <c r="B16" s="169"/>
-      <c r="C16" s="170"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="169"/>
-      <c r="H16" s="174"/>
-      <c r="I16" s="170"/>
-      <c r="J16" s="175"/>
-      <c r="K16" s="176"/>
-      <c r="L16" s="176"/>
-      <c r="M16" s="176"/>
-      <c r="N16" s="176"/>
-      <c r="O16" s="176"/>
-      <c r="P16" s="177"/>
-      <c r="Q16" s="178"/>
-      <c r="R16" s="179"/>
-      <c r="S16" s="179"/>
-      <c r="T16" s="179"/>
-      <c r="U16" s="179"/>
-      <c r="V16" s="179"/>
-      <c r="W16" s="179"/>
-      <c r="X16" s="179"/>
-      <c r="Y16" s="179"/>
-      <c r="Z16" s="179"/>
-      <c r="AA16" s="179"/>
-      <c r="AB16" s="179"/>
-      <c r="AC16" s="179"/>
-      <c r="AD16" s="179"/>
-      <c r="AE16" s="180"/>
-      <c r="AF16" s="175"/>
-      <c r="AG16" s="176"/>
-      <c r="AH16" s="176"/>
-      <c r="AI16" s="177"/>
-    </row>
-    <row r="17" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="168"/>
-      <c r="B17" s="169"/>
-      <c r="C17" s="170"/>
-      <c r="D17" s="171"/>
-      <c r="E17" s="172"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="169"/>
-      <c r="H17" s="174"/>
-      <c r="I17" s="170"/>
-      <c r="J17" s="175"/>
-      <c r="K17" s="176"/>
-      <c r="L17" s="176"/>
-      <c r="M17" s="176"/>
-      <c r="N17" s="176"/>
-      <c r="O17" s="176"/>
-      <c r="P17" s="177"/>
-      <c r="Q17" s="178"/>
-      <c r="R17" s="179"/>
-      <c r="S17" s="179"/>
-      <c r="T17" s="179"/>
-      <c r="U17" s="179"/>
-      <c r="V17" s="179"/>
-      <c r="W17" s="179"/>
-      <c r="X17" s="179"/>
-      <c r="Y17" s="179"/>
-      <c r="Z17" s="179"/>
-      <c r="AA17" s="179"/>
-      <c r="AB17" s="179"/>
-      <c r="AC17" s="179"/>
-      <c r="AD17" s="179"/>
-      <c r="AE17" s="180"/>
-      <c r="AF17" s="175"/>
-      <c r="AG17" s="176"/>
-      <c r="AH17" s="176"/>
-      <c r="AI17" s="177"/>
-    </row>
-    <row r="18" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="168"/>
-      <c r="B18" s="169"/>
-      <c r="C18" s="170"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
-      <c r="F18" s="173"/>
-      <c r="G18" s="169"/>
-      <c r="H18" s="174"/>
-      <c r="I18" s="170"/>
-      <c r="J18" s="175"/>
-      <c r="K18" s="176"/>
-      <c r="L18" s="176"/>
-      <c r="M18" s="176"/>
-      <c r="N18" s="176"/>
-      <c r="O18" s="176"/>
-      <c r="P18" s="177"/>
-      <c r="Q18" s="178"/>
-      <c r="R18" s="179"/>
-      <c r="S18" s="179"/>
-      <c r="T18" s="179"/>
-      <c r="U18" s="179"/>
-      <c r="V18" s="179"/>
-      <c r="W18" s="179"/>
-      <c r="X18" s="179"/>
-      <c r="Y18" s="179"/>
-      <c r="Z18" s="179"/>
-      <c r="AA18" s="179"/>
-      <c r="AB18" s="179"/>
-      <c r="AC18" s="179"/>
-      <c r="AD18" s="179"/>
-      <c r="AE18" s="180"/>
-      <c r="AF18" s="175"/>
-      <c r="AG18" s="176"/>
-      <c r="AH18" s="176"/>
-      <c r="AI18" s="177"/>
-    </row>
-    <row r="19" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="168"/>
-      <c r="B19" s="169"/>
-      <c r="C19" s="170"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
-      <c r="F19" s="173"/>
-      <c r="G19" s="169"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="170"/>
-      <c r="J19" s="175"/>
-      <c r="K19" s="176"/>
-      <c r="L19" s="176"/>
-      <c r="M19" s="176"/>
-      <c r="N19" s="176"/>
-      <c r="O19" s="176"/>
-      <c r="P19" s="177"/>
-      <c r="Q19" s="178"/>
-      <c r="R19" s="179"/>
-      <c r="S19" s="179"/>
-      <c r="T19" s="179"/>
-      <c r="U19" s="179"/>
-      <c r="V19" s="179"/>
-      <c r="W19" s="179"/>
-      <c r="X19" s="179"/>
-      <c r="Y19" s="179"/>
-      <c r="Z19" s="179"/>
-      <c r="AA19" s="179"/>
-      <c r="AB19" s="179"/>
-      <c r="AC19" s="179"/>
-      <c r="AD19" s="179"/>
-      <c r="AE19" s="180"/>
-      <c r="AF19" s="175"/>
-      <c r="AG19" s="176"/>
-      <c r="AH19" s="176"/>
-      <c r="AI19" s="177"/>
-    </row>
-    <row r="20" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="168"/>
-      <c r="B20" s="169"/>
-      <c r="C20" s="170"/>
-      <c r="D20" s="171"/>
-      <c r="E20" s="172"/>
-      <c r="F20" s="173"/>
-      <c r="G20" s="169"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="170"/>
-      <c r="J20" s="175"/>
-      <c r="K20" s="176"/>
-      <c r="L20" s="176"/>
-      <c r="M20" s="176"/>
-      <c r="N20" s="176"/>
-      <c r="O20" s="176"/>
-      <c r="P20" s="177"/>
-      <c r="Q20" s="178"/>
-      <c r="R20" s="179"/>
-      <c r="S20" s="179"/>
-      <c r="T20" s="179"/>
-      <c r="U20" s="179"/>
-      <c r="V20" s="179"/>
-      <c r="W20" s="179"/>
-      <c r="X20" s="179"/>
-      <c r="Y20" s="179"/>
-      <c r="Z20" s="179"/>
-      <c r="AA20" s="179"/>
-      <c r="AB20" s="179"/>
-      <c r="AC20" s="179"/>
-      <c r="AD20" s="179"/>
-      <c r="AE20" s="180"/>
-      <c r="AF20" s="175"/>
-      <c r="AG20" s="176"/>
-      <c r="AH20" s="176"/>
-      <c r="AI20" s="177"/>
-    </row>
-    <row r="21" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="168"/>
-      <c r="B21" s="169"/>
-      <c r="C21" s="170"/>
-      <c r="D21" s="171"/>
-      <c r="E21" s="172"/>
-      <c r="F21" s="173"/>
-      <c r="G21" s="169"/>
-      <c r="H21" s="174"/>
-      <c r="I21" s="170"/>
-      <c r="J21" s="175"/>
-      <c r="K21" s="176"/>
-      <c r="L21" s="176"/>
-      <c r="M21" s="176"/>
-      <c r="N21" s="176"/>
-      <c r="O21" s="176"/>
-      <c r="P21" s="177"/>
-      <c r="Q21" s="178"/>
-      <c r="R21" s="179"/>
-      <c r="S21" s="179"/>
-      <c r="T21" s="179"/>
-      <c r="U21" s="179"/>
-      <c r="V21" s="179"/>
-      <c r="W21" s="179"/>
-      <c r="X21" s="179"/>
-      <c r="Y21" s="179"/>
-      <c r="Z21" s="179"/>
-      <c r="AA21" s="179"/>
-      <c r="AB21" s="179"/>
-      <c r="AC21" s="179"/>
-      <c r="AD21" s="179"/>
-      <c r="AE21" s="180"/>
-      <c r="AF21" s="175"/>
-      <c r="AG21" s="176"/>
-      <c r="AH21" s="176"/>
-      <c r="AI21" s="177"/>
-    </row>
-    <row r="22" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="168"/>
-      <c r="B22" s="169"/>
-      <c r="C22" s="170"/>
-      <c r="D22" s="171"/>
-      <c r="E22" s="172"/>
-      <c r="F22" s="173"/>
-      <c r="G22" s="169"/>
-      <c r="H22" s="174"/>
-      <c r="I22" s="170"/>
-      <c r="J22" s="175"/>
-      <c r="K22" s="176"/>
-      <c r="L22" s="176"/>
-      <c r="M22" s="176"/>
-      <c r="N22" s="176"/>
-      <c r="O22" s="176"/>
-      <c r="P22" s="177"/>
-      <c r="Q22" s="178"/>
-      <c r="R22" s="179"/>
-      <c r="S22" s="179"/>
-      <c r="T22" s="179"/>
-      <c r="U22" s="179"/>
-      <c r="V22" s="179"/>
-      <c r="W22" s="179"/>
-      <c r="X22" s="179"/>
-      <c r="Y22" s="179"/>
-      <c r="Z22" s="179"/>
-      <c r="AA22" s="179"/>
-      <c r="AB22" s="179"/>
-      <c r="AC22" s="179"/>
-      <c r="AD22" s="179"/>
-      <c r="AE22" s="180"/>
-      <c r="AF22" s="175"/>
-      <c r="AG22" s="176"/>
-      <c r="AH22" s="176"/>
-      <c r="AI22" s="177"/>
-    </row>
-    <row r="23" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="168"/>
-      <c r="B23" s="169"/>
-      <c r="C23" s="170"/>
-      <c r="D23" s="171"/>
-      <c r="E23" s="172"/>
-      <c r="F23" s="173"/>
-      <c r="G23" s="169"/>
-      <c r="H23" s="174"/>
-      <c r="I23" s="170"/>
-      <c r="J23" s="175"/>
-      <c r="K23" s="176"/>
-      <c r="L23" s="176"/>
-      <c r="M23" s="176"/>
-      <c r="N23" s="176"/>
-      <c r="O23" s="176"/>
-      <c r="P23" s="177"/>
-      <c r="Q23" s="178"/>
-      <c r="R23" s="179"/>
-      <c r="S23" s="179"/>
-      <c r="T23" s="179"/>
-      <c r="U23" s="179"/>
-      <c r="V23" s="179"/>
-      <c r="W23" s="179"/>
-      <c r="X23" s="179"/>
-      <c r="Y23" s="179"/>
-      <c r="Z23" s="179"/>
-      <c r="AA23" s="179"/>
-      <c r="AB23" s="179"/>
-      <c r="AC23" s="179"/>
-      <c r="AD23" s="179"/>
-      <c r="AE23" s="180"/>
-      <c r="AF23" s="175"/>
-      <c r="AG23" s="176"/>
-      <c r="AH23" s="176"/>
-      <c r="AI23" s="177"/>
-    </row>
-    <row r="24" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="168"/>
-      <c r="B24" s="169"/>
-      <c r="C24" s="170"/>
-      <c r="D24" s="171"/>
-      <c r="E24" s="172"/>
-      <c r="F24" s="173"/>
-      <c r="G24" s="169"/>
-      <c r="H24" s="174"/>
-      <c r="I24" s="170"/>
-      <c r="J24" s="175"/>
-      <c r="K24" s="176"/>
-      <c r="L24" s="176"/>
-      <c r="M24" s="176"/>
-      <c r="N24" s="176"/>
-      <c r="O24" s="176"/>
-      <c r="P24" s="177"/>
-      <c r="Q24" s="178"/>
-      <c r="R24" s="179"/>
-      <c r="S24" s="179"/>
-      <c r="T24" s="179"/>
-      <c r="U24" s="179"/>
-      <c r="V24" s="179"/>
-      <c r="W24" s="179"/>
-      <c r="X24" s="179"/>
-      <c r="Y24" s="179"/>
-      <c r="Z24" s="179"/>
-      <c r="AA24" s="179"/>
-      <c r="AB24" s="179"/>
-      <c r="AC24" s="179"/>
-      <c r="AD24" s="179"/>
-      <c r="AE24" s="180"/>
-      <c r="AF24" s="175"/>
-      <c r="AG24" s="176"/>
-      <c r="AH24" s="176"/>
-      <c r="AI24" s="177"/>
-    </row>
-    <row r="25" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="168"/>
-      <c r="B25" s="169"/>
-      <c r="C25" s="170"/>
-      <c r="D25" s="171"/>
-      <c r="E25" s="172"/>
-      <c r="F25" s="173"/>
-      <c r="G25" s="169"/>
-      <c r="H25" s="174"/>
-      <c r="I25" s="170"/>
-      <c r="J25" s="175"/>
-      <c r="K25" s="176"/>
-      <c r="L25" s="176"/>
-      <c r="M25" s="176"/>
-      <c r="N25" s="176"/>
-      <c r="O25" s="176"/>
-      <c r="P25" s="177"/>
-      <c r="Q25" s="178"/>
-      <c r="R25" s="179"/>
-      <c r="S25" s="179"/>
-      <c r="T25" s="179"/>
-      <c r="U25" s="179"/>
-      <c r="V25" s="179"/>
-      <c r="W25" s="179"/>
-      <c r="X25" s="179"/>
-      <c r="Y25" s="179"/>
-      <c r="Z25" s="179"/>
-      <c r="AA25" s="179"/>
-      <c r="AB25" s="179"/>
-      <c r="AC25" s="179"/>
-      <c r="AD25" s="179"/>
-      <c r="AE25" s="180"/>
-      <c r="AF25" s="175"/>
-      <c r="AG25" s="176"/>
-      <c r="AH25" s="176"/>
-      <c r="AI25" s="177"/>
-    </row>
-    <row r="26" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="168"/>
-      <c r="B26" s="169"/>
-      <c r="C26" s="170"/>
-      <c r="D26" s="171"/>
-      <c r="E26" s="172"/>
-      <c r="F26" s="173"/>
-      <c r="G26" s="169"/>
-      <c r="H26" s="174"/>
-      <c r="I26" s="170"/>
-      <c r="J26" s="175"/>
-      <c r="K26" s="176"/>
-      <c r="L26" s="176"/>
-      <c r="M26" s="176"/>
-      <c r="N26" s="176"/>
-      <c r="O26" s="176"/>
-      <c r="P26" s="177"/>
-      <c r="Q26" s="178"/>
-      <c r="R26" s="179"/>
-      <c r="S26" s="179"/>
-      <c r="T26" s="179"/>
-      <c r="U26" s="179"/>
-      <c r="V26" s="179"/>
-      <c r="W26" s="179"/>
-      <c r="X26" s="179"/>
-      <c r="Y26" s="179"/>
-      <c r="Z26" s="179"/>
-      <c r="AA26" s="179"/>
-      <c r="AB26" s="179"/>
-      <c r="AC26" s="179"/>
-      <c r="AD26" s="179"/>
-      <c r="AE26" s="180"/>
-      <c r="AF26" s="175"/>
-      <c r="AG26" s="176"/>
-      <c r="AH26" s="176"/>
-      <c r="AI26" s="177"/>
-    </row>
-    <row r="27" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="168"/>
-      <c r="B27" s="169"/>
-      <c r="C27" s="170"/>
-      <c r="D27" s="171"/>
-      <c r="E27" s="172"/>
-      <c r="F27" s="173"/>
-      <c r="G27" s="169"/>
-      <c r="H27" s="174"/>
-      <c r="I27" s="170"/>
-      <c r="J27" s="175"/>
-      <c r="K27" s="176"/>
-      <c r="L27" s="176"/>
-      <c r="M27" s="176"/>
-      <c r="N27" s="176"/>
-      <c r="O27" s="176"/>
-      <c r="P27" s="177"/>
-      <c r="Q27" s="178"/>
-      <c r="R27" s="179"/>
-      <c r="S27" s="179"/>
-      <c r="T27" s="179"/>
-      <c r="U27" s="179"/>
-      <c r="V27" s="179"/>
-      <c r="W27" s="179"/>
-      <c r="X27" s="179"/>
-      <c r="Y27" s="179"/>
-      <c r="Z27" s="179"/>
-      <c r="AA27" s="179"/>
-      <c r="AB27" s="179"/>
-      <c r="AC27" s="179"/>
-      <c r="AD27" s="179"/>
-      <c r="AE27" s="180"/>
-      <c r="AF27" s="175"/>
-      <c r="AG27" s="176"/>
-      <c r="AH27" s="176"/>
-      <c r="AI27" s="177"/>
-    </row>
-    <row r="28" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="168"/>
-      <c r="B28" s="169"/>
-      <c r="C28" s="170"/>
-      <c r="D28" s="171"/>
-      <c r="E28" s="172"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="169"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="170"/>
-      <c r="J28" s="175"/>
-      <c r="K28" s="176"/>
-      <c r="L28" s="176"/>
-      <c r="M28" s="176"/>
-      <c r="N28" s="176"/>
-      <c r="O28" s="176"/>
-      <c r="P28" s="177"/>
-      <c r="Q28" s="178"/>
-      <c r="R28" s="179"/>
-      <c r="S28" s="179"/>
-      <c r="T28" s="179"/>
-      <c r="U28" s="179"/>
-      <c r="V28" s="179"/>
-      <c r="W28" s="179"/>
-      <c r="X28" s="179"/>
-      <c r="Y28" s="179"/>
-      <c r="Z28" s="179"/>
-      <c r="AA28" s="179"/>
-      <c r="AB28" s="179"/>
-      <c r="AC28" s="179"/>
-      <c r="AD28" s="179"/>
-      <c r="AE28" s="180"/>
-      <c r="AF28" s="175"/>
-      <c r="AG28" s="176"/>
-      <c r="AH28" s="176"/>
-      <c r="AI28" s="177"/>
-    </row>
-    <row r="29" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="168"/>
-      <c r="B29" s="169"/>
-      <c r="C29" s="170"/>
-      <c r="D29" s="171"/>
-      <c r="E29" s="172"/>
-      <c r="F29" s="173"/>
-      <c r="G29" s="169"/>
-      <c r="H29" s="174"/>
-      <c r="I29" s="170"/>
-      <c r="J29" s="175"/>
-      <c r="K29" s="176"/>
-      <c r="L29" s="176"/>
-      <c r="M29" s="176"/>
-      <c r="N29" s="176"/>
-      <c r="O29" s="176"/>
-      <c r="P29" s="177"/>
-      <c r="Q29" s="178"/>
-      <c r="R29" s="179"/>
-      <c r="S29" s="179"/>
-      <c r="T29" s="179"/>
-      <c r="U29" s="179"/>
-      <c r="V29" s="179"/>
-      <c r="W29" s="179"/>
-      <c r="X29" s="179"/>
-      <c r="Y29" s="179"/>
-      <c r="Z29" s="179"/>
-      <c r="AA29" s="179"/>
-      <c r="AB29" s="179"/>
-      <c r="AC29" s="179"/>
-      <c r="AD29" s="179"/>
-      <c r="AE29" s="180"/>
-      <c r="AF29" s="175"/>
-      <c r="AG29" s="176"/>
-      <c r="AH29" s="176"/>
-      <c r="AI29" s="177"/>
-    </row>
-    <row r="30" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="168"/>
-      <c r="B30" s="169"/>
-      <c r="C30" s="170"/>
-      <c r="D30" s="171"/>
-      <c r="E30" s="172"/>
-      <c r="F30" s="173"/>
-      <c r="G30" s="169"/>
-      <c r="H30" s="174"/>
-      <c r="I30" s="170"/>
-      <c r="J30" s="175"/>
-      <c r="K30" s="176"/>
-      <c r="L30" s="176"/>
-      <c r="M30" s="176"/>
-      <c r="N30" s="176"/>
-      <c r="O30" s="176"/>
-      <c r="P30" s="177"/>
-      <c r="Q30" s="178"/>
-      <c r="R30" s="179"/>
-      <c r="S30" s="179"/>
-      <c r="T30" s="179"/>
-      <c r="U30" s="179"/>
-      <c r="V30" s="179"/>
-      <c r="W30" s="179"/>
-      <c r="X30" s="179"/>
-      <c r="Y30" s="179"/>
-      <c r="Z30" s="179"/>
-      <c r="AA30" s="179"/>
-      <c r="AB30" s="179"/>
-      <c r="AC30" s="179"/>
-      <c r="AD30" s="179"/>
-      <c r="AE30" s="180"/>
-      <c r="AF30" s="175"/>
-      <c r="AG30" s="176"/>
-      <c r="AH30" s="176"/>
-      <c r="AI30" s="177"/>
-    </row>
-    <row r="31" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="168"/>
-      <c r="B31" s="169"/>
-      <c r="C31" s="170"/>
-      <c r="D31" s="171"/>
-      <c r="E31" s="172"/>
-      <c r="F31" s="173"/>
-      <c r="G31" s="169"/>
-      <c r="H31" s="174"/>
-      <c r="I31" s="170"/>
-      <c r="J31" s="175"/>
-      <c r="K31" s="176"/>
-      <c r="L31" s="176"/>
-      <c r="M31" s="176"/>
-      <c r="N31" s="176"/>
-      <c r="O31" s="176"/>
-      <c r="P31" s="177"/>
-      <c r="Q31" s="178"/>
-      <c r="R31" s="179"/>
-      <c r="S31" s="179"/>
-      <c r="T31" s="179"/>
-      <c r="U31" s="179"/>
-      <c r="V31" s="179"/>
-      <c r="W31" s="179"/>
-      <c r="X31" s="179"/>
-      <c r="Y31" s="179"/>
-      <c r="Z31" s="179"/>
-      <c r="AA31" s="179"/>
-      <c r="AB31" s="179"/>
-      <c r="AC31" s="179"/>
-      <c r="AD31" s="179"/>
-      <c r="AE31" s="180"/>
-      <c r="AF31" s="175"/>
-      <c r="AG31" s="176"/>
-      <c r="AH31" s="176"/>
-      <c r="AI31" s="177"/>
-    </row>
-    <row r="32" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="168"/>
-      <c r="B32" s="169"/>
-      <c r="C32" s="170"/>
-      <c r="D32" s="171"/>
-      <c r="E32" s="172"/>
-      <c r="F32" s="173"/>
-      <c r="G32" s="169"/>
-      <c r="H32" s="174"/>
-      <c r="I32" s="170"/>
-      <c r="J32" s="175"/>
-      <c r="K32" s="181"/>
-      <c r="L32" s="176"/>
-      <c r="M32" s="176"/>
-      <c r="N32" s="176"/>
-      <c r="O32" s="176"/>
-      <c r="P32" s="177"/>
-      <c r="Q32" s="178"/>
-      <c r="R32" s="179"/>
-      <c r="S32" s="179"/>
-      <c r="T32" s="179"/>
-      <c r="U32" s="179"/>
-      <c r="V32" s="179"/>
-      <c r="W32" s="179"/>
-      <c r="X32" s="179"/>
-      <c r="Y32" s="179"/>
-      <c r="Z32" s="179"/>
-      <c r="AA32" s="179"/>
-      <c r="AB32" s="179"/>
-      <c r="AC32" s="179"/>
-      <c r="AD32" s="179"/>
-      <c r="AE32" s="180"/>
-      <c r="AF32" s="175"/>
-      <c r="AG32" s="176"/>
-      <c r="AH32" s="176"/>
-      <c r="AI32" s="177"/>
-    </row>
-    <row r="33" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="168"/>
-      <c r="B33" s="169"/>
-      <c r="C33" s="170"/>
-      <c r="D33" s="171"/>
-      <c r="E33" s="172"/>
-      <c r="F33" s="173"/>
-      <c r="G33" s="169"/>
-      <c r="H33" s="174"/>
-      <c r="I33" s="170"/>
-      <c r="J33" s="175"/>
-      <c r="K33" s="176"/>
-      <c r="L33" s="176"/>
-      <c r="M33" s="176"/>
-      <c r="N33" s="176"/>
-      <c r="O33" s="176"/>
-      <c r="P33" s="177"/>
-      <c r="Q33" s="178"/>
-      <c r="R33" s="179"/>
-      <c r="S33" s="179"/>
-      <c r="T33" s="179"/>
-      <c r="U33" s="179"/>
-      <c r="V33" s="179"/>
-      <c r="W33" s="179"/>
-      <c r="X33" s="179"/>
-      <c r="Y33" s="179"/>
-      <c r="Z33" s="179"/>
-      <c r="AA33" s="179"/>
-      <c r="AB33" s="179"/>
-      <c r="AC33" s="179"/>
-      <c r="AD33" s="179"/>
-      <c r="AE33" s="180"/>
-      <c r="AF33" s="175"/>
-      <c r="AG33" s="176"/>
-      <c r="AH33" s="176"/>
-      <c r="AI33" s="177"/>
+      <c r="AG8" s="101"/>
+      <c r="AH8" s="101"/>
+      <c r="AI8" s="102"/>
+    </row>
+    <row r="9" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="76"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="88"/>
+      <c r="R9" s="89"/>
+      <c r="S9" s="89"/>
+      <c r="T9" s="89"/>
+      <c r="U9" s="89"/>
+      <c r="V9" s="89"/>
+      <c r="W9" s="89"/>
+      <c r="X9" s="89"/>
+      <c r="Y9" s="89"/>
+      <c r="Z9" s="89"/>
+      <c r="AA9" s="89"/>
+      <c r="AB9" s="89"/>
+      <c r="AC9" s="89"/>
+      <c r="AD9" s="89"/>
+      <c r="AE9" s="90"/>
+      <c r="AF9" s="85"/>
+      <c r="AG9" s="86"/>
+      <c r="AH9" s="86"/>
+      <c r="AI9" s="87"/>
+    </row>
+    <row r="10" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="76"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="86"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="87"/>
+      <c r="Q10" s="88"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="89"/>
+      <c r="T10" s="89"/>
+      <c r="U10" s="89"/>
+      <c r="V10" s="89"/>
+      <c r="W10" s="89"/>
+      <c r="X10" s="89"/>
+      <c r="Y10" s="89"/>
+      <c r="Z10" s="89"/>
+      <c r="AA10" s="89"/>
+      <c r="AB10" s="89"/>
+      <c r="AC10" s="89"/>
+      <c r="AD10" s="89"/>
+      <c r="AE10" s="90"/>
+      <c r="AF10" s="85"/>
+      <c r="AG10" s="86"/>
+      <c r="AH10" s="86"/>
+      <c r="AI10" s="87"/>
+    </row>
+    <row r="11" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="76"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="87"/>
+      <c r="Q11" s="88"/>
+      <c r="R11" s="89"/>
+      <c r="S11" s="89"/>
+      <c r="T11" s="89"/>
+      <c r="U11" s="89"/>
+      <c r="V11" s="89"/>
+      <c r="W11" s="89"/>
+      <c r="X11" s="89"/>
+      <c r="Y11" s="89"/>
+      <c r="Z11" s="89"/>
+      <c r="AA11" s="89"/>
+      <c r="AB11" s="89"/>
+      <c r="AC11" s="89"/>
+      <c r="AD11" s="89"/>
+      <c r="AE11" s="90"/>
+      <c r="AF11" s="85"/>
+      <c r="AG11" s="86"/>
+      <c r="AH11" s="86"/>
+      <c r="AI11" s="87"/>
+    </row>
+    <row r="12" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="76"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="88"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="89"/>
+      <c r="T12" s="89"/>
+      <c r="U12" s="89"/>
+      <c r="V12" s="89"/>
+      <c r="W12" s="89"/>
+      <c r="X12" s="89"/>
+      <c r="Y12" s="89"/>
+      <c r="Z12" s="89"/>
+      <c r="AA12" s="89"/>
+      <c r="AB12" s="89"/>
+      <c r="AC12" s="89"/>
+      <c r="AD12" s="89"/>
+      <c r="AE12" s="90"/>
+      <c r="AF12" s="85"/>
+      <c r="AG12" s="86"/>
+      <c r="AH12" s="86"/>
+      <c r="AI12" s="87"/>
+    </row>
+    <row r="13" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="76"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="87"/>
+      <c r="Q13" s="88"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="89"/>
+      <c r="T13" s="89"/>
+      <c r="U13" s="89"/>
+      <c r="V13" s="89"/>
+      <c r="W13" s="89"/>
+      <c r="X13" s="89"/>
+      <c r="Y13" s="89"/>
+      <c r="Z13" s="89"/>
+      <c r="AA13" s="89"/>
+      <c r="AB13" s="89"/>
+      <c r="AC13" s="89"/>
+      <c r="AD13" s="89"/>
+      <c r="AE13" s="90"/>
+      <c r="AF13" s="85"/>
+      <c r="AG13" s="86"/>
+      <c r="AH13" s="86"/>
+      <c r="AI13" s="87"/>
+    </row>
+    <row r="14" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="76"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="84"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="87"/>
+      <c r="Q14" s="88"/>
+      <c r="R14" s="89"/>
+      <c r="S14" s="89"/>
+      <c r="T14" s="89"/>
+      <c r="U14" s="89"/>
+      <c r="V14" s="89"/>
+      <c r="W14" s="89"/>
+      <c r="X14" s="89"/>
+      <c r="Y14" s="89"/>
+      <c r="Z14" s="89"/>
+      <c r="AA14" s="89"/>
+      <c r="AB14" s="89"/>
+      <c r="AC14" s="89"/>
+      <c r="AD14" s="89"/>
+      <c r="AE14" s="90"/>
+      <c r="AF14" s="85"/>
+      <c r="AG14" s="86"/>
+      <c r="AH14" s="86"/>
+      <c r="AI14" s="87"/>
+    </row>
+    <row r="15" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="76"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="86"/>
+      <c r="N15" s="86"/>
+      <c r="O15" s="86"/>
+      <c r="P15" s="87"/>
+      <c r="Q15" s="88"/>
+      <c r="R15" s="89"/>
+      <c r="S15" s="89"/>
+      <c r="T15" s="89"/>
+      <c r="U15" s="89"/>
+      <c r="V15" s="89"/>
+      <c r="W15" s="89"/>
+      <c r="X15" s="89"/>
+      <c r="Y15" s="89"/>
+      <c r="Z15" s="89"/>
+      <c r="AA15" s="89"/>
+      <c r="AB15" s="89"/>
+      <c r="AC15" s="89"/>
+      <c r="AD15" s="89"/>
+      <c r="AE15" s="90"/>
+      <c r="AF15" s="85"/>
+      <c r="AG15" s="86"/>
+      <c r="AH15" s="86"/>
+      <c r="AI15" s="87"/>
+    </row>
+    <row r="16" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="76"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="85"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="86"/>
+      <c r="N16" s="86"/>
+      <c r="O16" s="86"/>
+      <c r="P16" s="87"/>
+      <c r="Q16" s="88"/>
+      <c r="R16" s="89"/>
+      <c r="S16" s="89"/>
+      <c r="T16" s="89"/>
+      <c r="U16" s="89"/>
+      <c r="V16" s="89"/>
+      <c r="W16" s="89"/>
+      <c r="X16" s="89"/>
+      <c r="Y16" s="89"/>
+      <c r="Z16" s="89"/>
+      <c r="AA16" s="89"/>
+      <c r="AB16" s="89"/>
+      <c r="AC16" s="89"/>
+      <c r="AD16" s="89"/>
+      <c r="AE16" s="90"/>
+      <c r="AF16" s="85"/>
+      <c r="AG16" s="86"/>
+      <c r="AH16" s="86"/>
+      <c r="AI16" s="87"/>
+    </row>
+    <row r="17" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="76"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="85"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
+      <c r="N17" s="86"/>
+      <c r="O17" s="86"/>
+      <c r="P17" s="87"/>
+      <c r="Q17" s="88"/>
+      <c r="R17" s="89"/>
+      <c r="S17" s="89"/>
+      <c r="T17" s="89"/>
+      <c r="U17" s="89"/>
+      <c r="V17" s="89"/>
+      <c r="W17" s="89"/>
+      <c r="X17" s="89"/>
+      <c r="Y17" s="89"/>
+      <c r="Z17" s="89"/>
+      <c r="AA17" s="89"/>
+      <c r="AB17" s="89"/>
+      <c r="AC17" s="89"/>
+      <c r="AD17" s="89"/>
+      <c r="AE17" s="90"/>
+      <c r="AF17" s="85"/>
+      <c r="AG17" s="86"/>
+      <c r="AH17" s="86"/>
+      <c r="AI17" s="87"/>
+    </row>
+    <row r="18" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="76"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="80"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="86"/>
+      <c r="N18" s="86"/>
+      <c r="O18" s="86"/>
+      <c r="P18" s="87"/>
+      <c r="Q18" s="88"/>
+      <c r="R18" s="89"/>
+      <c r="S18" s="89"/>
+      <c r="T18" s="89"/>
+      <c r="U18" s="89"/>
+      <c r="V18" s="89"/>
+      <c r="W18" s="89"/>
+      <c r="X18" s="89"/>
+      <c r="Y18" s="89"/>
+      <c r="Z18" s="89"/>
+      <c r="AA18" s="89"/>
+      <c r="AB18" s="89"/>
+      <c r="AC18" s="89"/>
+      <c r="AD18" s="89"/>
+      <c r="AE18" s="90"/>
+      <c r="AF18" s="85"/>
+      <c r="AG18" s="86"/>
+      <c r="AH18" s="86"/>
+      <c r="AI18" s="87"/>
+    </row>
+    <row r="19" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="76"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="86"/>
+      <c r="N19" s="86"/>
+      <c r="O19" s="86"/>
+      <c r="P19" s="87"/>
+      <c r="Q19" s="88"/>
+      <c r="R19" s="89"/>
+      <c r="S19" s="89"/>
+      <c r="T19" s="89"/>
+      <c r="U19" s="89"/>
+      <c r="V19" s="89"/>
+      <c r="W19" s="89"/>
+      <c r="X19" s="89"/>
+      <c r="Y19" s="89"/>
+      <c r="Z19" s="89"/>
+      <c r="AA19" s="89"/>
+      <c r="AB19" s="89"/>
+      <c r="AC19" s="89"/>
+      <c r="AD19" s="89"/>
+      <c r="AE19" s="90"/>
+      <c r="AF19" s="85"/>
+      <c r="AG19" s="86"/>
+      <c r="AH19" s="86"/>
+      <c r="AI19" s="87"/>
+    </row>
+    <row r="20" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="76"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="84"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="86"/>
+      <c r="L20" s="86"/>
+      <c r="M20" s="86"/>
+      <c r="N20" s="86"/>
+      <c r="O20" s="86"/>
+      <c r="P20" s="87"/>
+      <c r="Q20" s="88"/>
+      <c r="R20" s="89"/>
+      <c r="S20" s="89"/>
+      <c r="T20" s="89"/>
+      <c r="U20" s="89"/>
+      <c r="V20" s="89"/>
+      <c r="W20" s="89"/>
+      <c r="X20" s="89"/>
+      <c r="Y20" s="89"/>
+      <c r="Z20" s="89"/>
+      <c r="AA20" s="89"/>
+      <c r="AB20" s="89"/>
+      <c r="AC20" s="89"/>
+      <c r="AD20" s="89"/>
+      <c r="AE20" s="90"/>
+      <c r="AF20" s="85"/>
+      <c r="AG20" s="86"/>
+      <c r="AH20" s="86"/>
+      <c r="AI20" s="87"/>
+    </row>
+    <row r="21" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="76"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="86"/>
+      <c r="L21" s="86"/>
+      <c r="M21" s="86"/>
+      <c r="N21" s="86"/>
+      <c r="O21" s="86"/>
+      <c r="P21" s="87"/>
+      <c r="Q21" s="88"/>
+      <c r="R21" s="89"/>
+      <c r="S21" s="89"/>
+      <c r="T21" s="89"/>
+      <c r="U21" s="89"/>
+      <c r="V21" s="89"/>
+      <c r="W21" s="89"/>
+      <c r="X21" s="89"/>
+      <c r="Y21" s="89"/>
+      <c r="Z21" s="89"/>
+      <c r="AA21" s="89"/>
+      <c r="AB21" s="89"/>
+      <c r="AC21" s="89"/>
+      <c r="AD21" s="89"/>
+      <c r="AE21" s="90"/>
+      <c r="AF21" s="85"/>
+      <c r="AG21" s="86"/>
+      <c r="AH21" s="86"/>
+      <c r="AI21" s="87"/>
+    </row>
+    <row r="22" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="76"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="86"/>
+      <c r="L22" s="86"/>
+      <c r="M22" s="86"/>
+      <c r="N22" s="86"/>
+      <c r="O22" s="86"/>
+      <c r="P22" s="87"/>
+      <c r="Q22" s="88"/>
+      <c r="R22" s="89"/>
+      <c r="S22" s="89"/>
+      <c r="T22" s="89"/>
+      <c r="U22" s="89"/>
+      <c r="V22" s="89"/>
+      <c r="W22" s="89"/>
+      <c r="X22" s="89"/>
+      <c r="Y22" s="89"/>
+      <c r="Z22" s="89"/>
+      <c r="AA22" s="89"/>
+      <c r="AB22" s="89"/>
+      <c r="AC22" s="89"/>
+      <c r="AD22" s="89"/>
+      <c r="AE22" s="90"/>
+      <c r="AF22" s="85"/>
+      <c r="AG22" s="86"/>
+      <c r="AH22" s="86"/>
+      <c r="AI22" s="87"/>
+    </row>
+    <row r="23" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="76"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="86"/>
+      <c r="M23" s="86"/>
+      <c r="N23" s="86"/>
+      <c r="O23" s="86"/>
+      <c r="P23" s="87"/>
+      <c r="Q23" s="88"/>
+      <c r="R23" s="89"/>
+      <c r="S23" s="89"/>
+      <c r="T23" s="89"/>
+      <c r="U23" s="89"/>
+      <c r="V23" s="89"/>
+      <c r="W23" s="89"/>
+      <c r="X23" s="89"/>
+      <c r="Y23" s="89"/>
+      <c r="Z23" s="89"/>
+      <c r="AA23" s="89"/>
+      <c r="AB23" s="89"/>
+      <c r="AC23" s="89"/>
+      <c r="AD23" s="89"/>
+      <c r="AE23" s="90"/>
+      <c r="AF23" s="85"/>
+      <c r="AG23" s="86"/>
+      <c r="AH23" s="86"/>
+      <c r="AI23" s="87"/>
+    </row>
+    <row r="24" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="76"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="84"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="86"/>
+      <c r="L24" s="86"/>
+      <c r="M24" s="86"/>
+      <c r="N24" s="86"/>
+      <c r="O24" s="86"/>
+      <c r="P24" s="87"/>
+      <c r="Q24" s="88"/>
+      <c r="R24" s="89"/>
+      <c r="S24" s="89"/>
+      <c r="T24" s="89"/>
+      <c r="U24" s="89"/>
+      <c r="V24" s="89"/>
+      <c r="W24" s="89"/>
+      <c r="X24" s="89"/>
+      <c r="Y24" s="89"/>
+      <c r="Z24" s="89"/>
+      <c r="AA24" s="89"/>
+      <c r="AB24" s="89"/>
+      <c r="AC24" s="89"/>
+      <c r="AD24" s="89"/>
+      <c r="AE24" s="90"/>
+      <c r="AF24" s="85"/>
+      <c r="AG24" s="86"/>
+      <c r="AH24" s="86"/>
+      <c r="AI24" s="87"/>
+    </row>
+    <row r="25" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="76"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="86"/>
+      <c r="L25" s="86"/>
+      <c r="M25" s="86"/>
+      <c r="N25" s="86"/>
+      <c r="O25" s="86"/>
+      <c r="P25" s="87"/>
+      <c r="Q25" s="88"/>
+      <c r="R25" s="89"/>
+      <c r="S25" s="89"/>
+      <c r="T25" s="89"/>
+      <c r="U25" s="89"/>
+      <c r="V25" s="89"/>
+      <c r="W25" s="89"/>
+      <c r="X25" s="89"/>
+      <c r="Y25" s="89"/>
+      <c r="Z25" s="89"/>
+      <c r="AA25" s="89"/>
+      <c r="AB25" s="89"/>
+      <c r="AC25" s="89"/>
+      <c r="AD25" s="89"/>
+      <c r="AE25" s="90"/>
+      <c r="AF25" s="85"/>
+      <c r="AG25" s="86"/>
+      <c r="AH25" s="86"/>
+      <c r="AI25" s="87"/>
+    </row>
+    <row r="26" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="76"/>
+      <c r="B26" s="79"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="84"/>
+      <c r="I26" s="80"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="86"/>
+      <c r="L26" s="86"/>
+      <c r="M26" s="86"/>
+      <c r="N26" s="86"/>
+      <c r="O26" s="86"/>
+      <c r="P26" s="87"/>
+      <c r="Q26" s="88"/>
+      <c r="R26" s="89"/>
+      <c r="S26" s="89"/>
+      <c r="T26" s="89"/>
+      <c r="U26" s="89"/>
+      <c r="V26" s="89"/>
+      <c r="W26" s="89"/>
+      <c r="X26" s="89"/>
+      <c r="Y26" s="89"/>
+      <c r="Z26" s="89"/>
+      <c r="AA26" s="89"/>
+      <c r="AB26" s="89"/>
+      <c r="AC26" s="89"/>
+      <c r="AD26" s="89"/>
+      <c r="AE26" s="90"/>
+      <c r="AF26" s="85"/>
+      <c r="AG26" s="86"/>
+      <c r="AH26" s="86"/>
+      <c r="AI26" s="87"/>
+    </row>
+    <row r="27" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="76"/>
+      <c r="B27" s="79"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="84"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="86"/>
+      <c r="L27" s="86"/>
+      <c r="M27" s="86"/>
+      <c r="N27" s="86"/>
+      <c r="O27" s="86"/>
+      <c r="P27" s="87"/>
+      <c r="Q27" s="88"/>
+      <c r="R27" s="89"/>
+      <c r="S27" s="89"/>
+      <c r="T27" s="89"/>
+      <c r="U27" s="89"/>
+      <c r="V27" s="89"/>
+      <c r="W27" s="89"/>
+      <c r="X27" s="89"/>
+      <c r="Y27" s="89"/>
+      <c r="Z27" s="89"/>
+      <c r="AA27" s="89"/>
+      <c r="AB27" s="89"/>
+      <c r="AC27" s="89"/>
+      <c r="AD27" s="89"/>
+      <c r="AE27" s="90"/>
+      <c r="AF27" s="85"/>
+      <c r="AG27" s="86"/>
+      <c r="AH27" s="86"/>
+      <c r="AI27" s="87"/>
+    </row>
+    <row r="28" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="76"/>
+      <c r="B28" s="79"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="84"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="86"/>
+      <c r="N28" s="86"/>
+      <c r="O28" s="86"/>
+      <c r="P28" s="87"/>
+      <c r="Q28" s="88"/>
+      <c r="R28" s="89"/>
+      <c r="S28" s="89"/>
+      <c r="T28" s="89"/>
+      <c r="U28" s="89"/>
+      <c r="V28" s="89"/>
+      <c r="W28" s="89"/>
+      <c r="X28" s="89"/>
+      <c r="Y28" s="89"/>
+      <c r="Z28" s="89"/>
+      <c r="AA28" s="89"/>
+      <c r="AB28" s="89"/>
+      <c r="AC28" s="89"/>
+      <c r="AD28" s="89"/>
+      <c r="AE28" s="90"/>
+      <c r="AF28" s="85"/>
+      <c r="AG28" s="86"/>
+      <c r="AH28" s="86"/>
+      <c r="AI28" s="87"/>
+    </row>
+    <row r="29" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="76"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="83"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="84"/>
+      <c r="I29" s="80"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="86"/>
+      <c r="M29" s="86"/>
+      <c r="N29" s="86"/>
+      <c r="O29" s="86"/>
+      <c r="P29" s="87"/>
+      <c r="Q29" s="88"/>
+      <c r="R29" s="89"/>
+      <c r="S29" s="89"/>
+      <c r="T29" s="89"/>
+      <c r="U29" s="89"/>
+      <c r="V29" s="89"/>
+      <c r="W29" s="89"/>
+      <c r="X29" s="89"/>
+      <c r="Y29" s="89"/>
+      <c r="Z29" s="89"/>
+      <c r="AA29" s="89"/>
+      <c r="AB29" s="89"/>
+      <c r="AC29" s="89"/>
+      <c r="AD29" s="89"/>
+      <c r="AE29" s="90"/>
+      <c r="AF29" s="85"/>
+      <c r="AG29" s="86"/>
+      <c r="AH29" s="86"/>
+      <c r="AI29" s="87"/>
+    </row>
+    <row r="30" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="76"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="84"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="85"/>
+      <c r="K30" s="86"/>
+      <c r="L30" s="86"/>
+      <c r="M30" s="86"/>
+      <c r="N30" s="86"/>
+      <c r="O30" s="86"/>
+      <c r="P30" s="87"/>
+      <c r="Q30" s="88"/>
+      <c r="R30" s="89"/>
+      <c r="S30" s="89"/>
+      <c r="T30" s="89"/>
+      <c r="U30" s="89"/>
+      <c r="V30" s="89"/>
+      <c r="W30" s="89"/>
+      <c r="X30" s="89"/>
+      <c r="Y30" s="89"/>
+      <c r="Z30" s="89"/>
+      <c r="AA30" s="89"/>
+      <c r="AB30" s="89"/>
+      <c r="AC30" s="89"/>
+      <c r="AD30" s="89"/>
+      <c r="AE30" s="90"/>
+      <c r="AF30" s="85"/>
+      <c r="AG30" s="86"/>
+      <c r="AH30" s="86"/>
+      <c r="AI30" s="87"/>
+    </row>
+    <row r="31" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="76"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="83"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="84"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="85"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="86"/>
+      <c r="M31" s="86"/>
+      <c r="N31" s="86"/>
+      <c r="O31" s="86"/>
+      <c r="P31" s="87"/>
+      <c r="Q31" s="88"/>
+      <c r="R31" s="89"/>
+      <c r="S31" s="89"/>
+      <c r="T31" s="89"/>
+      <c r="U31" s="89"/>
+      <c r="V31" s="89"/>
+      <c r="W31" s="89"/>
+      <c r="X31" s="89"/>
+      <c r="Y31" s="89"/>
+      <c r="Z31" s="89"/>
+      <c r="AA31" s="89"/>
+      <c r="AB31" s="89"/>
+      <c r="AC31" s="89"/>
+      <c r="AD31" s="89"/>
+      <c r="AE31" s="90"/>
+      <c r="AF31" s="85"/>
+      <c r="AG31" s="86"/>
+      <c r="AH31" s="86"/>
+      <c r="AI31" s="87"/>
+    </row>
+    <row r="32" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="76"/>
+      <c r="B32" s="79"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="84"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="85"/>
+      <c r="K32" s="91"/>
+      <c r="L32" s="86"/>
+      <c r="M32" s="86"/>
+      <c r="N32" s="86"/>
+      <c r="O32" s="86"/>
+      <c r="P32" s="87"/>
+      <c r="Q32" s="88"/>
+      <c r="R32" s="89"/>
+      <c r="S32" s="89"/>
+      <c r="T32" s="89"/>
+      <c r="U32" s="89"/>
+      <c r="V32" s="89"/>
+      <c r="W32" s="89"/>
+      <c r="X32" s="89"/>
+      <c r="Y32" s="89"/>
+      <c r="Z32" s="89"/>
+      <c r="AA32" s="89"/>
+      <c r="AB32" s="89"/>
+      <c r="AC32" s="89"/>
+      <c r="AD32" s="89"/>
+      <c r="AE32" s="90"/>
+      <c r="AF32" s="85"/>
+      <c r="AG32" s="86"/>
+      <c r="AH32" s="86"/>
+      <c r="AI32" s="87"/>
+    </row>
+    <row r="33" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="76"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="85"/>
+      <c r="K33" s="86"/>
+      <c r="L33" s="86"/>
+      <c r="M33" s="86"/>
+      <c r="N33" s="86"/>
+      <c r="O33" s="86"/>
+      <c r="P33" s="87"/>
+      <c r="Q33" s="88"/>
+      <c r="R33" s="89"/>
+      <c r="S33" s="89"/>
+      <c r="T33" s="89"/>
+      <c r="U33" s="89"/>
+      <c r="V33" s="89"/>
+      <c r="W33" s="89"/>
+      <c r="X33" s="89"/>
+      <c r="Y33" s="89"/>
+      <c r="Z33" s="89"/>
+      <c r="AA33" s="89"/>
+      <c r="AB33" s="89"/>
+      <c r="AC33" s="89"/>
+      <c r="AD33" s="89"/>
+      <c r="AE33" s="90"/>
+      <c r="AF33" s="85"/>
+      <c r="AG33" s="86"/>
+      <c r="AH33" s="86"/>
+      <c r="AI33" s="87"/>
     </row>
     <row r="34" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="K34" s="182"/>
+      <c r="K34" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="179">
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:P33"/>
-    <mergeCell ref="Q33:AE33"/>
-    <mergeCell ref="AF33:AI33"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:P32"/>
-    <mergeCell ref="Q32:AE32"/>
-    <mergeCell ref="AF32:AI32"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="Q31:AE31"/>
-    <mergeCell ref="AF31:AI31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:P30"/>
-    <mergeCell ref="Q30:AE30"/>
-    <mergeCell ref="AF30:AI30"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:P29"/>
-    <mergeCell ref="Q29:AE29"/>
-    <mergeCell ref="AF29:AI29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:P28"/>
-    <mergeCell ref="Q28:AE28"/>
-    <mergeCell ref="AF28:AI28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:P27"/>
-    <mergeCell ref="Q27:AE27"/>
-    <mergeCell ref="AF27:AI27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:P26"/>
-    <mergeCell ref="Q26:AE26"/>
-    <mergeCell ref="AF26:AI26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:P25"/>
-    <mergeCell ref="Q25:AE25"/>
-    <mergeCell ref="AF25:AI25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:P24"/>
-    <mergeCell ref="Q24:AE24"/>
-    <mergeCell ref="AF24:AI24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:P23"/>
-    <mergeCell ref="Q23:AE23"/>
-    <mergeCell ref="AF23:AI23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J22:P22"/>
-    <mergeCell ref="Q22:AE22"/>
-    <mergeCell ref="AF22:AI22"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="Q21:AE21"/>
-    <mergeCell ref="AF21:AI21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:P20"/>
-    <mergeCell ref="Q20:AE20"/>
-    <mergeCell ref="AF20:AI20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:P19"/>
-    <mergeCell ref="Q19:AE19"/>
-    <mergeCell ref="AF19:AI19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:P18"/>
-    <mergeCell ref="Q18:AE18"/>
-    <mergeCell ref="AF18:AI18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:P17"/>
-    <mergeCell ref="Q17:AE17"/>
-    <mergeCell ref="AF17:AI17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:P16"/>
-    <mergeCell ref="Q16:AE16"/>
-    <mergeCell ref="AF16:AI16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J15:P15"/>
-    <mergeCell ref="Q15:AE15"/>
-    <mergeCell ref="AF15:AI15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:P14"/>
-    <mergeCell ref="Q14:AE14"/>
-    <mergeCell ref="AF14:AI14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:P13"/>
-    <mergeCell ref="Q13:AE13"/>
-    <mergeCell ref="AF13:AI13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:P12"/>
-    <mergeCell ref="Q12:AE12"/>
-    <mergeCell ref="AF12:AI12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:P11"/>
-    <mergeCell ref="Q11:AE11"/>
-    <mergeCell ref="AF11:AI11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="J10:P10"/>
-    <mergeCell ref="Q10:AE10"/>
-    <mergeCell ref="AF10:AI10"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:P9"/>
-    <mergeCell ref="Q9:AE9"/>
-    <mergeCell ref="AF9:AI9"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:P8"/>
-    <mergeCell ref="Q8:AE8"/>
-    <mergeCell ref="AF8:AI8"/>
     <mergeCell ref="AG3:AI3"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:F7"/>
@@ -3888,6 +3730,162 @@
     <mergeCell ref="E3:N3"/>
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AC3:AF3"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:P9"/>
+    <mergeCell ref="Q9:AE9"/>
+    <mergeCell ref="AF9:AI9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:P8"/>
+    <mergeCell ref="Q8:AE8"/>
+    <mergeCell ref="AF8:AI8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:P11"/>
+    <mergeCell ref="Q11:AE11"/>
+    <mergeCell ref="AF11:AI11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:P10"/>
+    <mergeCell ref="Q10:AE10"/>
+    <mergeCell ref="AF10:AI10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:P13"/>
+    <mergeCell ref="Q13:AE13"/>
+    <mergeCell ref="AF13:AI13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:P12"/>
+    <mergeCell ref="Q12:AE12"/>
+    <mergeCell ref="AF12:AI12"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="J15:P15"/>
+    <mergeCell ref="Q15:AE15"/>
+    <mergeCell ref="AF15:AI15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="J14:P14"/>
+    <mergeCell ref="Q14:AE14"/>
+    <mergeCell ref="AF14:AI14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:P17"/>
+    <mergeCell ref="Q17:AE17"/>
+    <mergeCell ref="AF17:AI17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:P16"/>
+    <mergeCell ref="Q16:AE16"/>
+    <mergeCell ref="AF16:AI16"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:P19"/>
+    <mergeCell ref="Q19:AE19"/>
+    <mergeCell ref="AF19:AI19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:P18"/>
+    <mergeCell ref="Q18:AE18"/>
+    <mergeCell ref="AF18:AI18"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="Q21:AE21"/>
+    <mergeCell ref="AF21:AI21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:P20"/>
+    <mergeCell ref="Q20:AE20"/>
+    <mergeCell ref="AF20:AI20"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:P23"/>
+    <mergeCell ref="Q23:AE23"/>
+    <mergeCell ref="AF23:AI23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J22:P22"/>
+    <mergeCell ref="Q22:AE22"/>
+    <mergeCell ref="AF22:AI22"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:P25"/>
+    <mergeCell ref="Q25:AE25"/>
+    <mergeCell ref="AF25:AI25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:P24"/>
+    <mergeCell ref="Q24:AE24"/>
+    <mergeCell ref="AF24:AI24"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:P27"/>
+    <mergeCell ref="Q27:AE27"/>
+    <mergeCell ref="AF27:AI27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:P26"/>
+    <mergeCell ref="Q26:AE26"/>
+    <mergeCell ref="AF26:AI26"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:P29"/>
+    <mergeCell ref="Q29:AE29"/>
+    <mergeCell ref="AF29:AI29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:P28"/>
+    <mergeCell ref="Q28:AE28"/>
+    <mergeCell ref="AF28:AI28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="Q31:AE31"/>
+    <mergeCell ref="AF31:AI31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:P30"/>
+    <mergeCell ref="Q30:AE30"/>
+    <mergeCell ref="AF30:AI30"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:P33"/>
+    <mergeCell ref="Q33:AE33"/>
+    <mergeCell ref="AF33:AI33"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:P32"/>
+    <mergeCell ref="Q32:AE32"/>
+    <mergeCell ref="AF32:AI32"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <printOptions horizontalCentered="1"/>
@@ -4043,169 +4041,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="86" t="str">
+      <c r="A1" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A1")&lt;&gt;"",INDIRECT("'Revision history'!A1"),"")</f>
         <v>Project name</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="72" t="str">
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E1")&lt;&gt;"",INDIRECT("'Revision history'!E1"),"")</f>
         <v>Sample Project</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="116" t="str">
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="147" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!O1")&lt;&gt;"",INDIRECT("'Revision history'!O1"),"")</f>
         <v>Deliverable name</v>
       </c>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="118"/>
-      <c r="S1" s="119" t="str">
+      <c r="P1" s="148"/>
+      <c r="Q1" s="148"/>
+      <c r="R1" s="149"/>
+      <c r="S1" s="132" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!S1")&lt;&gt;"",INDIRECT("'Revision history'!S1"),"")</f>
         <v>System Function List</v>
       </c>
-      <c r="T1" s="120"/>
-      <c r="U1" s="120"/>
-      <c r="V1" s="120"/>
-      <c r="W1" s="120"/>
-      <c r="X1" s="120"/>
-      <c r="Y1" s="120"/>
-      <c r="Z1" s="121"/>
-      <c r="AA1" s="86" t="str">
+      <c r="T1" s="133"/>
+      <c r="U1" s="133"/>
+      <c r="V1" s="133"/>
+      <c r="W1" s="133"/>
+      <c r="X1" s="133"/>
+      <c r="Y1" s="133"/>
+      <c r="Z1" s="134"/>
+      <c r="AA1" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA1")&lt;&gt;"",INDIRECT("'Revision history'!AA1"),"")</f>
         <v>Prepared by</v>
       </c>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="183" t="str">
+      <c r="AB1" s="146"/>
+      <c r="AC1" s="159" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC1")&lt;&gt;"",INDIRECT("'Revision history'!AC1"),"")</f>
         <v>TIS</v>
       </c>
-      <c r="AD1" s="184"/>
-      <c r="AE1" s="184"/>
-      <c r="AF1" s="185"/>
-      <c r="AG1" s="186">
+      <c r="AD1" s="160"/>
+      <c r="AE1" s="160"/>
+      <c r="AF1" s="161"/>
+      <c r="AG1" s="156">
         <f ca="1">IF(INDIRECT("'Revision history'!AG1")&lt;&gt;"",INDIRECT("'Revision history'!AG1"),"")</f>
         <v>43404</v>
       </c>
-      <c r="AH1" s="187"/>
-      <c r="AI1" s="188"/>
+      <c r="AH1" s="157"/>
+      <c r="AI1" s="158"/>
       <c r="AJ1" s="17"/>
       <c r="AK1" s="17"/>
       <c r="AL1" s="26"/>
     </row>
     <row r="2" spans="1:38" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="str">
+      <c r="A2" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A2")&lt;&gt;"",INDIRECT("'Revision history'!A2"),"")</f>
         <v>System name</v>
       </c>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="72" t="str">
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E2")&lt;&gt;"",INDIRECT("'Revision history'!E2"),"")</f>
         <v>Sample System</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="123"/>
-      <c r="Q2" s="123"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="127"/>
-      <c r="AA2" s="86" t="str">
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="150"/>
+      <c r="P2" s="151"/>
+      <c r="Q2" s="151"/>
+      <c r="R2" s="152"/>
+      <c r="S2" s="135"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="136"/>
+      <c r="V2" s="136"/>
+      <c r="W2" s="136"/>
+      <c r="X2" s="136"/>
+      <c r="Y2" s="136"/>
+      <c r="Z2" s="137"/>
+      <c r="AA2" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA2")&lt;&gt;"",INDIRECT("'Revision history'!AA2"),"")</f>
         <v>Changes</v>
       </c>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="183" t="str">
+      <c r="AB2" s="146"/>
+      <c r="AC2" s="159" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC2")&lt;&gt;"",INDIRECT("'Revision history'!AC2"),"")</f>
         <v/>
       </c>
-      <c r="AD2" s="184"/>
-      <c r="AE2" s="184"/>
-      <c r="AF2" s="185"/>
-      <c r="AG2" s="186" t="str">
+      <c r="AD2" s="160"/>
+      <c r="AE2" s="160"/>
+      <c r="AF2" s="161"/>
+      <c r="AG2" s="156" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG2")&lt;&gt;"",INDIRECT("'Revision history'!AG2"),"")</f>
         <v/>
       </c>
-      <c r="AH2" s="187"/>
-      <c r="AI2" s="188"/>
+      <c r="AH2" s="157"/>
+      <c r="AI2" s="158"/>
       <c r="AJ2" s="17"/>
       <c r="AK2" s="17"/>
       <c r="AL2" s="17"/>
     </row>
     <row r="3" spans="1:38" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="86" t="str">
+      <c r="A3" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A3")&lt;&gt;"",INDIRECT("'Revision history'!A3"),"")</f>
         <v>Sub-system name</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="72" t="str">
+      <c r="B3" s="145"/>
+      <c r="C3" s="145"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E3")&lt;&gt;"",INDIRECT("'Revision history'!E3"),"")</f>
         <v>Client Management System</v>
       </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="128"/>
-      <c r="P3" s="129"/>
-      <c r="Q3" s="129"/>
-      <c r="R3" s="130"/>
-      <c r="S3" s="131"/>
-      <c r="T3" s="132"/>
-      <c r="U3" s="132"/>
-      <c r="V3" s="132"/>
-      <c r="W3" s="132"/>
-      <c r="X3" s="132"/>
-      <c r="Y3" s="132"/>
-      <c r="Z3" s="133"/>
-      <c r="AA3" s="86"/>
-      <c r="AB3" s="87"/>
-      <c r="AC3" s="183" t="str">
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="154"/>
+      <c r="Q3" s="154"/>
+      <c r="R3" s="155"/>
+      <c r="S3" s="138"/>
+      <c r="T3" s="139"/>
+      <c r="U3" s="139"/>
+      <c r="V3" s="139"/>
+      <c r="W3" s="139"/>
+      <c r="X3" s="139"/>
+      <c r="Y3" s="139"/>
+      <c r="Z3" s="140"/>
+      <c r="AA3" s="144"/>
+      <c r="AB3" s="146"/>
+      <c r="AC3" s="159" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC3")&lt;&gt;"",INDIRECT("'Revision history'!AC3"),"")</f>
         <v/>
       </c>
-      <c r="AD3" s="184"/>
-      <c r="AE3" s="184"/>
-      <c r="AF3" s="185"/>
-      <c r="AG3" s="186" t="str">
+      <c r="AD3" s="160"/>
+      <c r="AE3" s="160"/>
+      <c r="AF3" s="161"/>
+      <c r="AG3" s="156" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG3")&lt;&gt;"",INDIRECT("'Revision history'!AG3"),"")</f>
         <v/>
       </c>
-      <c r="AH3" s="187"/>
-      <c r="AI3" s="188"/>
+      <c r="AH3" s="157"/>
+      <c r="AI3" s="158"/>
       <c r="AJ3" s="17"/>
       <c r="AK3" s="17"/>
       <c r="AL3" s="17"/>
@@ -5668,6 +5666,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AG1:AI1"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AF3"/>
+    <mergeCell ref="AG3:AI3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:N1"/>
     <mergeCell ref="O1:R3"/>
@@ -5677,14 +5683,6 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:N2"/>
     <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AG1:AI1"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="E3:N3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AF3"/>
-    <mergeCell ref="AG3:AI3"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <printOptions horizontalCentered="1"/>
@@ -5710,169 +5708,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="86" t="str">
+      <c r="A1" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A1")&lt;&gt;"",INDIRECT("'Revision history'!A1"),"")</f>
         <v>Project name</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="72" t="str">
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E1")&lt;&gt;"",INDIRECT("'Revision history'!E1"),"")</f>
         <v>Sample Project</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="116" t="str">
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="147" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!O1")&lt;&gt;"",INDIRECT("'Revision history'!O1"),"")</f>
         <v>Deliverable name</v>
       </c>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="118"/>
-      <c r="S1" s="119" t="str">
+      <c r="P1" s="148"/>
+      <c r="Q1" s="148"/>
+      <c r="R1" s="149"/>
+      <c r="S1" s="132" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!S1")&lt;&gt;"",INDIRECT("'Revision history'!S1"),"")</f>
         <v>System Function List</v>
       </c>
-      <c r="T1" s="120"/>
-      <c r="U1" s="120"/>
-      <c r="V1" s="120"/>
-      <c r="W1" s="120"/>
-      <c r="X1" s="120"/>
-      <c r="Y1" s="120"/>
-      <c r="Z1" s="121"/>
-      <c r="AA1" s="86" t="str">
+      <c r="T1" s="133"/>
+      <c r="U1" s="133"/>
+      <c r="V1" s="133"/>
+      <c r="W1" s="133"/>
+      <c r="X1" s="133"/>
+      <c r="Y1" s="133"/>
+      <c r="Z1" s="134"/>
+      <c r="AA1" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA1")&lt;&gt;"",INDIRECT("'Revision history'!AA1"),"")</f>
         <v>Prepared by</v>
       </c>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="183" t="str">
+      <c r="AB1" s="146"/>
+      <c r="AC1" s="159" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC1")&lt;&gt;"",INDIRECT("'Revision history'!AC1"),"")</f>
         <v>TIS</v>
       </c>
-      <c r="AD1" s="184"/>
-      <c r="AE1" s="184"/>
-      <c r="AF1" s="185"/>
-      <c r="AG1" s="186">
+      <c r="AD1" s="160"/>
+      <c r="AE1" s="160"/>
+      <c r="AF1" s="161"/>
+      <c r="AG1" s="156">
         <f ca="1">IF(INDIRECT("'Revision history'!AG1")&lt;&gt;"",INDIRECT("'Revision history'!AG1"),"")</f>
         <v>43404</v>
       </c>
-      <c r="AH1" s="187"/>
-      <c r="AI1" s="188"/>
+      <c r="AH1" s="157"/>
+      <c r="AI1" s="158"/>
       <c r="AJ1" s="17"/>
       <c r="AK1" s="17"/>
       <c r="AL1" s="17"/>
     </row>
     <row r="2" spans="1:42" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="str">
+      <c r="A2" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A2")&lt;&gt;"",INDIRECT("'Revision history'!A2"),"")</f>
         <v>System name</v>
       </c>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="72" t="str">
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E2")&lt;&gt;"",INDIRECT("'Revision history'!E2"),"")</f>
         <v>Sample System</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="123"/>
-      <c r="Q2" s="123"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="127"/>
-      <c r="AA2" s="86" t="str">
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="150"/>
+      <c r="P2" s="151"/>
+      <c r="Q2" s="151"/>
+      <c r="R2" s="152"/>
+      <c r="S2" s="135"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="136"/>
+      <c r="V2" s="136"/>
+      <c r="W2" s="136"/>
+      <c r="X2" s="136"/>
+      <c r="Y2" s="136"/>
+      <c r="Z2" s="137"/>
+      <c r="AA2" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA2")&lt;&gt;"",INDIRECT("'Revision history'!AA2"),"")</f>
         <v>Changes</v>
       </c>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="183" t="str">
+      <c r="AB2" s="146"/>
+      <c r="AC2" s="159" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC2")&lt;&gt;"",INDIRECT("'Revision history'!AC2"),"")</f>
         <v/>
       </c>
-      <c r="AD2" s="184"/>
-      <c r="AE2" s="184"/>
-      <c r="AF2" s="185"/>
-      <c r="AG2" s="186" t="str">
+      <c r="AD2" s="160"/>
+      <c r="AE2" s="160"/>
+      <c r="AF2" s="161"/>
+      <c r="AG2" s="156" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG2")&lt;&gt;"",INDIRECT("'Revision history'!AG2"),"")</f>
         <v/>
       </c>
-      <c r="AH2" s="187"/>
-      <c r="AI2" s="188"/>
+      <c r="AH2" s="157"/>
+      <c r="AI2" s="158"/>
       <c r="AJ2" s="17"/>
       <c r="AK2" s="17"/>
       <c r="AL2" s="17"/>
     </row>
     <row r="3" spans="1:42" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="86" t="str">
+      <c r="A3" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A3")&lt;&gt;"",INDIRECT("'Revision history'!A3"),"")</f>
         <v>Sub-system name</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="72" t="str">
+      <c r="B3" s="145"/>
+      <c r="C3" s="145"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E3")&lt;&gt;"",INDIRECT("'Revision history'!E3"),"")</f>
         <v>Client Management System</v>
       </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="128"/>
-      <c r="P3" s="129"/>
-      <c r="Q3" s="129"/>
-      <c r="R3" s="130"/>
-      <c r="S3" s="131"/>
-      <c r="T3" s="132"/>
-      <c r="U3" s="132"/>
-      <c r="V3" s="132"/>
-      <c r="W3" s="132"/>
-      <c r="X3" s="132"/>
-      <c r="Y3" s="132"/>
-      <c r="Z3" s="133"/>
-      <c r="AA3" s="86"/>
-      <c r="AB3" s="87"/>
-      <c r="AC3" s="183" t="str">
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="154"/>
+      <c r="Q3" s="154"/>
+      <c r="R3" s="155"/>
+      <c r="S3" s="138"/>
+      <c r="T3" s="139"/>
+      <c r="U3" s="139"/>
+      <c r="V3" s="139"/>
+      <c r="W3" s="139"/>
+      <c r="X3" s="139"/>
+      <c r="Y3" s="139"/>
+      <c r="Z3" s="140"/>
+      <c r="AA3" s="144"/>
+      <c r="AB3" s="146"/>
+      <c r="AC3" s="159" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC3")&lt;&gt;"",INDIRECT("'Revision history'!AC3"),"")</f>
         <v/>
       </c>
-      <c r="AD3" s="184"/>
-      <c r="AE3" s="184"/>
-      <c r="AF3" s="185"/>
-      <c r="AG3" s="186" t="str">
+      <c r="AD3" s="160"/>
+      <c r="AE3" s="160"/>
+      <c r="AF3" s="161"/>
+      <c r="AG3" s="156" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG3")&lt;&gt;"",INDIRECT("'Revision history'!AG3"),"")</f>
         <v/>
       </c>
-      <c r="AH3" s="187"/>
-      <c r="AI3" s="188"/>
+      <c r="AH3" s="157"/>
+      <c r="AI3" s="158"/>
       <c r="AJ3" s="17"/>
       <c r="AK3" s="17"/>
       <c r="AL3" s="17"/>
@@ -5884,268 +5882,268 @@
     </row>
     <row r="6" spans="1:42" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:42" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="187" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="102" t="s">
+      <c r="D7" s="177" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="103"/>
-      <c r="F7" s="88" t="s">
+      <c r="E7" s="179"/>
+      <c r="F7" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="89"/>
-      <c r="H7" s="89"/>
-      <c r="I7" s="89"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="88" t="s">
+      <c r="G7" s="172"/>
+      <c r="H7" s="172"/>
+      <c r="I7" s="172"/>
+      <c r="J7" s="173"/>
+      <c r="K7" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="89"/>
-      <c r="M7" s="89"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="89"/>
-      <c r="P7" s="89"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="106" t="s">
+      <c r="L7" s="172"/>
+      <c r="M7" s="172"/>
+      <c r="N7" s="172"/>
+      <c r="O7" s="172"/>
+      <c r="P7" s="172"/>
+      <c r="Q7" s="173"/>
+      <c r="R7" s="183" t="s">
         <v>22</v>
       </c>
-      <c r="S7" s="107"/>
-      <c r="T7" s="88" t="s">
+      <c r="S7" s="184"/>
+      <c r="T7" s="171" t="s">
         <v>23</v>
       </c>
-      <c r="U7" s="89"/>
-      <c r="V7" s="89"/>
-      <c r="W7" s="89"/>
-      <c r="X7" s="89"/>
-      <c r="Y7" s="90"/>
-      <c r="Z7" s="88" t="s">
+      <c r="U7" s="172"/>
+      <c r="V7" s="172"/>
+      <c r="W7" s="172"/>
+      <c r="X7" s="172"/>
+      <c r="Y7" s="173"/>
+      <c r="Z7" s="171" t="s">
         <v>24</v>
       </c>
-      <c r="AA7" s="89"/>
-      <c r="AB7" s="89"/>
-      <c r="AC7" s="89"/>
-      <c r="AD7" s="89"/>
-      <c r="AE7" s="89"/>
-      <c r="AF7" s="89"/>
-      <c r="AG7" s="90"/>
-      <c r="AH7" s="102" t="s">
+      <c r="AA7" s="172"/>
+      <c r="AB7" s="172"/>
+      <c r="AC7" s="172"/>
+      <c r="AD7" s="172"/>
+      <c r="AE7" s="172"/>
+      <c r="AF7" s="172"/>
+      <c r="AG7" s="173"/>
+      <c r="AH7" s="177" t="s">
         <v>7</v>
       </c>
-      <c r="AI7" s="110"/>
-      <c r="AJ7" s="103"/>
-      <c r="AK7" s="88" t="s">
+      <c r="AI7" s="178"/>
+      <c r="AJ7" s="179"/>
+      <c r="AK7" s="171" t="s">
         <v>8</v>
       </c>
-      <c r="AL7" s="89"/>
-      <c r="AM7" s="89"/>
-      <c r="AN7" s="89"/>
-      <c r="AO7" s="89"/>
-      <c r="AP7" s="90"/>
+      <c r="AL7" s="172"/>
+      <c r="AM7" s="172"/>
+      <c r="AN7" s="172"/>
+      <c r="AO7" s="172"/>
+      <c r="AP7" s="173"/>
     </row>
     <row r="8" spans="1:42" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="95"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="92"/>
-      <c r="M8" s="92"/>
-      <c r="N8" s="92"/>
-      <c r="O8" s="92"/>
-      <c r="P8" s="92"/>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="108"/>
-      <c r="S8" s="109"/>
-      <c r="T8" s="91"/>
-      <c r="U8" s="92"/>
-      <c r="V8" s="92"/>
-      <c r="W8" s="92"/>
-      <c r="X8" s="92"/>
-      <c r="Y8" s="93"/>
-      <c r="Z8" s="91"/>
-      <c r="AA8" s="92"/>
-      <c r="AB8" s="92"/>
-      <c r="AC8" s="92"/>
-      <c r="AD8" s="92"/>
-      <c r="AE8" s="92"/>
-      <c r="AF8" s="92"/>
-      <c r="AG8" s="93"/>
-      <c r="AH8" s="104"/>
-      <c r="AI8" s="111"/>
-      <c r="AJ8" s="105"/>
-      <c r="AK8" s="91"/>
-      <c r="AL8" s="92"/>
-      <c r="AM8" s="92"/>
-      <c r="AN8" s="92"/>
-      <c r="AO8" s="92"/>
-      <c r="AP8" s="93"/>
+      <c r="C8" s="188"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="174"/>
+      <c r="G8" s="175"/>
+      <c r="H8" s="175"/>
+      <c r="I8" s="175"/>
+      <c r="J8" s="176"/>
+      <c r="K8" s="174"/>
+      <c r="L8" s="175"/>
+      <c r="M8" s="175"/>
+      <c r="N8" s="175"/>
+      <c r="O8" s="175"/>
+      <c r="P8" s="175"/>
+      <c r="Q8" s="176"/>
+      <c r="R8" s="185"/>
+      <c r="S8" s="186"/>
+      <c r="T8" s="174"/>
+      <c r="U8" s="175"/>
+      <c r="V8" s="175"/>
+      <c r="W8" s="175"/>
+      <c r="X8" s="175"/>
+      <c r="Y8" s="176"/>
+      <c r="Z8" s="174"/>
+      <c r="AA8" s="175"/>
+      <c r="AB8" s="175"/>
+      <c r="AC8" s="175"/>
+      <c r="AD8" s="175"/>
+      <c r="AE8" s="175"/>
+      <c r="AF8" s="175"/>
+      <c r="AG8" s="176"/>
+      <c r="AH8" s="180"/>
+      <c r="AI8" s="181"/>
+      <c r="AJ8" s="182"/>
+      <c r="AK8" s="174"/>
+      <c r="AL8" s="175"/>
+      <c r="AM8" s="175"/>
+      <c r="AN8" s="175"/>
+      <c r="AO8" s="175"/>
+      <c r="AP8" s="176"/>
     </row>
     <row r="9" spans="1:42" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="20">
         <v>1</v>
       </c>
-      <c r="D9" s="96" t="s">
+      <c r="D9" s="168" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="97"/>
-      <c r="F9" s="96" t="s">
+      <c r="E9" s="169"/>
+      <c r="F9" s="168" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="97"/>
-      <c r="K9" s="96" t="s">
+      <c r="G9" s="170"/>
+      <c r="H9" s="170"/>
+      <c r="I9" s="170"/>
+      <c r="J9" s="169"/>
+      <c r="K9" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101"/>
-      <c r="N9" s="101"/>
-      <c r="O9" s="101"/>
-      <c r="P9" s="101"/>
-      <c r="Q9" s="97"/>
-      <c r="R9" s="98" t="s">
+      <c r="L9" s="170"/>
+      <c r="M9" s="170"/>
+      <c r="N9" s="170"/>
+      <c r="O9" s="170"/>
+      <c r="P9" s="170"/>
+      <c r="Q9" s="169"/>
+      <c r="R9" s="165" t="s">
         <v>12</v>
       </c>
-      <c r="S9" s="100"/>
-      <c r="T9" s="98" t="s">
+      <c r="S9" s="167"/>
+      <c r="T9" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="U9" s="99"/>
-      <c r="V9" s="99"/>
-      <c r="W9" s="99"/>
-      <c r="X9" s="99"/>
-      <c r="Y9" s="100"/>
-      <c r="Z9" s="98" t="s">
+      <c r="U9" s="166"/>
+      <c r="V9" s="166"/>
+      <c r="W9" s="166"/>
+      <c r="X9" s="166"/>
+      <c r="Y9" s="167"/>
+      <c r="Z9" s="165" t="s">
         <v>14</v>
       </c>
-      <c r="AA9" s="99"/>
-      <c r="AB9" s="99"/>
-      <c r="AC9" s="99"/>
-      <c r="AD9" s="99"/>
-      <c r="AE9" s="99"/>
-      <c r="AF9" s="99"/>
-      <c r="AG9" s="100"/>
-      <c r="AH9" s="98" t="s">
+      <c r="AA9" s="166"/>
+      <c r="AB9" s="166"/>
+      <c r="AC9" s="166"/>
+      <c r="AD9" s="166"/>
+      <c r="AE9" s="166"/>
+      <c r="AF9" s="166"/>
+      <c r="AG9" s="167"/>
+      <c r="AH9" s="165" t="s">
         <v>15</v>
       </c>
-      <c r="AI9" s="99"/>
-      <c r="AJ9" s="100"/>
-      <c r="AK9" s="98"/>
-      <c r="AL9" s="99"/>
-      <c r="AM9" s="99"/>
-      <c r="AN9" s="99"/>
-      <c r="AO9" s="99"/>
-      <c r="AP9" s="100"/>
+      <c r="AI9" s="166"/>
+      <c r="AJ9" s="167"/>
+      <c r="AK9" s="165"/>
+      <c r="AL9" s="166"/>
+      <c r="AM9" s="166"/>
+      <c r="AN9" s="166"/>
+      <c r="AO9" s="166"/>
+      <c r="AP9" s="167"/>
     </row>
     <row r="10" spans="1:42" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="20">
         <v>2</v>
       </c>
-      <c r="D10" s="112"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="114"/>
-      <c r="H10" s="114"/>
-      <c r="I10" s="114"/>
-      <c r="J10" s="113"/>
-      <c r="K10" s="112"/>
-      <c r="L10" s="114"/>
-      <c r="M10" s="114"/>
-      <c r="N10" s="114"/>
-      <c r="O10" s="114"/>
-      <c r="P10" s="114"/>
-      <c r="Q10" s="113"/>
-      <c r="R10" s="98" t="s">
+      <c r="D10" s="162"/>
+      <c r="E10" s="163"/>
+      <c r="F10" s="162"/>
+      <c r="G10" s="164"/>
+      <c r="H10" s="164"/>
+      <c r="I10" s="164"/>
+      <c r="J10" s="163"/>
+      <c r="K10" s="162"/>
+      <c r="L10" s="164"/>
+      <c r="M10" s="164"/>
+      <c r="N10" s="164"/>
+      <c r="O10" s="164"/>
+      <c r="P10" s="164"/>
+      <c r="Q10" s="163"/>
+      <c r="R10" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="S10" s="100"/>
-      <c r="T10" s="98" t="s">
+      <c r="S10" s="167"/>
+      <c r="T10" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="U10" s="99"/>
-      <c r="V10" s="99"/>
-      <c r="W10" s="99"/>
-      <c r="X10" s="99"/>
-      <c r="Y10" s="100"/>
-      <c r="Z10" s="98" t="s">
+      <c r="U10" s="166"/>
+      <c r="V10" s="166"/>
+      <c r="W10" s="166"/>
+      <c r="X10" s="166"/>
+      <c r="Y10" s="167"/>
+      <c r="Z10" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="AA10" s="99"/>
-      <c r="AB10" s="99"/>
-      <c r="AC10" s="99"/>
-      <c r="AD10" s="99"/>
-      <c r="AE10" s="99"/>
-      <c r="AF10" s="99"/>
-      <c r="AG10" s="100"/>
-      <c r="AH10" s="98" t="s">
+      <c r="AA10" s="166"/>
+      <c r="AB10" s="166"/>
+      <c r="AC10" s="166"/>
+      <c r="AD10" s="166"/>
+      <c r="AE10" s="166"/>
+      <c r="AF10" s="166"/>
+      <c r="AG10" s="167"/>
+      <c r="AH10" s="165" t="s">
         <v>15</v>
       </c>
-      <c r="AI10" s="99"/>
-      <c r="AJ10" s="100"/>
-      <c r="AK10" s="98"/>
-      <c r="AL10" s="99"/>
-      <c r="AM10" s="99"/>
-      <c r="AN10" s="99"/>
-      <c r="AO10" s="99"/>
-      <c r="AP10" s="100"/>
+      <c r="AI10" s="166"/>
+      <c r="AJ10" s="167"/>
+      <c r="AK10" s="165"/>
+      <c r="AL10" s="166"/>
+      <c r="AM10" s="166"/>
+      <c r="AN10" s="166"/>
+      <c r="AO10" s="166"/>
+      <c r="AP10" s="167"/>
     </row>
     <row r="11" spans="1:42" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="21">
         <v>3</v>
       </c>
-      <c r="D11" s="112"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="112"/>
-      <c r="G11" s="114"/>
-      <c r="H11" s="114"/>
-      <c r="I11" s="114"/>
-      <c r="J11" s="113"/>
-      <c r="K11" s="112"/>
-      <c r="L11" s="114"/>
-      <c r="M11" s="114"/>
-      <c r="N11" s="114"/>
-      <c r="O11" s="114"/>
-      <c r="P11" s="114"/>
-      <c r="Q11" s="113"/>
-      <c r="R11" s="96" t="s">
+      <c r="D11" s="162"/>
+      <c r="E11" s="163"/>
+      <c r="F11" s="162"/>
+      <c r="G11" s="164"/>
+      <c r="H11" s="164"/>
+      <c r="I11" s="164"/>
+      <c r="J11" s="163"/>
+      <c r="K11" s="162"/>
+      <c r="L11" s="164"/>
+      <c r="M11" s="164"/>
+      <c r="N11" s="164"/>
+      <c r="O11" s="164"/>
+      <c r="P11" s="164"/>
+      <c r="Q11" s="163"/>
+      <c r="R11" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="S11" s="97"/>
-      <c r="T11" s="96" t="s">
+      <c r="S11" s="169"/>
+      <c r="T11" s="168" t="s">
         <v>20</v>
       </c>
-      <c r="U11" s="101"/>
-      <c r="V11" s="101"/>
-      <c r="W11" s="101"/>
-      <c r="X11" s="101"/>
-      <c r="Y11" s="97"/>
-      <c r="Z11" s="98" t="s">
+      <c r="U11" s="170"/>
+      <c r="V11" s="170"/>
+      <c r="W11" s="170"/>
+      <c r="X11" s="170"/>
+      <c r="Y11" s="169"/>
+      <c r="Z11" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="AA11" s="99"/>
-      <c r="AB11" s="99"/>
-      <c r="AC11" s="99"/>
-      <c r="AD11" s="99"/>
-      <c r="AE11" s="99"/>
-      <c r="AF11" s="99"/>
-      <c r="AG11" s="100"/>
-      <c r="AH11" s="98" t="s">
+      <c r="AA11" s="166"/>
+      <c r="AB11" s="166"/>
+      <c r="AC11" s="166"/>
+      <c r="AD11" s="166"/>
+      <c r="AE11" s="166"/>
+      <c r="AF11" s="166"/>
+      <c r="AG11" s="167"/>
+      <c r="AH11" s="165" t="s">
         <v>15</v>
       </c>
-      <c r="AI11" s="99"/>
-      <c r="AJ11" s="100"/>
-      <c r="AK11" s="98"/>
-      <c r="AL11" s="99"/>
-      <c r="AM11" s="99"/>
-      <c r="AN11" s="99"/>
-      <c r="AO11" s="99"/>
-      <c r="AP11" s="100"/>
+      <c r="AI11" s="166"/>
+      <c r="AJ11" s="167"/>
+      <c r="AK11" s="165"/>
+      <c r="AL11" s="166"/>
+      <c r="AM11" s="166"/>
+      <c r="AN11" s="166"/>
+      <c r="AO11" s="166"/>
+      <c r="AP11" s="167"/>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12" s="22"/>
@@ -6726,24 +6724,22 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="K10:Q10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="K11:Q11"/>
-    <mergeCell ref="AK10:AP10"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="T11:Y11"/>
-    <mergeCell ref="Z11:AG11"/>
-    <mergeCell ref="AH11:AJ11"/>
-    <mergeCell ref="AK11:AP11"/>
-    <mergeCell ref="Z7:AG8"/>
-    <mergeCell ref="AH7:AJ8"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="T10:Y10"/>
-    <mergeCell ref="Z10:AG10"/>
-    <mergeCell ref="AH10:AJ10"/>
+    <mergeCell ref="K7:Q8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="AK7:AP8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="AH9:AJ9"/>
+    <mergeCell ref="O1:R3"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="T9:Y9"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="K9:Q9"/>
+    <mergeCell ref="E1:N1"/>
+    <mergeCell ref="E2:N2"/>
+    <mergeCell ref="E3:N3"/>
     <mergeCell ref="D7:E8"/>
     <mergeCell ref="F7:J8"/>
     <mergeCell ref="AK9:AP9"/>
@@ -6760,22 +6756,24 @@
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="R7:S8"/>
     <mergeCell ref="T7:Y8"/>
-    <mergeCell ref="K7:Q8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="AK7:AP8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="AH9:AJ9"/>
-    <mergeCell ref="O1:R3"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="T9:Y9"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="K9:Q9"/>
-    <mergeCell ref="E1:N1"/>
-    <mergeCell ref="E2:N2"/>
-    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="Z7:AG8"/>
+    <mergeCell ref="AH7:AJ8"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="T10:Y10"/>
+    <mergeCell ref="Z10:AG10"/>
+    <mergeCell ref="AH10:AJ10"/>
+    <mergeCell ref="AK10:AP10"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="T11:Y11"/>
+    <mergeCell ref="Z11:AG11"/>
+    <mergeCell ref="AH11:AJ11"/>
+    <mergeCell ref="AK11:AP11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="K10:Q10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="K11:Q11"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>

</xml_diff>

<commit_message>
Nab 458 samples client management en (#113)
* Reflection of corrections in the Japanese version

* Revision history Update

* New Creation

* New Creation

* Reflection of corrections in the Japanese version

* Corrected component ID

* Revised document naming rules to be consistent

* 一貫性を保つために文書の命名規則に則りファイル名を修正

* 目的・概要の修正漏れ対応
</commit_message>
<xml_diff>
--- a/en/Sample_Project/Design_Document/B1_Client_Management_System/030_Application_Design/010_System_Functional_Design/System_Function_List_B1_Client_Management_System.xlsx
+++ b/en/Sample_Project/Design_Document/B1_Client_Management_System/030_Application_Design/010_System_Functional_Design/System_Function_List_B1_Client_Management_System.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0853D7-356A-46B1-A8C8-E661A5E56073}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676C98C8-7980-44F9-BA49-3DB4728EA6CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="360" windowWidth="27090" windowHeight="10830" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="17" r:id="rId1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -794,257 +792,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1065,6 +814,58 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1074,6 +875,15 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1092,49 +902,165 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1144,14 +1070,86 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1894,12 +1892,12 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="68">
+      <c r="I25" s="78">
         <f ca="1">IF(INDIRECT("'Revision history'!D8")="","",MAX(INDIRECT("'Revision history'!D8"):INDIRECT("'Revision history'!F33")))</f>
         <v>43404</v>
       </c>
-      <c r="J25" s="68"/>
-      <c r="K25" s="68"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
     </row>
     <row r="26" spans="6:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F26" s="6"/>
@@ -2496,55 +2494,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="72" t="s">
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="78" t="s">
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="119" t="s">
+      <c r="P1" s="124"/>
+      <c r="Q1" s="124"/>
+      <c r="R1" s="125"/>
+      <c r="S1" s="132" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="120"/>
-      <c r="U1" s="120"/>
-      <c r="V1" s="120"/>
-      <c r="W1" s="120"/>
-      <c r="X1" s="120"/>
-      <c r="Y1" s="120"/>
-      <c r="Z1" s="121"/>
-      <c r="AA1" s="75" t="s">
+      <c r="T1" s="133"/>
+      <c r="U1" s="133"/>
+      <c r="V1" s="133"/>
+      <c r="W1" s="133"/>
+      <c r="X1" s="133"/>
+      <c r="Y1" s="133"/>
+      <c r="Z1" s="134"/>
+      <c r="AA1" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="69" t="s">
+      <c r="AB1" s="116"/>
+      <c r="AC1" s="141" t="s">
         <v>2</v>
       </c>
-      <c r="AD1" s="70"/>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="71"/>
-      <c r="AG1" s="146">
+      <c r="AD1" s="142"/>
+      <c r="AE1" s="142"/>
+      <c r="AF1" s="143"/>
+      <c r="AG1" s="106">
         <v>43404</v>
       </c>
-      <c r="AH1" s="147"/>
-      <c r="AI1" s="148"/>
+      <c r="AH1" s="107"/>
+      <c r="AI1" s="108"/>
       <c r="AJ1" s="17"/>
       <c r="AK1" s="17"/>
       <c r="AL1" s="17"/>
@@ -2552,53 +2550,53 @@
       <c r="AN1" s="26"/>
     </row>
     <row r="2" spans="1:40" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="72" t="s">
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="134"/>
-      <c r="Q2" s="134"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="127"/>
-      <c r="AA2" s="75" t="s">
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="126"/>
+      <c r="P2" s="127"/>
+      <c r="Q2" s="127"/>
+      <c r="R2" s="128"/>
+      <c r="S2" s="135"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="136"/>
+      <c r="V2" s="136"/>
+      <c r="W2" s="136"/>
+      <c r="X2" s="136"/>
+      <c r="Y2" s="136"/>
+      <c r="Z2" s="137"/>
+      <c r="AA2" s="114" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="149" t="str">
+      <c r="AB2" s="116"/>
+      <c r="AC2" s="120" t="str">
         <f ca="1">IF(COUNTA(AF9:AF33)&lt;&gt;0,INDIRECT("AF"&amp;(COUNTA(AF9:AF33)+8)),"")</f>
         <v/>
       </c>
-      <c r="AD2" s="150"/>
-      <c r="AE2" s="150"/>
-      <c r="AF2" s="151"/>
-      <c r="AG2" s="146" t="str">
+      <c r="AD2" s="121"/>
+      <c r="AE2" s="121"/>
+      <c r="AF2" s="122"/>
+      <c r="AG2" s="106" t="str">
         <f>IF(D9="","",MAX(D9:F33))</f>
         <v/>
       </c>
-      <c r="AH2" s="147"/>
-      <c r="AI2" s="148"/>
+      <c r="AH2" s="107"/>
+      <c r="AI2" s="108"/>
       <c r="AJ2" s="17"/>
       <c r="AK2" s="17"/>
       <c r="AL2" s="17"/>
@@ -2606,1265 +2604,1109 @@
       <c r="AN2" s="17"/>
     </row>
     <row r="3" spans="1:40" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="114" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="72" t="s">
+      <c r="B3" s="115"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="131"/>
-      <c r="T3" s="132"/>
-      <c r="U3" s="132"/>
-      <c r="V3" s="132"/>
-      <c r="W3" s="132"/>
-      <c r="X3" s="132"/>
-      <c r="Y3" s="132"/>
-      <c r="Z3" s="133"/>
-      <c r="AA3" s="75"/>
-      <c r="AB3" s="77"/>
-      <c r="AC3" s="69"/>
-      <c r="AD3" s="70"/>
-      <c r="AE3" s="70"/>
-      <c r="AF3" s="71"/>
-      <c r="AG3" s="146"/>
-      <c r="AH3" s="147"/>
-      <c r="AI3" s="148"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="129"/>
+      <c r="P3" s="130"/>
+      <c r="Q3" s="130"/>
+      <c r="R3" s="131"/>
+      <c r="S3" s="138"/>
+      <c r="T3" s="139"/>
+      <c r="U3" s="139"/>
+      <c r="V3" s="139"/>
+      <c r="W3" s="139"/>
+      <c r="X3" s="139"/>
+      <c r="Y3" s="139"/>
+      <c r="Z3" s="140"/>
+      <c r="AA3" s="114"/>
+      <c r="AB3" s="116"/>
+      <c r="AC3" s="141"/>
+      <c r="AD3" s="142"/>
+      <c r="AE3" s="142"/>
+      <c r="AF3" s="143"/>
+      <c r="AG3" s="106"/>
+      <c r="AH3" s="107"/>
+      <c r="AI3" s="108"/>
       <c r="AJ3" s="17"/>
       <c r="AK3" s="17"/>
       <c r="AL3" s="17"/>
       <c r="AM3" s="17"/>
       <c r="AN3" s="17"/>
     </row>
-    <row r="5" spans="1:40" s="152" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N5" s="153" t="s">
+    <row r="5" spans="1:40" s="69" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="AA5" s="154"/>
-      <c r="AB5" s="154"/>
-      <c r="AC5" s="155"/>
-      <c r="AD5" s="156"/>
-      <c r="AE5" s="156"/>
-      <c r="AF5" s="156"/>
-      <c r="AG5" s="154"/>
-      <c r="AH5" s="154"/>
-      <c r="AI5" s="154"/>
-    </row>
-    <row r="6" spans="1:40" s="152" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N6" s="153"/>
-      <c r="AA6" s="154"/>
-      <c r="AB6" s="154"/>
-      <c r="AC6" s="155"/>
-      <c r="AD6" s="156"/>
-      <c r="AE6" s="156"/>
-      <c r="AF6" s="156"/>
-      <c r="AG6" s="154"/>
-      <c r="AH6" s="154"/>
-      <c r="AI6" s="154"/>
-    </row>
-    <row r="7" spans="1:40" s="157" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="135" t="s">
+      <c r="AA5" s="71"/>
+      <c r="AB5" s="71"/>
+      <c r="AC5" s="72"/>
+      <c r="AD5" s="73"/>
+      <c r="AE5" s="73"/>
+      <c r="AF5" s="73"/>
+      <c r="AG5" s="71"/>
+      <c r="AH5" s="71"/>
+      <c r="AI5" s="71"/>
+    </row>
+    <row r="6" spans="1:40" s="69" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="70"/>
+      <c r="AA6" s="71"/>
+      <c r="AB6" s="71"/>
+      <c r="AC6" s="72"/>
+      <c r="AD6" s="73"/>
+      <c r="AE6" s="73"/>
+      <c r="AF6" s="73"/>
+      <c r="AG6" s="71"/>
+      <c r="AH6" s="71"/>
+      <c r="AI6" s="71"/>
+    </row>
+    <row r="7" spans="1:40" s="74" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="136" t="s">
+      <c r="B7" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="137"/>
-      <c r="D7" s="138" t="s">
+      <c r="C7" s="110"/>
+      <c r="D7" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="139"/>
-      <c r="F7" s="140"/>
-      <c r="G7" s="138" t="s">
+      <c r="E7" s="112"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="139"/>
-      <c r="I7" s="140"/>
-      <c r="J7" s="138" t="s">
+      <c r="H7" s="112"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="139"/>
-      <c r="L7" s="139"/>
-      <c r="M7" s="139"/>
-      <c r="N7" s="139"/>
-      <c r="O7" s="139"/>
-      <c r="P7" s="140"/>
-      <c r="Q7" s="138" t="s">
+      <c r="K7" s="112"/>
+      <c r="L7" s="112"/>
+      <c r="M7" s="112"/>
+      <c r="N7" s="112"/>
+      <c r="O7" s="112"/>
+      <c r="P7" s="113"/>
+      <c r="Q7" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="R7" s="139"/>
-      <c r="S7" s="139"/>
-      <c r="T7" s="139"/>
-      <c r="U7" s="139"/>
-      <c r="V7" s="139"/>
-      <c r="W7" s="139"/>
-      <c r="X7" s="139"/>
-      <c r="Y7" s="139"/>
-      <c r="Z7" s="139"/>
-      <c r="AA7" s="139"/>
-      <c r="AB7" s="139"/>
-      <c r="AC7" s="139"/>
-      <c r="AD7" s="139"/>
-      <c r="AE7" s="140"/>
-      <c r="AF7" s="138" t="s">
+      <c r="R7" s="112"/>
+      <c r="S7" s="112"/>
+      <c r="T7" s="112"/>
+      <c r="U7" s="112"/>
+      <c r="V7" s="112"/>
+      <c r="W7" s="112"/>
+      <c r="X7" s="112"/>
+      <c r="Y7" s="112"/>
+      <c r="Z7" s="112"/>
+      <c r="AA7" s="112"/>
+      <c r="AB7" s="112"/>
+      <c r="AC7" s="112"/>
+      <c r="AD7" s="112"/>
+      <c r="AE7" s="113"/>
+      <c r="AF7" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="AG7" s="139"/>
-      <c r="AH7" s="139"/>
-      <c r="AI7" s="140"/>
-    </row>
-    <row r="8" spans="1:40" s="157" customFormat="1" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="158">
+      <c r="AG7" s="112"/>
+      <c r="AH7" s="112"/>
+      <c r="AI7" s="113"/>
+    </row>
+    <row r="8" spans="1:40" s="74" customFormat="1" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="75">
         <v>1</v>
       </c>
-      <c r="B8" s="141" t="s">
+      <c r="B8" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="142"/>
-      <c r="D8" s="159">
+      <c r="C8" s="93"/>
+      <c r="D8" s="94">
         <v>43404</v>
       </c>
-      <c r="E8" s="160"/>
-      <c r="F8" s="161"/>
-      <c r="G8" s="143" t="s">
+      <c r="E8" s="95"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="144"/>
-      <c r="I8" s="145"/>
-      <c r="J8" s="162" t="s">
+      <c r="H8" s="98"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="163"/>
-      <c r="L8" s="163"/>
-      <c r="M8" s="163"/>
-      <c r="N8" s="163"/>
-      <c r="O8" s="163"/>
-      <c r="P8" s="164"/>
-      <c r="Q8" s="165" t="s">
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
+      <c r="M8" s="101"/>
+      <c r="N8" s="101"/>
+      <c r="O8" s="101"/>
+      <c r="P8" s="102"/>
+      <c r="Q8" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="R8" s="166"/>
-      <c r="S8" s="166"/>
-      <c r="T8" s="166"/>
-      <c r="U8" s="166"/>
-      <c r="V8" s="166"/>
-      <c r="W8" s="166"/>
-      <c r="X8" s="166"/>
-      <c r="Y8" s="166"/>
-      <c r="Z8" s="166"/>
-      <c r="AA8" s="166"/>
-      <c r="AB8" s="166"/>
-      <c r="AC8" s="166"/>
-      <c r="AD8" s="166"/>
-      <c r="AE8" s="167"/>
-      <c r="AF8" s="162" t="s">
+      <c r="R8" s="104"/>
+      <c r="S8" s="104"/>
+      <c r="T8" s="104"/>
+      <c r="U8" s="104"/>
+      <c r="V8" s="104"/>
+      <c r="W8" s="104"/>
+      <c r="X8" s="104"/>
+      <c r="Y8" s="104"/>
+      <c r="Z8" s="104"/>
+      <c r="AA8" s="104"/>
+      <c r="AB8" s="104"/>
+      <c r="AC8" s="104"/>
+      <c r="AD8" s="104"/>
+      <c r="AE8" s="105"/>
+      <c r="AF8" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="AG8" s="163"/>
-      <c r="AH8" s="163"/>
-      <c r="AI8" s="164"/>
-    </row>
-    <row r="9" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="168"/>
-      <c r="B9" s="169"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="171"/>
-      <c r="E9" s="172"/>
-      <c r="F9" s="173"/>
-      <c r="G9" s="171"/>
-      <c r="H9" s="174"/>
-      <c r="I9" s="170"/>
-      <c r="J9" s="175"/>
-      <c r="K9" s="176"/>
-      <c r="L9" s="176"/>
-      <c r="M9" s="176"/>
-      <c r="N9" s="176"/>
-      <c r="O9" s="176"/>
-      <c r="P9" s="177"/>
-      <c r="Q9" s="178"/>
-      <c r="R9" s="179"/>
-      <c r="S9" s="179"/>
-      <c r="T9" s="179"/>
-      <c r="U9" s="179"/>
-      <c r="V9" s="179"/>
-      <c r="W9" s="179"/>
-      <c r="X9" s="179"/>
-      <c r="Y9" s="179"/>
-      <c r="Z9" s="179"/>
-      <c r="AA9" s="179"/>
-      <c r="AB9" s="179"/>
-      <c r="AC9" s="179"/>
-      <c r="AD9" s="179"/>
-      <c r="AE9" s="180"/>
-      <c r="AF9" s="175"/>
-      <c r="AG9" s="176"/>
-      <c r="AH9" s="176"/>
-      <c r="AI9" s="177"/>
-    </row>
-    <row r="10" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="168"/>
-      <c r="B10" s="169"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="171"/>
-      <c r="E10" s="172"/>
-      <c r="F10" s="173"/>
-      <c r="G10" s="169"/>
-      <c r="H10" s="174"/>
-      <c r="I10" s="170"/>
-      <c r="J10" s="175"/>
-      <c r="K10" s="176"/>
-      <c r="L10" s="176"/>
-      <c r="M10" s="176"/>
-      <c r="N10" s="176"/>
-      <c r="O10" s="176"/>
-      <c r="P10" s="177"/>
-      <c r="Q10" s="178"/>
-      <c r="R10" s="179"/>
-      <c r="S10" s="179"/>
-      <c r="T10" s="179"/>
-      <c r="U10" s="179"/>
-      <c r="V10" s="179"/>
-      <c r="W10" s="179"/>
-      <c r="X10" s="179"/>
-      <c r="Y10" s="179"/>
-      <c r="Z10" s="179"/>
-      <c r="AA10" s="179"/>
-      <c r="AB10" s="179"/>
-      <c r="AC10" s="179"/>
-      <c r="AD10" s="179"/>
-      <c r="AE10" s="180"/>
-      <c r="AF10" s="175"/>
-      <c r="AG10" s="176"/>
-      <c r="AH10" s="176"/>
-      <c r="AI10" s="177"/>
-    </row>
-    <row r="11" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="168"/>
-      <c r="B11" s="169"/>
-      <c r="C11" s="170"/>
-      <c r="D11" s="171"/>
-      <c r="E11" s="172"/>
-      <c r="F11" s="173"/>
-      <c r="G11" s="169"/>
-      <c r="H11" s="174"/>
-      <c r="I11" s="170"/>
-      <c r="J11" s="175"/>
-      <c r="K11" s="176"/>
-      <c r="L11" s="176"/>
-      <c r="M11" s="176"/>
-      <c r="N11" s="176"/>
-      <c r="O11" s="176"/>
-      <c r="P11" s="177"/>
-      <c r="Q11" s="178"/>
-      <c r="R11" s="179"/>
-      <c r="S11" s="179"/>
-      <c r="T11" s="179"/>
-      <c r="U11" s="179"/>
-      <c r="V11" s="179"/>
-      <c r="W11" s="179"/>
-      <c r="X11" s="179"/>
-      <c r="Y11" s="179"/>
-      <c r="Z11" s="179"/>
-      <c r="AA11" s="179"/>
-      <c r="AB11" s="179"/>
-      <c r="AC11" s="179"/>
-      <c r="AD11" s="179"/>
-      <c r="AE11" s="180"/>
-      <c r="AF11" s="175"/>
-      <c r="AG11" s="176"/>
-      <c r="AH11" s="176"/>
-      <c r="AI11" s="177"/>
-    </row>
-    <row r="12" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="168"/>
-      <c r="B12" s="169"/>
-      <c r="C12" s="170"/>
-      <c r="D12" s="171"/>
-      <c r="E12" s="172"/>
-      <c r="F12" s="173"/>
-      <c r="G12" s="169"/>
-      <c r="H12" s="174"/>
-      <c r="I12" s="170"/>
-      <c r="J12" s="175"/>
-      <c r="K12" s="176"/>
-      <c r="L12" s="176"/>
-      <c r="M12" s="176"/>
-      <c r="N12" s="176"/>
-      <c r="O12" s="176"/>
-      <c r="P12" s="177"/>
-      <c r="Q12" s="178"/>
-      <c r="R12" s="179"/>
-      <c r="S12" s="179"/>
-      <c r="T12" s="179"/>
-      <c r="U12" s="179"/>
-      <c r="V12" s="179"/>
-      <c r="W12" s="179"/>
-      <c r="X12" s="179"/>
-      <c r="Y12" s="179"/>
-      <c r="Z12" s="179"/>
-      <c r="AA12" s="179"/>
-      <c r="AB12" s="179"/>
-      <c r="AC12" s="179"/>
-      <c r="AD12" s="179"/>
-      <c r="AE12" s="180"/>
-      <c r="AF12" s="175"/>
-      <c r="AG12" s="176"/>
-      <c r="AH12" s="176"/>
-      <c r="AI12" s="177"/>
-    </row>
-    <row r="13" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="168"/>
-      <c r="B13" s="169"/>
-      <c r="C13" s="170"/>
-      <c r="D13" s="171"/>
-      <c r="E13" s="172"/>
-      <c r="F13" s="173"/>
-      <c r="G13" s="169"/>
-      <c r="H13" s="174"/>
-      <c r="I13" s="170"/>
-      <c r="J13" s="175"/>
-      <c r="K13" s="176"/>
-      <c r="L13" s="176"/>
-      <c r="M13" s="176"/>
-      <c r="N13" s="176"/>
-      <c r="O13" s="176"/>
-      <c r="P13" s="177"/>
-      <c r="Q13" s="178"/>
-      <c r="R13" s="179"/>
-      <c r="S13" s="179"/>
-      <c r="T13" s="179"/>
-      <c r="U13" s="179"/>
-      <c r="V13" s="179"/>
-      <c r="W13" s="179"/>
-      <c r="X13" s="179"/>
-      <c r="Y13" s="179"/>
-      <c r="Z13" s="179"/>
-      <c r="AA13" s="179"/>
-      <c r="AB13" s="179"/>
-      <c r="AC13" s="179"/>
-      <c r="AD13" s="179"/>
-      <c r="AE13" s="180"/>
-      <c r="AF13" s="175"/>
-      <c r="AG13" s="176"/>
-      <c r="AH13" s="176"/>
-      <c r="AI13" s="177"/>
-    </row>
-    <row r="14" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="168"/>
-      <c r="B14" s="169"/>
-      <c r="C14" s="170"/>
-      <c r="D14" s="171"/>
-      <c r="E14" s="172"/>
-      <c r="F14" s="173"/>
-      <c r="G14" s="169"/>
-      <c r="H14" s="174"/>
-      <c r="I14" s="170"/>
-      <c r="J14" s="175"/>
-      <c r="K14" s="176"/>
-      <c r="L14" s="176"/>
-      <c r="M14" s="176"/>
-      <c r="N14" s="176"/>
-      <c r="O14" s="176"/>
-      <c r="P14" s="177"/>
-      <c r="Q14" s="178"/>
-      <c r="R14" s="179"/>
-      <c r="S14" s="179"/>
-      <c r="T14" s="179"/>
-      <c r="U14" s="179"/>
-      <c r="V14" s="179"/>
-      <c r="W14" s="179"/>
-      <c r="X14" s="179"/>
-      <c r="Y14" s="179"/>
-      <c r="Z14" s="179"/>
-      <c r="AA14" s="179"/>
-      <c r="AB14" s="179"/>
-      <c r="AC14" s="179"/>
-      <c r="AD14" s="179"/>
-      <c r="AE14" s="180"/>
-      <c r="AF14" s="175"/>
-      <c r="AG14" s="176"/>
-      <c r="AH14" s="176"/>
-      <c r="AI14" s="177"/>
-    </row>
-    <row r="15" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="168"/>
-      <c r="B15" s="169"/>
-      <c r="C15" s="170"/>
-      <c r="D15" s="171"/>
-      <c r="E15" s="172"/>
-      <c r="F15" s="173"/>
-      <c r="G15" s="169"/>
-      <c r="H15" s="174"/>
-      <c r="I15" s="170"/>
-      <c r="J15" s="175"/>
-      <c r="K15" s="176"/>
-      <c r="L15" s="176"/>
-      <c r="M15" s="176"/>
-      <c r="N15" s="176"/>
-      <c r="O15" s="176"/>
-      <c r="P15" s="177"/>
-      <c r="Q15" s="178"/>
-      <c r="R15" s="179"/>
-      <c r="S15" s="179"/>
-      <c r="T15" s="179"/>
-      <c r="U15" s="179"/>
-      <c r="V15" s="179"/>
-      <c r="W15" s="179"/>
-      <c r="X15" s="179"/>
-      <c r="Y15" s="179"/>
-      <c r="Z15" s="179"/>
-      <c r="AA15" s="179"/>
-      <c r="AB15" s="179"/>
-      <c r="AC15" s="179"/>
-      <c r="AD15" s="179"/>
-      <c r="AE15" s="180"/>
-      <c r="AF15" s="175"/>
-      <c r="AG15" s="176"/>
-      <c r="AH15" s="176"/>
-      <c r="AI15" s="177"/>
-    </row>
-    <row r="16" spans="1:40" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="168"/>
-      <c r="B16" s="169"/>
-      <c r="C16" s="170"/>
-      <c r="D16" s="171"/>
-      <c r="E16" s="172"/>
-      <c r="F16" s="173"/>
-      <c r="G16" s="169"/>
-      <c r="H16" s="174"/>
-      <c r="I16" s="170"/>
-      <c r="J16" s="175"/>
-      <c r="K16" s="176"/>
-      <c r="L16" s="176"/>
-      <c r="M16" s="176"/>
-      <c r="N16" s="176"/>
-      <c r="O16" s="176"/>
-      <c r="P16" s="177"/>
-      <c r="Q16" s="178"/>
-      <c r="R16" s="179"/>
-      <c r="S16" s="179"/>
-      <c r="T16" s="179"/>
-      <c r="U16" s="179"/>
-      <c r="V16" s="179"/>
-      <c r="W16" s="179"/>
-      <c r="X16" s="179"/>
-      <c r="Y16" s="179"/>
-      <c r="Z16" s="179"/>
-      <c r="AA16" s="179"/>
-      <c r="AB16" s="179"/>
-      <c r="AC16" s="179"/>
-      <c r="AD16" s="179"/>
-      <c r="AE16" s="180"/>
-      <c r="AF16" s="175"/>
-      <c r="AG16" s="176"/>
-      <c r="AH16" s="176"/>
-      <c r="AI16" s="177"/>
-    </row>
-    <row r="17" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="168"/>
-      <c r="B17" s="169"/>
-      <c r="C17" s="170"/>
-      <c r="D17" s="171"/>
-      <c r="E17" s="172"/>
-      <c r="F17" s="173"/>
-      <c r="G17" s="169"/>
-      <c r="H17" s="174"/>
-      <c r="I17" s="170"/>
-      <c r="J17" s="175"/>
-      <c r="K17" s="176"/>
-      <c r="L17" s="176"/>
-      <c r="M17" s="176"/>
-      <c r="N17" s="176"/>
-      <c r="O17" s="176"/>
-      <c r="P17" s="177"/>
-      <c r="Q17" s="178"/>
-      <c r="R17" s="179"/>
-      <c r="S17" s="179"/>
-      <c r="T17" s="179"/>
-      <c r="U17" s="179"/>
-      <c r="V17" s="179"/>
-      <c r="W17" s="179"/>
-      <c r="X17" s="179"/>
-      <c r="Y17" s="179"/>
-      <c r="Z17" s="179"/>
-      <c r="AA17" s="179"/>
-      <c r="AB17" s="179"/>
-      <c r="AC17" s="179"/>
-      <c r="AD17" s="179"/>
-      <c r="AE17" s="180"/>
-      <c r="AF17" s="175"/>
-      <c r="AG17" s="176"/>
-      <c r="AH17" s="176"/>
-      <c r="AI17" s="177"/>
-    </row>
-    <row r="18" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="168"/>
-      <c r="B18" s="169"/>
-      <c r="C18" s="170"/>
-      <c r="D18" s="171"/>
-      <c r="E18" s="172"/>
-      <c r="F18" s="173"/>
-      <c r="G18" s="169"/>
-      <c r="H18" s="174"/>
-      <c r="I18" s="170"/>
-      <c r="J18" s="175"/>
-      <c r="K18" s="176"/>
-      <c r="L18" s="176"/>
-      <c r="M18" s="176"/>
-      <c r="N18" s="176"/>
-      <c r="O18" s="176"/>
-      <c r="P18" s="177"/>
-      <c r="Q18" s="178"/>
-      <c r="R18" s="179"/>
-      <c r="S18" s="179"/>
-      <c r="T18" s="179"/>
-      <c r="U18" s="179"/>
-      <c r="V18" s="179"/>
-      <c r="W18" s="179"/>
-      <c r="X18" s="179"/>
-      <c r="Y18" s="179"/>
-      <c r="Z18" s="179"/>
-      <c r="AA18" s="179"/>
-      <c r="AB18" s="179"/>
-      <c r="AC18" s="179"/>
-      <c r="AD18" s="179"/>
-      <c r="AE18" s="180"/>
-      <c r="AF18" s="175"/>
-      <c r="AG18" s="176"/>
-      <c r="AH18" s="176"/>
-      <c r="AI18" s="177"/>
-    </row>
-    <row r="19" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="168"/>
-      <c r="B19" s="169"/>
-      <c r="C19" s="170"/>
-      <c r="D19" s="171"/>
-      <c r="E19" s="172"/>
-      <c r="F19" s="173"/>
-      <c r="G19" s="169"/>
-      <c r="H19" s="174"/>
-      <c r="I19" s="170"/>
-      <c r="J19" s="175"/>
-      <c r="K19" s="176"/>
-      <c r="L19" s="176"/>
-      <c r="M19" s="176"/>
-      <c r="N19" s="176"/>
-      <c r="O19" s="176"/>
-      <c r="P19" s="177"/>
-      <c r="Q19" s="178"/>
-      <c r="R19" s="179"/>
-      <c r="S19" s="179"/>
-      <c r="T19" s="179"/>
-      <c r="U19" s="179"/>
-      <c r="V19" s="179"/>
-      <c r="W19" s="179"/>
-      <c r="X19" s="179"/>
-      <c r="Y19" s="179"/>
-      <c r="Z19" s="179"/>
-      <c r="AA19" s="179"/>
-      <c r="AB19" s="179"/>
-      <c r="AC19" s="179"/>
-      <c r="AD19" s="179"/>
-      <c r="AE19" s="180"/>
-      <c r="AF19" s="175"/>
-      <c r="AG19" s="176"/>
-      <c r="AH19" s="176"/>
-      <c r="AI19" s="177"/>
-    </row>
-    <row r="20" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="168"/>
-      <c r="B20" s="169"/>
-      <c r="C20" s="170"/>
-      <c r="D20" s="171"/>
-      <c r="E20" s="172"/>
-      <c r="F20" s="173"/>
-      <c r="G20" s="169"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="170"/>
-      <c r="J20" s="175"/>
-      <c r="K20" s="176"/>
-      <c r="L20" s="176"/>
-      <c r="M20" s="176"/>
-      <c r="N20" s="176"/>
-      <c r="O20" s="176"/>
-      <c r="P20" s="177"/>
-      <c r="Q20" s="178"/>
-      <c r="R20" s="179"/>
-      <c r="S20" s="179"/>
-      <c r="T20" s="179"/>
-      <c r="U20" s="179"/>
-      <c r="V20" s="179"/>
-      <c r="W20" s="179"/>
-      <c r="X20" s="179"/>
-      <c r="Y20" s="179"/>
-      <c r="Z20" s="179"/>
-      <c r="AA20" s="179"/>
-      <c r="AB20" s="179"/>
-      <c r="AC20" s="179"/>
-      <c r="AD20" s="179"/>
-      <c r="AE20" s="180"/>
-      <c r="AF20" s="175"/>
-      <c r="AG20" s="176"/>
-      <c r="AH20" s="176"/>
-      <c r="AI20" s="177"/>
-    </row>
-    <row r="21" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="168"/>
-      <c r="B21" s="169"/>
-      <c r="C21" s="170"/>
-      <c r="D21" s="171"/>
-      <c r="E21" s="172"/>
-      <c r="F21" s="173"/>
-      <c r="G21" s="169"/>
-      <c r="H21" s="174"/>
-      <c r="I21" s="170"/>
-      <c r="J21" s="175"/>
-      <c r="K21" s="176"/>
-      <c r="L21" s="176"/>
-      <c r="M21" s="176"/>
-      <c r="N21" s="176"/>
-      <c r="O21" s="176"/>
-      <c r="P21" s="177"/>
-      <c r="Q21" s="178"/>
-      <c r="R21" s="179"/>
-      <c r="S21" s="179"/>
-      <c r="T21" s="179"/>
-      <c r="U21" s="179"/>
-      <c r="V21" s="179"/>
-      <c r="W21" s="179"/>
-      <c r="X21" s="179"/>
-      <c r="Y21" s="179"/>
-      <c r="Z21" s="179"/>
-      <c r="AA21" s="179"/>
-      <c r="AB21" s="179"/>
-      <c r="AC21" s="179"/>
-      <c r="AD21" s="179"/>
-      <c r="AE21" s="180"/>
-      <c r="AF21" s="175"/>
-      <c r="AG21" s="176"/>
-      <c r="AH21" s="176"/>
-      <c r="AI21" s="177"/>
-    </row>
-    <row r="22" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="168"/>
-      <c r="B22" s="169"/>
-      <c r="C22" s="170"/>
-      <c r="D22" s="171"/>
-      <c r="E22" s="172"/>
-      <c r="F22" s="173"/>
-      <c r="G22" s="169"/>
-      <c r="H22" s="174"/>
-      <c r="I22" s="170"/>
-      <c r="J22" s="175"/>
-      <c r="K22" s="176"/>
-      <c r="L22" s="176"/>
-      <c r="M22" s="176"/>
-      <c r="N22" s="176"/>
-      <c r="O22" s="176"/>
-      <c r="P22" s="177"/>
-      <c r="Q22" s="178"/>
-      <c r="R22" s="179"/>
-      <c r="S22" s="179"/>
-      <c r="T22" s="179"/>
-      <c r="U22" s="179"/>
-      <c r="V22" s="179"/>
-      <c r="W22" s="179"/>
-      <c r="X22" s="179"/>
-      <c r="Y22" s="179"/>
-      <c r="Z22" s="179"/>
-      <c r="AA22" s="179"/>
-      <c r="AB22" s="179"/>
-      <c r="AC22" s="179"/>
-      <c r="AD22" s="179"/>
-      <c r="AE22" s="180"/>
-      <c r="AF22" s="175"/>
-      <c r="AG22" s="176"/>
-      <c r="AH22" s="176"/>
-      <c r="AI22" s="177"/>
-    </row>
-    <row r="23" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="168"/>
-      <c r="B23" s="169"/>
-      <c r="C23" s="170"/>
-      <c r="D23" s="171"/>
-      <c r="E23" s="172"/>
-      <c r="F23" s="173"/>
-      <c r="G23" s="169"/>
-      <c r="H23" s="174"/>
-      <c r="I23" s="170"/>
-      <c r="J23" s="175"/>
-      <c r="K23" s="176"/>
-      <c r="L23" s="176"/>
-      <c r="M23" s="176"/>
-      <c r="N23" s="176"/>
-      <c r="O23" s="176"/>
-      <c r="P23" s="177"/>
-      <c r="Q23" s="178"/>
-      <c r="R23" s="179"/>
-      <c r="S23" s="179"/>
-      <c r="T23" s="179"/>
-      <c r="U23" s="179"/>
-      <c r="V23" s="179"/>
-      <c r="W23" s="179"/>
-      <c r="X23" s="179"/>
-      <c r="Y23" s="179"/>
-      <c r="Z23" s="179"/>
-      <c r="AA23" s="179"/>
-      <c r="AB23" s="179"/>
-      <c r="AC23" s="179"/>
-      <c r="AD23" s="179"/>
-      <c r="AE23" s="180"/>
-      <c r="AF23" s="175"/>
-      <c r="AG23" s="176"/>
-      <c r="AH23" s="176"/>
-      <c r="AI23" s="177"/>
-    </row>
-    <row r="24" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="168"/>
-      <c r="B24" s="169"/>
-      <c r="C24" s="170"/>
-      <c r="D24" s="171"/>
-      <c r="E24" s="172"/>
-      <c r="F24" s="173"/>
-      <c r="G24" s="169"/>
-      <c r="H24" s="174"/>
-      <c r="I24" s="170"/>
-      <c r="J24" s="175"/>
-      <c r="K24" s="176"/>
-      <c r="L24" s="176"/>
-      <c r="M24" s="176"/>
-      <c r="N24" s="176"/>
-      <c r="O24" s="176"/>
-      <c r="P24" s="177"/>
-      <c r="Q24" s="178"/>
-      <c r="R24" s="179"/>
-      <c r="S24" s="179"/>
-      <c r="T24" s="179"/>
-      <c r="U24" s="179"/>
-      <c r="V24" s="179"/>
-      <c r="W24" s="179"/>
-      <c r="X24" s="179"/>
-      <c r="Y24" s="179"/>
-      <c r="Z24" s="179"/>
-      <c r="AA24" s="179"/>
-      <c r="AB24" s="179"/>
-      <c r="AC24" s="179"/>
-      <c r="AD24" s="179"/>
-      <c r="AE24" s="180"/>
-      <c r="AF24" s="175"/>
-      <c r="AG24" s="176"/>
-      <c r="AH24" s="176"/>
-      <c r="AI24" s="177"/>
-    </row>
-    <row r="25" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="168"/>
-      <c r="B25" s="169"/>
-      <c r="C25" s="170"/>
-      <c r="D25" s="171"/>
-      <c r="E25" s="172"/>
-      <c r="F25" s="173"/>
-      <c r="G25" s="169"/>
-      <c r="H25" s="174"/>
-      <c r="I25" s="170"/>
-      <c r="J25" s="175"/>
-      <c r="K25" s="176"/>
-      <c r="L25" s="176"/>
-      <c r="M25" s="176"/>
-      <c r="N25" s="176"/>
-      <c r="O25" s="176"/>
-      <c r="P25" s="177"/>
-      <c r="Q25" s="178"/>
-      <c r="R25" s="179"/>
-      <c r="S25" s="179"/>
-      <c r="T25" s="179"/>
-      <c r="U25" s="179"/>
-      <c r="V25" s="179"/>
-      <c r="W25" s="179"/>
-      <c r="X25" s="179"/>
-      <c r="Y25" s="179"/>
-      <c r="Z25" s="179"/>
-      <c r="AA25" s="179"/>
-      <c r="AB25" s="179"/>
-      <c r="AC25" s="179"/>
-      <c r="AD25" s="179"/>
-      <c r="AE25" s="180"/>
-      <c r="AF25" s="175"/>
-      <c r="AG25" s="176"/>
-      <c r="AH25" s="176"/>
-      <c r="AI25" s="177"/>
-    </row>
-    <row r="26" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="168"/>
-      <c r="B26" s="169"/>
-      <c r="C26" s="170"/>
-      <c r="D26" s="171"/>
-      <c r="E26" s="172"/>
-      <c r="F26" s="173"/>
-      <c r="G26" s="169"/>
-      <c r="H26" s="174"/>
-      <c r="I26" s="170"/>
-      <c r="J26" s="175"/>
-      <c r="K26" s="176"/>
-      <c r="L26" s="176"/>
-      <c r="M26" s="176"/>
-      <c r="N26" s="176"/>
-      <c r="O26" s="176"/>
-      <c r="P26" s="177"/>
-      <c r="Q26" s="178"/>
-      <c r="R26" s="179"/>
-      <c r="S26" s="179"/>
-      <c r="T26" s="179"/>
-      <c r="U26" s="179"/>
-      <c r="V26" s="179"/>
-      <c r="W26" s="179"/>
-      <c r="X26" s="179"/>
-      <c r="Y26" s="179"/>
-      <c r="Z26" s="179"/>
-      <c r="AA26" s="179"/>
-      <c r="AB26" s="179"/>
-      <c r="AC26" s="179"/>
-      <c r="AD26" s="179"/>
-      <c r="AE26" s="180"/>
-      <c r="AF26" s="175"/>
-      <c r="AG26" s="176"/>
-      <c r="AH26" s="176"/>
-      <c r="AI26" s="177"/>
-    </row>
-    <row r="27" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="168"/>
-      <c r="B27" s="169"/>
-      <c r="C27" s="170"/>
-      <c r="D27" s="171"/>
-      <c r="E27" s="172"/>
-      <c r="F27" s="173"/>
-      <c r="G27" s="169"/>
-      <c r="H27" s="174"/>
-      <c r="I27" s="170"/>
-      <c r="J27" s="175"/>
-      <c r="K27" s="176"/>
-      <c r="L27" s="176"/>
-      <c r="M27" s="176"/>
-      <c r="N27" s="176"/>
-      <c r="O27" s="176"/>
-      <c r="P27" s="177"/>
-      <c r="Q27" s="178"/>
-      <c r="R27" s="179"/>
-      <c r="S27" s="179"/>
-      <c r="T27" s="179"/>
-      <c r="U27" s="179"/>
-      <c r="V27" s="179"/>
-      <c r="W27" s="179"/>
-      <c r="X27" s="179"/>
-      <c r="Y27" s="179"/>
-      <c r="Z27" s="179"/>
-      <c r="AA27" s="179"/>
-      <c r="AB27" s="179"/>
-      <c r="AC27" s="179"/>
-      <c r="AD27" s="179"/>
-      <c r="AE27" s="180"/>
-      <c r="AF27" s="175"/>
-      <c r="AG27" s="176"/>
-      <c r="AH27" s="176"/>
-      <c r="AI27" s="177"/>
-    </row>
-    <row r="28" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="168"/>
-      <c r="B28" s="169"/>
-      <c r="C28" s="170"/>
-      <c r="D28" s="171"/>
-      <c r="E28" s="172"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="169"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="170"/>
-      <c r="J28" s="175"/>
-      <c r="K28" s="176"/>
-      <c r="L28" s="176"/>
-      <c r="M28" s="176"/>
-      <c r="N28" s="176"/>
-      <c r="O28" s="176"/>
-      <c r="P28" s="177"/>
-      <c r="Q28" s="178"/>
-      <c r="R28" s="179"/>
-      <c r="S28" s="179"/>
-      <c r="T28" s="179"/>
-      <c r="U28" s="179"/>
-      <c r="V28" s="179"/>
-      <c r="W28" s="179"/>
-      <c r="X28" s="179"/>
-      <c r="Y28" s="179"/>
-      <c r="Z28" s="179"/>
-      <c r="AA28" s="179"/>
-      <c r="AB28" s="179"/>
-      <c r="AC28" s="179"/>
-      <c r="AD28" s="179"/>
-      <c r="AE28" s="180"/>
-      <c r="AF28" s="175"/>
-      <c r="AG28" s="176"/>
-      <c r="AH28" s="176"/>
-      <c r="AI28" s="177"/>
-    </row>
-    <row r="29" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="168"/>
-      <c r="B29" s="169"/>
-      <c r="C29" s="170"/>
-      <c r="D29" s="171"/>
-      <c r="E29" s="172"/>
-      <c r="F29" s="173"/>
-      <c r="G29" s="169"/>
-      <c r="H29" s="174"/>
-      <c r="I29" s="170"/>
-      <c r="J29" s="175"/>
-      <c r="K29" s="176"/>
-      <c r="L29" s="176"/>
-      <c r="M29" s="176"/>
-      <c r="N29" s="176"/>
-      <c r="O29" s="176"/>
-      <c r="P29" s="177"/>
-      <c r="Q29" s="178"/>
-      <c r="R29" s="179"/>
-      <c r="S29" s="179"/>
-      <c r="T29" s="179"/>
-      <c r="U29" s="179"/>
-      <c r="V29" s="179"/>
-      <c r="W29" s="179"/>
-      <c r="X29" s="179"/>
-      <c r="Y29" s="179"/>
-      <c r="Z29" s="179"/>
-      <c r="AA29" s="179"/>
-      <c r="AB29" s="179"/>
-      <c r="AC29" s="179"/>
-      <c r="AD29" s="179"/>
-      <c r="AE29" s="180"/>
-      <c r="AF29" s="175"/>
-      <c r="AG29" s="176"/>
-      <c r="AH29" s="176"/>
-      <c r="AI29" s="177"/>
-    </row>
-    <row r="30" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="168"/>
-      <c r="B30" s="169"/>
-      <c r="C30" s="170"/>
-      <c r="D30" s="171"/>
-      <c r="E30" s="172"/>
-      <c r="F30" s="173"/>
-      <c r="G30" s="169"/>
-      <c r="H30" s="174"/>
-      <c r="I30" s="170"/>
-      <c r="J30" s="175"/>
-      <c r="K30" s="176"/>
-      <c r="L30" s="176"/>
-      <c r="M30" s="176"/>
-      <c r="N30" s="176"/>
-      <c r="O30" s="176"/>
-      <c r="P30" s="177"/>
-      <c r="Q30" s="178"/>
-      <c r="R30" s="179"/>
-      <c r="S30" s="179"/>
-      <c r="T30" s="179"/>
-      <c r="U30" s="179"/>
-      <c r="V30" s="179"/>
-      <c r="W30" s="179"/>
-      <c r="X30" s="179"/>
-      <c r="Y30" s="179"/>
-      <c r="Z30" s="179"/>
-      <c r="AA30" s="179"/>
-      <c r="AB30" s="179"/>
-      <c r="AC30" s="179"/>
-      <c r="AD30" s="179"/>
-      <c r="AE30" s="180"/>
-      <c r="AF30" s="175"/>
-      <c r="AG30" s="176"/>
-      <c r="AH30" s="176"/>
-      <c r="AI30" s="177"/>
-    </row>
-    <row r="31" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="168"/>
-      <c r="B31" s="169"/>
-      <c r="C31" s="170"/>
-      <c r="D31" s="171"/>
-      <c r="E31" s="172"/>
-      <c r="F31" s="173"/>
-      <c r="G31" s="169"/>
-      <c r="H31" s="174"/>
-      <c r="I31" s="170"/>
-      <c r="J31" s="175"/>
-      <c r="K31" s="176"/>
-      <c r="L31" s="176"/>
-      <c r="M31" s="176"/>
-      <c r="N31" s="176"/>
-      <c r="O31" s="176"/>
-      <c r="P31" s="177"/>
-      <c r="Q31" s="178"/>
-      <c r="R31" s="179"/>
-      <c r="S31" s="179"/>
-      <c r="T31" s="179"/>
-      <c r="U31" s="179"/>
-      <c r="V31" s="179"/>
-      <c r="W31" s="179"/>
-      <c r="X31" s="179"/>
-      <c r="Y31" s="179"/>
-      <c r="Z31" s="179"/>
-      <c r="AA31" s="179"/>
-      <c r="AB31" s="179"/>
-      <c r="AC31" s="179"/>
-      <c r="AD31" s="179"/>
-      <c r="AE31" s="180"/>
-      <c r="AF31" s="175"/>
-      <c r="AG31" s="176"/>
-      <c r="AH31" s="176"/>
-      <c r="AI31" s="177"/>
-    </row>
-    <row r="32" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="168"/>
-      <c r="B32" s="169"/>
-      <c r="C32" s="170"/>
-      <c r="D32" s="171"/>
-      <c r="E32" s="172"/>
-      <c r="F32" s="173"/>
-      <c r="G32" s="169"/>
-      <c r="H32" s="174"/>
-      <c r="I32" s="170"/>
-      <c r="J32" s="175"/>
-      <c r="K32" s="181"/>
-      <c r="L32" s="176"/>
-      <c r="M32" s="176"/>
-      <c r="N32" s="176"/>
-      <c r="O32" s="176"/>
-      <c r="P32" s="177"/>
-      <c r="Q32" s="178"/>
-      <c r="R32" s="179"/>
-      <c r="S32" s="179"/>
-      <c r="T32" s="179"/>
-      <c r="U32" s="179"/>
-      <c r="V32" s="179"/>
-      <c r="W32" s="179"/>
-      <c r="X32" s="179"/>
-      <c r="Y32" s="179"/>
-      <c r="Z32" s="179"/>
-      <c r="AA32" s="179"/>
-      <c r="AB32" s="179"/>
-      <c r="AC32" s="179"/>
-      <c r="AD32" s="179"/>
-      <c r="AE32" s="180"/>
-      <c r="AF32" s="175"/>
-      <c r="AG32" s="176"/>
-      <c r="AH32" s="176"/>
-      <c r="AI32" s="177"/>
-    </row>
-    <row r="33" spans="1:35" s="157" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="168"/>
-      <c r="B33" s="169"/>
-      <c r="C33" s="170"/>
-      <c r="D33" s="171"/>
-      <c r="E33" s="172"/>
-      <c r="F33" s="173"/>
-      <c r="G33" s="169"/>
-      <c r="H33" s="174"/>
-      <c r="I33" s="170"/>
-      <c r="J33" s="175"/>
-      <c r="K33" s="176"/>
-      <c r="L33" s="176"/>
-      <c r="M33" s="176"/>
-      <c r="N33" s="176"/>
-      <c r="O33" s="176"/>
-      <c r="P33" s="177"/>
-      <c r="Q33" s="178"/>
-      <c r="R33" s="179"/>
-      <c r="S33" s="179"/>
-      <c r="T33" s="179"/>
-      <c r="U33" s="179"/>
-      <c r="V33" s="179"/>
-      <c r="W33" s="179"/>
-      <c r="X33" s="179"/>
-      <c r="Y33" s="179"/>
-      <c r="Z33" s="179"/>
-      <c r="AA33" s="179"/>
-      <c r="AB33" s="179"/>
-      <c r="AC33" s="179"/>
-      <c r="AD33" s="179"/>
-      <c r="AE33" s="180"/>
-      <c r="AF33" s="175"/>
-      <c r="AG33" s="176"/>
-      <c r="AH33" s="176"/>
-      <c r="AI33" s="177"/>
+      <c r="AG8" s="101"/>
+      <c r="AH8" s="101"/>
+      <c r="AI8" s="102"/>
+    </row>
+    <row r="9" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="76"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="87"/>
+      <c r="Q9" s="88"/>
+      <c r="R9" s="89"/>
+      <c r="S9" s="89"/>
+      <c r="T9" s="89"/>
+      <c r="U9" s="89"/>
+      <c r="V9" s="89"/>
+      <c r="W9" s="89"/>
+      <c r="X9" s="89"/>
+      <c r="Y9" s="89"/>
+      <c r="Z9" s="89"/>
+      <c r="AA9" s="89"/>
+      <c r="AB9" s="89"/>
+      <c r="AC9" s="89"/>
+      <c r="AD9" s="89"/>
+      <c r="AE9" s="90"/>
+      <c r="AF9" s="85"/>
+      <c r="AG9" s="86"/>
+      <c r="AH9" s="86"/>
+      <c r="AI9" s="87"/>
+    </row>
+    <row r="10" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="76"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="86"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="87"/>
+      <c r="Q10" s="88"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="89"/>
+      <c r="T10" s="89"/>
+      <c r="U10" s="89"/>
+      <c r="V10" s="89"/>
+      <c r="W10" s="89"/>
+      <c r="X10" s="89"/>
+      <c r="Y10" s="89"/>
+      <c r="Z10" s="89"/>
+      <c r="AA10" s="89"/>
+      <c r="AB10" s="89"/>
+      <c r="AC10" s="89"/>
+      <c r="AD10" s="89"/>
+      <c r="AE10" s="90"/>
+      <c r="AF10" s="85"/>
+      <c r="AG10" s="86"/>
+      <c r="AH10" s="86"/>
+      <c r="AI10" s="87"/>
+    </row>
+    <row r="11" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="76"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="87"/>
+      <c r="Q11" s="88"/>
+      <c r="R11" s="89"/>
+      <c r="S11" s="89"/>
+      <c r="T11" s="89"/>
+      <c r="U11" s="89"/>
+      <c r="V11" s="89"/>
+      <c r="W11" s="89"/>
+      <c r="X11" s="89"/>
+      <c r="Y11" s="89"/>
+      <c r="Z11" s="89"/>
+      <c r="AA11" s="89"/>
+      <c r="AB11" s="89"/>
+      <c r="AC11" s="89"/>
+      <c r="AD11" s="89"/>
+      <c r="AE11" s="90"/>
+      <c r="AF11" s="85"/>
+      <c r="AG11" s="86"/>
+      <c r="AH11" s="86"/>
+      <c r="AI11" s="87"/>
+    </row>
+    <row r="12" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="76"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="88"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="89"/>
+      <c r="T12" s="89"/>
+      <c r="U12" s="89"/>
+      <c r="V12" s="89"/>
+      <c r="W12" s="89"/>
+      <c r="X12" s="89"/>
+      <c r="Y12" s="89"/>
+      <c r="Z12" s="89"/>
+      <c r="AA12" s="89"/>
+      <c r="AB12" s="89"/>
+      <c r="AC12" s="89"/>
+      <c r="AD12" s="89"/>
+      <c r="AE12" s="90"/>
+      <c r="AF12" s="85"/>
+      <c r="AG12" s="86"/>
+      <c r="AH12" s="86"/>
+      <c r="AI12" s="87"/>
+    </row>
+    <row r="13" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="76"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="80"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="87"/>
+      <c r="Q13" s="88"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="89"/>
+      <c r="T13" s="89"/>
+      <c r="U13" s="89"/>
+      <c r="V13" s="89"/>
+      <c r="W13" s="89"/>
+      <c r="X13" s="89"/>
+      <c r="Y13" s="89"/>
+      <c r="Z13" s="89"/>
+      <c r="AA13" s="89"/>
+      <c r="AB13" s="89"/>
+      <c r="AC13" s="89"/>
+      <c r="AD13" s="89"/>
+      <c r="AE13" s="90"/>
+      <c r="AF13" s="85"/>
+      <c r="AG13" s="86"/>
+      <c r="AH13" s="86"/>
+      <c r="AI13" s="87"/>
+    </row>
+    <row r="14" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="76"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="84"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="86"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="87"/>
+      <c r="Q14" s="88"/>
+      <c r="R14" s="89"/>
+      <c r="S14" s="89"/>
+      <c r="T14" s="89"/>
+      <c r="U14" s="89"/>
+      <c r="V14" s="89"/>
+      <c r="W14" s="89"/>
+      <c r="X14" s="89"/>
+      <c r="Y14" s="89"/>
+      <c r="Z14" s="89"/>
+      <c r="AA14" s="89"/>
+      <c r="AB14" s="89"/>
+      <c r="AC14" s="89"/>
+      <c r="AD14" s="89"/>
+      <c r="AE14" s="90"/>
+      <c r="AF14" s="85"/>
+      <c r="AG14" s="86"/>
+      <c r="AH14" s="86"/>
+      <c r="AI14" s="87"/>
+    </row>
+    <row r="15" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="76"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="86"/>
+      <c r="N15" s="86"/>
+      <c r="O15" s="86"/>
+      <c r="P15" s="87"/>
+      <c r="Q15" s="88"/>
+      <c r="R15" s="89"/>
+      <c r="S15" s="89"/>
+      <c r="T15" s="89"/>
+      <c r="U15" s="89"/>
+      <c r="V15" s="89"/>
+      <c r="W15" s="89"/>
+      <c r="X15" s="89"/>
+      <c r="Y15" s="89"/>
+      <c r="Z15" s="89"/>
+      <c r="AA15" s="89"/>
+      <c r="AB15" s="89"/>
+      <c r="AC15" s="89"/>
+      <c r="AD15" s="89"/>
+      <c r="AE15" s="90"/>
+      <c r="AF15" s="85"/>
+      <c r="AG15" s="86"/>
+      <c r="AH15" s="86"/>
+      <c r="AI15" s="87"/>
+    </row>
+    <row r="16" spans="1:40" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="76"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="83"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="85"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="86"/>
+      <c r="N16" s="86"/>
+      <c r="O16" s="86"/>
+      <c r="P16" s="87"/>
+      <c r="Q16" s="88"/>
+      <c r="R16" s="89"/>
+      <c r="S16" s="89"/>
+      <c r="T16" s="89"/>
+      <c r="U16" s="89"/>
+      <c r="V16" s="89"/>
+      <c r="W16" s="89"/>
+      <c r="X16" s="89"/>
+      <c r="Y16" s="89"/>
+      <c r="Z16" s="89"/>
+      <c r="AA16" s="89"/>
+      <c r="AB16" s="89"/>
+      <c r="AC16" s="89"/>
+      <c r="AD16" s="89"/>
+      <c r="AE16" s="90"/>
+      <c r="AF16" s="85"/>
+      <c r="AG16" s="86"/>
+      <c r="AH16" s="86"/>
+      <c r="AI16" s="87"/>
+    </row>
+    <row r="17" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="76"/>
+      <c r="B17" s="79"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="83"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="85"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
+      <c r="N17" s="86"/>
+      <c r="O17" s="86"/>
+      <c r="P17" s="87"/>
+      <c r="Q17" s="88"/>
+      <c r="R17" s="89"/>
+      <c r="S17" s="89"/>
+      <c r="T17" s="89"/>
+      <c r="U17" s="89"/>
+      <c r="V17" s="89"/>
+      <c r="W17" s="89"/>
+      <c r="X17" s="89"/>
+      <c r="Y17" s="89"/>
+      <c r="Z17" s="89"/>
+      <c r="AA17" s="89"/>
+      <c r="AB17" s="89"/>
+      <c r="AC17" s="89"/>
+      <c r="AD17" s="89"/>
+      <c r="AE17" s="90"/>
+      <c r="AF17" s="85"/>
+      <c r="AG17" s="86"/>
+      <c r="AH17" s="86"/>
+      <c r="AI17" s="87"/>
+    </row>
+    <row r="18" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="76"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="80"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="86"/>
+      <c r="N18" s="86"/>
+      <c r="O18" s="86"/>
+      <c r="P18" s="87"/>
+      <c r="Q18" s="88"/>
+      <c r="R18" s="89"/>
+      <c r="S18" s="89"/>
+      <c r="T18" s="89"/>
+      <c r="U18" s="89"/>
+      <c r="V18" s="89"/>
+      <c r="W18" s="89"/>
+      <c r="X18" s="89"/>
+      <c r="Y18" s="89"/>
+      <c r="Z18" s="89"/>
+      <c r="AA18" s="89"/>
+      <c r="AB18" s="89"/>
+      <c r="AC18" s="89"/>
+      <c r="AD18" s="89"/>
+      <c r="AE18" s="90"/>
+      <c r="AF18" s="85"/>
+      <c r="AG18" s="86"/>
+      <c r="AH18" s="86"/>
+      <c r="AI18" s="87"/>
+    </row>
+    <row r="19" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="76"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="83"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="86"/>
+      <c r="N19" s="86"/>
+      <c r="O19" s="86"/>
+      <c r="P19" s="87"/>
+      <c r="Q19" s="88"/>
+      <c r="R19" s="89"/>
+      <c r="S19" s="89"/>
+      <c r="T19" s="89"/>
+      <c r="U19" s="89"/>
+      <c r="V19" s="89"/>
+      <c r="W19" s="89"/>
+      <c r="X19" s="89"/>
+      <c r="Y19" s="89"/>
+      <c r="Z19" s="89"/>
+      <c r="AA19" s="89"/>
+      <c r="AB19" s="89"/>
+      <c r="AC19" s="89"/>
+      <c r="AD19" s="89"/>
+      <c r="AE19" s="90"/>
+      <c r="AF19" s="85"/>
+      <c r="AG19" s="86"/>
+      <c r="AH19" s="86"/>
+      <c r="AI19" s="87"/>
+    </row>
+    <row r="20" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="76"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="84"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="86"/>
+      <c r="L20" s="86"/>
+      <c r="M20" s="86"/>
+      <c r="N20" s="86"/>
+      <c r="O20" s="86"/>
+      <c r="P20" s="87"/>
+      <c r="Q20" s="88"/>
+      <c r="R20" s="89"/>
+      <c r="S20" s="89"/>
+      <c r="T20" s="89"/>
+      <c r="U20" s="89"/>
+      <c r="V20" s="89"/>
+      <c r="W20" s="89"/>
+      <c r="X20" s="89"/>
+      <c r="Y20" s="89"/>
+      <c r="Z20" s="89"/>
+      <c r="AA20" s="89"/>
+      <c r="AB20" s="89"/>
+      <c r="AC20" s="89"/>
+      <c r="AD20" s="89"/>
+      <c r="AE20" s="90"/>
+      <c r="AF20" s="85"/>
+      <c r="AG20" s="86"/>
+      <c r="AH20" s="86"/>
+      <c r="AI20" s="87"/>
+    </row>
+    <row r="21" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="76"/>
+      <c r="B21" s="79"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="86"/>
+      <c r="L21" s="86"/>
+      <c r="M21" s="86"/>
+      <c r="N21" s="86"/>
+      <c r="O21" s="86"/>
+      <c r="P21" s="87"/>
+      <c r="Q21" s="88"/>
+      <c r="R21" s="89"/>
+      <c r="S21" s="89"/>
+      <c r="T21" s="89"/>
+      <c r="U21" s="89"/>
+      <c r="V21" s="89"/>
+      <c r="W21" s="89"/>
+      <c r="X21" s="89"/>
+      <c r="Y21" s="89"/>
+      <c r="Z21" s="89"/>
+      <c r="AA21" s="89"/>
+      <c r="AB21" s="89"/>
+      <c r="AC21" s="89"/>
+      <c r="AD21" s="89"/>
+      <c r="AE21" s="90"/>
+      <c r="AF21" s="85"/>
+      <c r="AG21" s="86"/>
+      <c r="AH21" s="86"/>
+      <c r="AI21" s="87"/>
+    </row>
+    <row r="22" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="76"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="86"/>
+      <c r="L22" s="86"/>
+      <c r="M22" s="86"/>
+      <c r="N22" s="86"/>
+      <c r="O22" s="86"/>
+      <c r="P22" s="87"/>
+      <c r="Q22" s="88"/>
+      <c r="R22" s="89"/>
+      <c r="S22" s="89"/>
+      <c r="T22" s="89"/>
+      <c r="U22" s="89"/>
+      <c r="V22" s="89"/>
+      <c r="W22" s="89"/>
+      <c r="X22" s="89"/>
+      <c r="Y22" s="89"/>
+      <c r="Z22" s="89"/>
+      <c r="AA22" s="89"/>
+      <c r="AB22" s="89"/>
+      <c r="AC22" s="89"/>
+      <c r="AD22" s="89"/>
+      <c r="AE22" s="90"/>
+      <c r="AF22" s="85"/>
+      <c r="AG22" s="86"/>
+      <c r="AH22" s="86"/>
+      <c r="AI22" s="87"/>
+    </row>
+    <row r="23" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="76"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="86"/>
+      <c r="M23" s="86"/>
+      <c r="N23" s="86"/>
+      <c r="O23" s="86"/>
+      <c r="P23" s="87"/>
+      <c r="Q23" s="88"/>
+      <c r="R23" s="89"/>
+      <c r="S23" s="89"/>
+      <c r="T23" s="89"/>
+      <c r="U23" s="89"/>
+      <c r="V23" s="89"/>
+      <c r="W23" s="89"/>
+      <c r="X23" s="89"/>
+      <c r="Y23" s="89"/>
+      <c r="Z23" s="89"/>
+      <c r="AA23" s="89"/>
+      <c r="AB23" s="89"/>
+      <c r="AC23" s="89"/>
+      <c r="AD23" s="89"/>
+      <c r="AE23" s="90"/>
+      <c r="AF23" s="85"/>
+      <c r="AG23" s="86"/>
+      <c r="AH23" s="86"/>
+      <c r="AI23" s="87"/>
+    </row>
+    <row r="24" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="76"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="84"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="86"/>
+      <c r="L24" s="86"/>
+      <c r="M24" s="86"/>
+      <c r="N24" s="86"/>
+      <c r="O24" s="86"/>
+      <c r="P24" s="87"/>
+      <c r="Q24" s="88"/>
+      <c r="R24" s="89"/>
+      <c r="S24" s="89"/>
+      <c r="T24" s="89"/>
+      <c r="U24" s="89"/>
+      <c r="V24" s="89"/>
+      <c r="W24" s="89"/>
+      <c r="X24" s="89"/>
+      <c r="Y24" s="89"/>
+      <c r="Z24" s="89"/>
+      <c r="AA24" s="89"/>
+      <c r="AB24" s="89"/>
+      <c r="AC24" s="89"/>
+      <c r="AD24" s="89"/>
+      <c r="AE24" s="90"/>
+      <c r="AF24" s="85"/>
+      <c r="AG24" s="86"/>
+      <c r="AH24" s="86"/>
+      <c r="AI24" s="87"/>
+    </row>
+    <row r="25" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="76"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="86"/>
+      <c r="L25" s="86"/>
+      <c r="M25" s="86"/>
+      <c r="N25" s="86"/>
+      <c r="O25" s="86"/>
+      <c r="P25" s="87"/>
+      <c r="Q25" s="88"/>
+      <c r="R25" s="89"/>
+      <c r="S25" s="89"/>
+      <c r="T25" s="89"/>
+      <c r="U25" s="89"/>
+      <c r="V25" s="89"/>
+      <c r="W25" s="89"/>
+      <c r="X25" s="89"/>
+      <c r="Y25" s="89"/>
+      <c r="Z25" s="89"/>
+      <c r="AA25" s="89"/>
+      <c r="AB25" s="89"/>
+      <c r="AC25" s="89"/>
+      <c r="AD25" s="89"/>
+      <c r="AE25" s="90"/>
+      <c r="AF25" s="85"/>
+      <c r="AG25" s="86"/>
+      <c r="AH25" s="86"/>
+      <c r="AI25" s="87"/>
+    </row>
+    <row r="26" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="76"/>
+      <c r="B26" s="79"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="83"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="84"/>
+      <c r="I26" s="80"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="86"/>
+      <c r="L26" s="86"/>
+      <c r="M26" s="86"/>
+      <c r="N26" s="86"/>
+      <c r="O26" s="86"/>
+      <c r="P26" s="87"/>
+      <c r="Q26" s="88"/>
+      <c r="R26" s="89"/>
+      <c r="S26" s="89"/>
+      <c r="T26" s="89"/>
+      <c r="U26" s="89"/>
+      <c r="V26" s="89"/>
+      <c r="W26" s="89"/>
+      <c r="X26" s="89"/>
+      <c r="Y26" s="89"/>
+      <c r="Z26" s="89"/>
+      <c r="AA26" s="89"/>
+      <c r="AB26" s="89"/>
+      <c r="AC26" s="89"/>
+      <c r="AD26" s="89"/>
+      <c r="AE26" s="90"/>
+      <c r="AF26" s="85"/>
+      <c r="AG26" s="86"/>
+      <c r="AH26" s="86"/>
+      <c r="AI26" s="87"/>
+    </row>
+    <row r="27" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="76"/>
+      <c r="B27" s="79"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="84"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="86"/>
+      <c r="L27" s="86"/>
+      <c r="M27" s="86"/>
+      <c r="N27" s="86"/>
+      <c r="O27" s="86"/>
+      <c r="P27" s="87"/>
+      <c r="Q27" s="88"/>
+      <c r="R27" s="89"/>
+      <c r="S27" s="89"/>
+      <c r="T27" s="89"/>
+      <c r="U27" s="89"/>
+      <c r="V27" s="89"/>
+      <c r="W27" s="89"/>
+      <c r="X27" s="89"/>
+      <c r="Y27" s="89"/>
+      <c r="Z27" s="89"/>
+      <c r="AA27" s="89"/>
+      <c r="AB27" s="89"/>
+      <c r="AC27" s="89"/>
+      <c r="AD27" s="89"/>
+      <c r="AE27" s="90"/>
+      <c r="AF27" s="85"/>
+      <c r="AG27" s="86"/>
+      <c r="AH27" s="86"/>
+      <c r="AI27" s="87"/>
+    </row>
+    <row r="28" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="76"/>
+      <c r="B28" s="79"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="84"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="86"/>
+      <c r="N28" s="86"/>
+      <c r="O28" s="86"/>
+      <c r="P28" s="87"/>
+      <c r="Q28" s="88"/>
+      <c r="R28" s="89"/>
+      <c r="S28" s="89"/>
+      <c r="T28" s="89"/>
+      <c r="U28" s="89"/>
+      <c r="V28" s="89"/>
+      <c r="W28" s="89"/>
+      <c r="X28" s="89"/>
+      <c r="Y28" s="89"/>
+      <c r="Z28" s="89"/>
+      <c r="AA28" s="89"/>
+      <c r="AB28" s="89"/>
+      <c r="AC28" s="89"/>
+      <c r="AD28" s="89"/>
+      <c r="AE28" s="90"/>
+      <c r="AF28" s="85"/>
+      <c r="AG28" s="86"/>
+      <c r="AH28" s="86"/>
+      <c r="AI28" s="87"/>
+    </row>
+    <row r="29" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="76"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="83"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="84"/>
+      <c r="I29" s="80"/>
+      <c r="J29" s="85"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="86"/>
+      <c r="M29" s="86"/>
+      <c r="N29" s="86"/>
+      <c r="O29" s="86"/>
+      <c r="P29" s="87"/>
+      <c r="Q29" s="88"/>
+      <c r="R29" s="89"/>
+      <c r="S29" s="89"/>
+      <c r="T29" s="89"/>
+      <c r="U29" s="89"/>
+      <c r="V29" s="89"/>
+      <c r="W29" s="89"/>
+      <c r="X29" s="89"/>
+      <c r="Y29" s="89"/>
+      <c r="Z29" s="89"/>
+      <c r="AA29" s="89"/>
+      <c r="AB29" s="89"/>
+      <c r="AC29" s="89"/>
+      <c r="AD29" s="89"/>
+      <c r="AE29" s="90"/>
+      <c r="AF29" s="85"/>
+      <c r="AG29" s="86"/>
+      <c r="AH29" s="86"/>
+      <c r="AI29" s="87"/>
+    </row>
+    <row r="30" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="76"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="84"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="85"/>
+      <c r="K30" s="86"/>
+      <c r="L30" s="86"/>
+      <c r="M30" s="86"/>
+      <c r="N30" s="86"/>
+      <c r="O30" s="86"/>
+      <c r="P30" s="87"/>
+      <c r="Q30" s="88"/>
+      <c r="R30" s="89"/>
+      <c r="S30" s="89"/>
+      <c r="T30" s="89"/>
+      <c r="U30" s="89"/>
+      <c r="V30" s="89"/>
+      <c r="W30" s="89"/>
+      <c r="X30" s="89"/>
+      <c r="Y30" s="89"/>
+      <c r="Z30" s="89"/>
+      <c r="AA30" s="89"/>
+      <c r="AB30" s="89"/>
+      <c r="AC30" s="89"/>
+      <c r="AD30" s="89"/>
+      <c r="AE30" s="90"/>
+      <c r="AF30" s="85"/>
+      <c r="AG30" s="86"/>
+      <c r="AH30" s="86"/>
+      <c r="AI30" s="87"/>
+    </row>
+    <row r="31" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="76"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="83"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="84"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="85"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="86"/>
+      <c r="M31" s="86"/>
+      <c r="N31" s="86"/>
+      <c r="O31" s="86"/>
+      <c r="P31" s="87"/>
+      <c r="Q31" s="88"/>
+      <c r="R31" s="89"/>
+      <c r="S31" s="89"/>
+      <c r="T31" s="89"/>
+      <c r="U31" s="89"/>
+      <c r="V31" s="89"/>
+      <c r="W31" s="89"/>
+      <c r="X31" s="89"/>
+      <c r="Y31" s="89"/>
+      <c r="Z31" s="89"/>
+      <c r="AA31" s="89"/>
+      <c r="AB31" s="89"/>
+      <c r="AC31" s="89"/>
+      <c r="AD31" s="89"/>
+      <c r="AE31" s="90"/>
+      <c r="AF31" s="85"/>
+      <c r="AG31" s="86"/>
+      <c r="AH31" s="86"/>
+      <c r="AI31" s="87"/>
+    </row>
+    <row r="32" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="76"/>
+      <c r="B32" s="79"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="84"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="85"/>
+      <c r="K32" s="91"/>
+      <c r="L32" s="86"/>
+      <c r="M32" s="86"/>
+      <c r="N32" s="86"/>
+      <c r="O32" s="86"/>
+      <c r="P32" s="87"/>
+      <c r="Q32" s="88"/>
+      <c r="R32" s="89"/>
+      <c r="S32" s="89"/>
+      <c r="T32" s="89"/>
+      <c r="U32" s="89"/>
+      <c r="V32" s="89"/>
+      <c r="W32" s="89"/>
+      <c r="X32" s="89"/>
+      <c r="Y32" s="89"/>
+      <c r="Z32" s="89"/>
+      <c r="AA32" s="89"/>
+      <c r="AB32" s="89"/>
+      <c r="AC32" s="89"/>
+      <c r="AD32" s="89"/>
+      <c r="AE32" s="90"/>
+      <c r="AF32" s="85"/>
+      <c r="AG32" s="86"/>
+      <c r="AH32" s="86"/>
+      <c r="AI32" s="87"/>
+    </row>
+    <row r="33" spans="1:35" s="74" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="76"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="85"/>
+      <c r="K33" s="86"/>
+      <c r="L33" s="86"/>
+      <c r="M33" s="86"/>
+      <c r="N33" s="86"/>
+      <c r="O33" s="86"/>
+      <c r="P33" s="87"/>
+      <c r="Q33" s="88"/>
+      <c r="R33" s="89"/>
+      <c r="S33" s="89"/>
+      <c r="T33" s="89"/>
+      <c r="U33" s="89"/>
+      <c r="V33" s="89"/>
+      <c r="W33" s="89"/>
+      <c r="X33" s="89"/>
+      <c r="Y33" s="89"/>
+      <c r="Z33" s="89"/>
+      <c r="AA33" s="89"/>
+      <c r="AB33" s="89"/>
+      <c r="AC33" s="89"/>
+      <c r="AD33" s="89"/>
+      <c r="AE33" s="90"/>
+      <c r="AF33" s="85"/>
+      <c r="AG33" s="86"/>
+      <c r="AH33" s="86"/>
+      <c r="AI33" s="87"/>
     </row>
     <row r="34" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="K34" s="182"/>
+      <c r="K34" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="179">
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:P33"/>
-    <mergeCell ref="Q33:AE33"/>
-    <mergeCell ref="AF33:AI33"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:P32"/>
-    <mergeCell ref="Q32:AE32"/>
-    <mergeCell ref="AF32:AI32"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="Q31:AE31"/>
-    <mergeCell ref="AF31:AI31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:P30"/>
-    <mergeCell ref="Q30:AE30"/>
-    <mergeCell ref="AF30:AI30"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:P29"/>
-    <mergeCell ref="Q29:AE29"/>
-    <mergeCell ref="AF29:AI29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:P28"/>
-    <mergeCell ref="Q28:AE28"/>
-    <mergeCell ref="AF28:AI28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:P27"/>
-    <mergeCell ref="Q27:AE27"/>
-    <mergeCell ref="AF27:AI27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:P26"/>
-    <mergeCell ref="Q26:AE26"/>
-    <mergeCell ref="AF26:AI26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:P25"/>
-    <mergeCell ref="Q25:AE25"/>
-    <mergeCell ref="AF25:AI25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:P24"/>
-    <mergeCell ref="Q24:AE24"/>
-    <mergeCell ref="AF24:AI24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:P23"/>
-    <mergeCell ref="Q23:AE23"/>
-    <mergeCell ref="AF23:AI23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J22:P22"/>
-    <mergeCell ref="Q22:AE22"/>
-    <mergeCell ref="AF22:AI22"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="Q21:AE21"/>
-    <mergeCell ref="AF21:AI21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:P20"/>
-    <mergeCell ref="Q20:AE20"/>
-    <mergeCell ref="AF20:AI20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:P19"/>
-    <mergeCell ref="Q19:AE19"/>
-    <mergeCell ref="AF19:AI19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:P18"/>
-    <mergeCell ref="Q18:AE18"/>
-    <mergeCell ref="AF18:AI18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:P17"/>
-    <mergeCell ref="Q17:AE17"/>
-    <mergeCell ref="AF17:AI17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:P16"/>
-    <mergeCell ref="Q16:AE16"/>
-    <mergeCell ref="AF16:AI16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J15:P15"/>
-    <mergeCell ref="Q15:AE15"/>
-    <mergeCell ref="AF15:AI15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:P14"/>
-    <mergeCell ref="Q14:AE14"/>
-    <mergeCell ref="AF14:AI14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:P13"/>
-    <mergeCell ref="Q13:AE13"/>
-    <mergeCell ref="AF13:AI13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:P12"/>
-    <mergeCell ref="Q12:AE12"/>
-    <mergeCell ref="AF12:AI12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:P11"/>
-    <mergeCell ref="Q11:AE11"/>
-    <mergeCell ref="AF11:AI11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="J10:P10"/>
-    <mergeCell ref="Q10:AE10"/>
-    <mergeCell ref="AF10:AI10"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:P9"/>
-    <mergeCell ref="Q9:AE9"/>
-    <mergeCell ref="AF9:AI9"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:P8"/>
-    <mergeCell ref="Q8:AE8"/>
-    <mergeCell ref="AF8:AI8"/>
     <mergeCell ref="AG3:AI3"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:F7"/>
@@ -3888,6 +3730,162 @@
     <mergeCell ref="E3:N3"/>
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AC3:AF3"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:P9"/>
+    <mergeCell ref="Q9:AE9"/>
+    <mergeCell ref="AF9:AI9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:P8"/>
+    <mergeCell ref="Q8:AE8"/>
+    <mergeCell ref="AF8:AI8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:P11"/>
+    <mergeCell ref="Q11:AE11"/>
+    <mergeCell ref="AF11:AI11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:P10"/>
+    <mergeCell ref="Q10:AE10"/>
+    <mergeCell ref="AF10:AI10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:P13"/>
+    <mergeCell ref="Q13:AE13"/>
+    <mergeCell ref="AF13:AI13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:P12"/>
+    <mergeCell ref="Q12:AE12"/>
+    <mergeCell ref="AF12:AI12"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="J15:P15"/>
+    <mergeCell ref="Q15:AE15"/>
+    <mergeCell ref="AF15:AI15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="J14:P14"/>
+    <mergeCell ref="Q14:AE14"/>
+    <mergeCell ref="AF14:AI14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:P17"/>
+    <mergeCell ref="Q17:AE17"/>
+    <mergeCell ref="AF17:AI17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:P16"/>
+    <mergeCell ref="Q16:AE16"/>
+    <mergeCell ref="AF16:AI16"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:P19"/>
+    <mergeCell ref="Q19:AE19"/>
+    <mergeCell ref="AF19:AI19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:P18"/>
+    <mergeCell ref="Q18:AE18"/>
+    <mergeCell ref="AF18:AI18"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="Q21:AE21"/>
+    <mergeCell ref="AF21:AI21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:P20"/>
+    <mergeCell ref="Q20:AE20"/>
+    <mergeCell ref="AF20:AI20"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:P23"/>
+    <mergeCell ref="Q23:AE23"/>
+    <mergeCell ref="AF23:AI23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J22:P22"/>
+    <mergeCell ref="Q22:AE22"/>
+    <mergeCell ref="AF22:AI22"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:P25"/>
+    <mergeCell ref="Q25:AE25"/>
+    <mergeCell ref="AF25:AI25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:P24"/>
+    <mergeCell ref="Q24:AE24"/>
+    <mergeCell ref="AF24:AI24"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:P27"/>
+    <mergeCell ref="Q27:AE27"/>
+    <mergeCell ref="AF27:AI27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:P26"/>
+    <mergeCell ref="Q26:AE26"/>
+    <mergeCell ref="AF26:AI26"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:P29"/>
+    <mergeCell ref="Q29:AE29"/>
+    <mergeCell ref="AF29:AI29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:P28"/>
+    <mergeCell ref="Q28:AE28"/>
+    <mergeCell ref="AF28:AI28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="Q31:AE31"/>
+    <mergeCell ref="AF31:AI31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:P30"/>
+    <mergeCell ref="Q30:AE30"/>
+    <mergeCell ref="AF30:AI30"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:P33"/>
+    <mergeCell ref="Q33:AE33"/>
+    <mergeCell ref="AF33:AI33"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:P32"/>
+    <mergeCell ref="Q32:AE32"/>
+    <mergeCell ref="AF32:AI32"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <printOptions horizontalCentered="1"/>
@@ -4043,169 +4041,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="86" t="str">
+      <c r="A1" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A1")&lt;&gt;"",INDIRECT("'Revision history'!A1"),"")</f>
         <v>Project name</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="72" t="str">
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E1")&lt;&gt;"",INDIRECT("'Revision history'!E1"),"")</f>
         <v>Sample Project</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="116" t="str">
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="147" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!O1")&lt;&gt;"",INDIRECT("'Revision history'!O1"),"")</f>
         <v>Deliverable name</v>
       </c>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="118"/>
-      <c r="S1" s="119" t="str">
+      <c r="P1" s="148"/>
+      <c r="Q1" s="148"/>
+      <c r="R1" s="149"/>
+      <c r="S1" s="132" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!S1")&lt;&gt;"",INDIRECT("'Revision history'!S1"),"")</f>
         <v>System Function List</v>
       </c>
-      <c r="T1" s="120"/>
-      <c r="U1" s="120"/>
-      <c r="V1" s="120"/>
-      <c r="W1" s="120"/>
-      <c r="X1" s="120"/>
-      <c r="Y1" s="120"/>
-      <c r="Z1" s="121"/>
-      <c r="AA1" s="86" t="str">
+      <c r="T1" s="133"/>
+      <c r="U1" s="133"/>
+      <c r="V1" s="133"/>
+      <c r="W1" s="133"/>
+      <c r="X1" s="133"/>
+      <c r="Y1" s="133"/>
+      <c r="Z1" s="134"/>
+      <c r="AA1" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA1")&lt;&gt;"",INDIRECT("'Revision history'!AA1"),"")</f>
         <v>Prepared by</v>
       </c>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="183" t="str">
+      <c r="AB1" s="146"/>
+      <c r="AC1" s="159" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC1")&lt;&gt;"",INDIRECT("'Revision history'!AC1"),"")</f>
         <v>TIS</v>
       </c>
-      <c r="AD1" s="184"/>
-      <c r="AE1" s="184"/>
-      <c r="AF1" s="185"/>
-      <c r="AG1" s="186">
+      <c r="AD1" s="160"/>
+      <c r="AE1" s="160"/>
+      <c r="AF1" s="161"/>
+      <c r="AG1" s="156">
         <f ca="1">IF(INDIRECT("'Revision history'!AG1")&lt;&gt;"",INDIRECT("'Revision history'!AG1"),"")</f>
         <v>43404</v>
       </c>
-      <c r="AH1" s="187"/>
-      <c r="AI1" s="188"/>
+      <c r="AH1" s="157"/>
+      <c r="AI1" s="158"/>
       <c r="AJ1" s="17"/>
       <c r="AK1" s="17"/>
       <c r="AL1" s="26"/>
     </row>
     <row r="2" spans="1:38" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="str">
+      <c r="A2" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A2")&lt;&gt;"",INDIRECT("'Revision history'!A2"),"")</f>
         <v>System name</v>
       </c>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="72" t="str">
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E2")&lt;&gt;"",INDIRECT("'Revision history'!E2"),"")</f>
         <v>Sample System</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="123"/>
-      <c r="Q2" s="123"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="127"/>
-      <c r="AA2" s="86" t="str">
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="150"/>
+      <c r="P2" s="151"/>
+      <c r="Q2" s="151"/>
+      <c r="R2" s="152"/>
+      <c r="S2" s="135"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="136"/>
+      <c r="V2" s="136"/>
+      <c r="W2" s="136"/>
+      <c r="X2" s="136"/>
+      <c r="Y2" s="136"/>
+      <c r="Z2" s="137"/>
+      <c r="AA2" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA2")&lt;&gt;"",INDIRECT("'Revision history'!AA2"),"")</f>
         <v>Changes</v>
       </c>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="183" t="str">
+      <c r="AB2" s="146"/>
+      <c r="AC2" s="159" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC2")&lt;&gt;"",INDIRECT("'Revision history'!AC2"),"")</f>
         <v/>
       </c>
-      <c r="AD2" s="184"/>
-      <c r="AE2" s="184"/>
-      <c r="AF2" s="185"/>
-      <c r="AG2" s="186" t="str">
+      <c r="AD2" s="160"/>
+      <c r="AE2" s="160"/>
+      <c r="AF2" s="161"/>
+      <c r="AG2" s="156" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG2")&lt;&gt;"",INDIRECT("'Revision history'!AG2"),"")</f>
         <v/>
       </c>
-      <c r="AH2" s="187"/>
-      <c r="AI2" s="188"/>
+      <c r="AH2" s="157"/>
+      <c r="AI2" s="158"/>
       <c r="AJ2" s="17"/>
       <c r="AK2" s="17"/>
       <c r="AL2" s="17"/>
     </row>
     <row r="3" spans="1:38" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="86" t="str">
+      <c r="A3" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A3")&lt;&gt;"",INDIRECT("'Revision history'!A3"),"")</f>
         <v>Sub-system name</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="72" t="str">
+      <c r="B3" s="145"/>
+      <c r="C3" s="145"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E3")&lt;&gt;"",INDIRECT("'Revision history'!E3"),"")</f>
         <v>Client Management System</v>
       </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="128"/>
-      <c r="P3" s="129"/>
-      <c r="Q3" s="129"/>
-      <c r="R3" s="130"/>
-      <c r="S3" s="131"/>
-      <c r="T3" s="132"/>
-      <c r="U3" s="132"/>
-      <c r="V3" s="132"/>
-      <c r="W3" s="132"/>
-      <c r="X3" s="132"/>
-      <c r="Y3" s="132"/>
-      <c r="Z3" s="133"/>
-      <c r="AA3" s="86"/>
-      <c r="AB3" s="87"/>
-      <c r="AC3" s="183" t="str">
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="154"/>
+      <c r="Q3" s="154"/>
+      <c r="R3" s="155"/>
+      <c r="S3" s="138"/>
+      <c r="T3" s="139"/>
+      <c r="U3" s="139"/>
+      <c r="V3" s="139"/>
+      <c r="W3" s="139"/>
+      <c r="X3" s="139"/>
+      <c r="Y3" s="139"/>
+      <c r="Z3" s="140"/>
+      <c r="AA3" s="144"/>
+      <c r="AB3" s="146"/>
+      <c r="AC3" s="159" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC3")&lt;&gt;"",INDIRECT("'Revision history'!AC3"),"")</f>
         <v/>
       </c>
-      <c r="AD3" s="184"/>
-      <c r="AE3" s="184"/>
-      <c r="AF3" s="185"/>
-      <c r="AG3" s="186" t="str">
+      <c r="AD3" s="160"/>
+      <c r="AE3" s="160"/>
+      <c r="AF3" s="161"/>
+      <c r="AG3" s="156" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG3")&lt;&gt;"",INDIRECT("'Revision history'!AG3"),"")</f>
         <v/>
       </c>
-      <c r="AH3" s="187"/>
-      <c r="AI3" s="188"/>
+      <c r="AH3" s="157"/>
+      <c r="AI3" s="158"/>
       <c r="AJ3" s="17"/>
       <c r="AK3" s="17"/>
       <c r="AL3" s="17"/>
@@ -5668,6 +5666,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AG1:AI1"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AF3"/>
+    <mergeCell ref="AG3:AI3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:N1"/>
     <mergeCell ref="O1:R3"/>
@@ -5677,14 +5683,6 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E2:N2"/>
     <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AG1:AI1"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="E3:N3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AF3"/>
-    <mergeCell ref="AG3:AI3"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <printOptions horizontalCentered="1"/>
@@ -5710,169 +5708,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="86" t="str">
+      <c r="A1" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A1")&lt;&gt;"",INDIRECT("'Revision history'!A1"),"")</f>
         <v>Project name</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="72" t="str">
+      <c r="B1" s="145"/>
+      <c r="C1" s="145"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E1")&lt;&gt;"",INDIRECT("'Revision history'!E1"),"")</f>
         <v>Sample Project</v>
       </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="116" t="str">
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
+      <c r="K1" s="118"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="147" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!O1")&lt;&gt;"",INDIRECT("'Revision history'!O1"),"")</f>
         <v>Deliverable name</v>
       </c>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="118"/>
-      <c r="S1" s="119" t="str">
+      <c r="P1" s="148"/>
+      <c r="Q1" s="148"/>
+      <c r="R1" s="149"/>
+      <c r="S1" s="132" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!S1")&lt;&gt;"",INDIRECT("'Revision history'!S1"),"")</f>
         <v>System Function List</v>
       </c>
-      <c r="T1" s="120"/>
-      <c r="U1" s="120"/>
-      <c r="V1" s="120"/>
-      <c r="W1" s="120"/>
-      <c r="X1" s="120"/>
-      <c r="Y1" s="120"/>
-      <c r="Z1" s="121"/>
-      <c r="AA1" s="86" t="str">
+      <c r="T1" s="133"/>
+      <c r="U1" s="133"/>
+      <c r="V1" s="133"/>
+      <c r="W1" s="133"/>
+      <c r="X1" s="133"/>
+      <c r="Y1" s="133"/>
+      <c r="Z1" s="134"/>
+      <c r="AA1" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA1")&lt;&gt;"",INDIRECT("'Revision history'!AA1"),"")</f>
         <v>Prepared by</v>
       </c>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="183" t="str">
+      <c r="AB1" s="146"/>
+      <c r="AC1" s="159" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC1")&lt;&gt;"",INDIRECT("'Revision history'!AC1"),"")</f>
         <v>TIS</v>
       </c>
-      <c r="AD1" s="184"/>
-      <c r="AE1" s="184"/>
-      <c r="AF1" s="185"/>
-      <c r="AG1" s="186">
+      <c r="AD1" s="160"/>
+      <c r="AE1" s="160"/>
+      <c r="AF1" s="161"/>
+      <c r="AG1" s="156">
         <f ca="1">IF(INDIRECT("'Revision history'!AG1")&lt;&gt;"",INDIRECT("'Revision history'!AG1"),"")</f>
         <v>43404</v>
       </c>
-      <c r="AH1" s="187"/>
-      <c r="AI1" s="188"/>
+      <c r="AH1" s="157"/>
+      <c r="AI1" s="158"/>
       <c r="AJ1" s="17"/>
       <c r="AK1" s="17"/>
       <c r="AL1" s="17"/>
     </row>
     <row r="2" spans="1:42" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="str">
+      <c r="A2" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A2")&lt;&gt;"",INDIRECT("'Revision history'!A2"),"")</f>
         <v>System name</v>
       </c>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="72" t="str">
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E2")&lt;&gt;"",INDIRECT("'Revision history'!E2"),"")</f>
         <v>Sample System</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="123"/>
-      <c r="Q2" s="123"/>
-      <c r="R2" s="124"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="127"/>
-      <c r="AA2" s="86" t="str">
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="150"/>
+      <c r="P2" s="151"/>
+      <c r="Q2" s="151"/>
+      <c r="R2" s="152"/>
+      <c r="S2" s="135"/>
+      <c r="T2" s="136"/>
+      <c r="U2" s="136"/>
+      <c r="V2" s="136"/>
+      <c r="W2" s="136"/>
+      <c r="X2" s="136"/>
+      <c r="Y2" s="136"/>
+      <c r="Z2" s="137"/>
+      <c r="AA2" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA2")&lt;&gt;"",INDIRECT("'Revision history'!AA2"),"")</f>
         <v>Changes</v>
       </c>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="183" t="str">
+      <c r="AB2" s="146"/>
+      <c r="AC2" s="159" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC2")&lt;&gt;"",INDIRECT("'Revision history'!AC2"),"")</f>
         <v/>
       </c>
-      <c r="AD2" s="184"/>
-      <c r="AE2" s="184"/>
-      <c r="AF2" s="185"/>
-      <c r="AG2" s="186" t="str">
+      <c r="AD2" s="160"/>
+      <c r="AE2" s="160"/>
+      <c r="AF2" s="161"/>
+      <c r="AG2" s="156" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG2")&lt;&gt;"",INDIRECT("'Revision history'!AG2"),"")</f>
         <v/>
       </c>
-      <c r="AH2" s="187"/>
-      <c r="AI2" s="188"/>
+      <c r="AH2" s="157"/>
+      <c r="AI2" s="158"/>
       <c r="AJ2" s="17"/>
       <c r="AK2" s="17"/>
       <c r="AL2" s="17"/>
     </row>
     <row r="3" spans="1:42" s="18" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="86" t="str">
+      <c r="A3" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A3")&lt;&gt;"",INDIRECT("'Revision history'!A3"),"")</f>
         <v>Sub-system name</v>
       </c>
-      <c r="B3" s="115"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="72" t="str">
+      <c r="B3" s="145"/>
+      <c r="C3" s="145"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E3")&lt;&gt;"",INDIRECT("'Revision history'!E3"),"")</f>
         <v>Client Management System</v>
       </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="74"/>
-      <c r="O3" s="128"/>
-      <c r="P3" s="129"/>
-      <c r="Q3" s="129"/>
-      <c r="R3" s="130"/>
-      <c r="S3" s="131"/>
-      <c r="T3" s="132"/>
-      <c r="U3" s="132"/>
-      <c r="V3" s="132"/>
-      <c r="W3" s="132"/>
-      <c r="X3" s="132"/>
-      <c r="Y3" s="132"/>
-      <c r="Z3" s="133"/>
-      <c r="AA3" s="86"/>
-      <c r="AB3" s="87"/>
-      <c r="AC3" s="183" t="str">
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="153"/>
+      <c r="P3" s="154"/>
+      <c r="Q3" s="154"/>
+      <c r="R3" s="155"/>
+      <c r="S3" s="138"/>
+      <c r="T3" s="139"/>
+      <c r="U3" s="139"/>
+      <c r="V3" s="139"/>
+      <c r="W3" s="139"/>
+      <c r="X3" s="139"/>
+      <c r="Y3" s="139"/>
+      <c r="Z3" s="140"/>
+      <c r="AA3" s="144"/>
+      <c r="AB3" s="146"/>
+      <c r="AC3" s="159" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC3")&lt;&gt;"",INDIRECT("'Revision history'!AC3"),"")</f>
         <v/>
       </c>
-      <c r="AD3" s="184"/>
-      <c r="AE3" s="184"/>
-      <c r="AF3" s="185"/>
-      <c r="AG3" s="186" t="str">
+      <c r="AD3" s="160"/>
+      <c r="AE3" s="160"/>
+      <c r="AF3" s="161"/>
+      <c r="AG3" s="156" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG3")&lt;&gt;"",INDIRECT("'Revision history'!AG3"),"")</f>
         <v/>
       </c>
-      <c r="AH3" s="187"/>
-      <c r="AI3" s="188"/>
+      <c r="AH3" s="157"/>
+      <c r="AI3" s="158"/>
       <c r="AJ3" s="17"/>
       <c r="AK3" s="17"/>
       <c r="AL3" s="17"/>
@@ -5884,268 +5882,268 @@
     </row>
     <row r="6" spans="1:42" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:42" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="187" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="102" t="s">
+      <c r="D7" s="177" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="103"/>
-      <c r="F7" s="88" t="s">
+      <c r="E7" s="179"/>
+      <c r="F7" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="89"/>
-      <c r="H7" s="89"/>
-      <c r="I7" s="89"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="88" t="s">
+      <c r="G7" s="172"/>
+      <c r="H7" s="172"/>
+      <c r="I7" s="172"/>
+      <c r="J7" s="173"/>
+      <c r="K7" s="171" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="89"/>
-      <c r="M7" s="89"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="89"/>
-      <c r="P7" s="89"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="106" t="s">
+      <c r="L7" s="172"/>
+      <c r="M7" s="172"/>
+      <c r="N7" s="172"/>
+      <c r="O7" s="172"/>
+      <c r="P7" s="172"/>
+      <c r="Q7" s="173"/>
+      <c r="R7" s="183" t="s">
         <v>22</v>
       </c>
-      <c r="S7" s="107"/>
-      <c r="T7" s="88" t="s">
+      <c r="S7" s="184"/>
+      <c r="T7" s="171" t="s">
         <v>23</v>
       </c>
-      <c r="U7" s="89"/>
-      <c r="V7" s="89"/>
-      <c r="W7" s="89"/>
-      <c r="X7" s="89"/>
-      <c r="Y7" s="90"/>
-      <c r="Z7" s="88" t="s">
+      <c r="U7" s="172"/>
+      <c r="V7" s="172"/>
+      <c r="W7" s="172"/>
+      <c r="X7" s="172"/>
+      <c r="Y7" s="173"/>
+      <c r="Z7" s="171" t="s">
         <v>24</v>
       </c>
-      <c r="AA7" s="89"/>
-      <c r="AB7" s="89"/>
-      <c r="AC7" s="89"/>
-      <c r="AD7" s="89"/>
-      <c r="AE7" s="89"/>
-      <c r="AF7" s="89"/>
-      <c r="AG7" s="90"/>
-      <c r="AH7" s="102" t="s">
+      <c r="AA7" s="172"/>
+      <c r="AB7" s="172"/>
+      <c r="AC7" s="172"/>
+      <c r="AD7" s="172"/>
+      <c r="AE7" s="172"/>
+      <c r="AF7" s="172"/>
+      <c r="AG7" s="173"/>
+      <c r="AH7" s="177" t="s">
         <v>7</v>
       </c>
-      <c r="AI7" s="110"/>
-      <c r="AJ7" s="103"/>
-      <c r="AK7" s="88" t="s">
+      <c r="AI7" s="178"/>
+      <c r="AJ7" s="179"/>
+      <c r="AK7" s="171" t="s">
         <v>8</v>
       </c>
-      <c r="AL7" s="89"/>
-      <c r="AM7" s="89"/>
-      <c r="AN7" s="89"/>
-      <c r="AO7" s="89"/>
-      <c r="AP7" s="90"/>
+      <c r="AL7" s="172"/>
+      <c r="AM7" s="172"/>
+      <c r="AN7" s="172"/>
+      <c r="AO7" s="172"/>
+      <c r="AP7" s="173"/>
     </row>
     <row r="8" spans="1:42" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="95"/>
-      <c r="D8" s="104"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="92"/>
-      <c r="M8" s="92"/>
-      <c r="N8" s="92"/>
-      <c r="O8" s="92"/>
-      <c r="P8" s="92"/>
-      <c r="Q8" s="93"/>
-      <c r="R8" s="108"/>
-      <c r="S8" s="109"/>
-      <c r="T8" s="91"/>
-      <c r="U8" s="92"/>
-      <c r="V8" s="92"/>
-      <c r="W8" s="92"/>
-      <c r="X8" s="92"/>
-      <c r="Y8" s="93"/>
-      <c r="Z8" s="91"/>
-      <c r="AA8" s="92"/>
-      <c r="AB8" s="92"/>
-      <c r="AC8" s="92"/>
-      <c r="AD8" s="92"/>
-      <c r="AE8" s="92"/>
-      <c r="AF8" s="92"/>
-      <c r="AG8" s="93"/>
-      <c r="AH8" s="104"/>
-      <c r="AI8" s="111"/>
-      <c r="AJ8" s="105"/>
-      <c r="AK8" s="91"/>
-      <c r="AL8" s="92"/>
-      <c r="AM8" s="92"/>
-      <c r="AN8" s="92"/>
-      <c r="AO8" s="92"/>
-      <c r="AP8" s="93"/>
+      <c r="C8" s="188"/>
+      <c r="D8" s="180"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="174"/>
+      <c r="G8" s="175"/>
+      <c r="H8" s="175"/>
+      <c r="I8" s="175"/>
+      <c r="J8" s="176"/>
+      <c r="K8" s="174"/>
+      <c r="L8" s="175"/>
+      <c r="M8" s="175"/>
+      <c r="N8" s="175"/>
+      <c r="O8" s="175"/>
+      <c r="P8" s="175"/>
+      <c r="Q8" s="176"/>
+      <c r="R8" s="185"/>
+      <c r="S8" s="186"/>
+      <c r="T8" s="174"/>
+      <c r="U8" s="175"/>
+      <c r="V8" s="175"/>
+      <c r="W8" s="175"/>
+      <c r="X8" s="175"/>
+      <c r="Y8" s="176"/>
+      <c r="Z8" s="174"/>
+      <c r="AA8" s="175"/>
+      <c r="AB8" s="175"/>
+      <c r="AC8" s="175"/>
+      <c r="AD8" s="175"/>
+      <c r="AE8" s="175"/>
+      <c r="AF8" s="175"/>
+      <c r="AG8" s="176"/>
+      <c r="AH8" s="180"/>
+      <c r="AI8" s="181"/>
+      <c r="AJ8" s="182"/>
+      <c r="AK8" s="174"/>
+      <c r="AL8" s="175"/>
+      <c r="AM8" s="175"/>
+      <c r="AN8" s="175"/>
+      <c r="AO8" s="175"/>
+      <c r="AP8" s="176"/>
     </row>
     <row r="9" spans="1:42" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="20">
         <v>1</v>
       </c>
-      <c r="D9" s="96" t="s">
+      <c r="D9" s="168" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="97"/>
-      <c r="F9" s="96" t="s">
+      <c r="E9" s="169"/>
+      <c r="F9" s="168" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="97"/>
-      <c r="K9" s="96" t="s">
+      <c r="G9" s="170"/>
+      <c r="H9" s="170"/>
+      <c r="I9" s="170"/>
+      <c r="J9" s="169"/>
+      <c r="K9" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101"/>
-      <c r="N9" s="101"/>
-      <c r="O9" s="101"/>
-      <c r="P9" s="101"/>
-      <c r="Q9" s="97"/>
-      <c r="R9" s="98" t="s">
+      <c r="L9" s="170"/>
+      <c r="M9" s="170"/>
+      <c r="N9" s="170"/>
+      <c r="O9" s="170"/>
+      <c r="P9" s="170"/>
+      <c r="Q9" s="169"/>
+      <c r="R9" s="165" t="s">
         <v>12</v>
       </c>
-      <c r="S9" s="100"/>
-      <c r="T9" s="98" t="s">
+      <c r="S9" s="167"/>
+      <c r="T9" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="U9" s="99"/>
-      <c r="V9" s="99"/>
-      <c r="W9" s="99"/>
-      <c r="X9" s="99"/>
-      <c r="Y9" s="100"/>
-      <c r="Z9" s="98" t="s">
+      <c r="U9" s="166"/>
+      <c r="V9" s="166"/>
+      <c r="W9" s="166"/>
+      <c r="X9" s="166"/>
+      <c r="Y9" s="167"/>
+      <c r="Z9" s="165" t="s">
         <v>14</v>
       </c>
-      <c r="AA9" s="99"/>
-      <c r="AB9" s="99"/>
-      <c r="AC9" s="99"/>
-      <c r="AD9" s="99"/>
-      <c r="AE9" s="99"/>
-      <c r="AF9" s="99"/>
-      <c r="AG9" s="100"/>
-      <c r="AH9" s="98" t="s">
+      <c r="AA9" s="166"/>
+      <c r="AB9" s="166"/>
+      <c r="AC9" s="166"/>
+      <c r="AD9" s="166"/>
+      <c r="AE9" s="166"/>
+      <c r="AF9" s="166"/>
+      <c r="AG9" s="167"/>
+      <c r="AH9" s="165" t="s">
         <v>15</v>
       </c>
-      <c r="AI9" s="99"/>
-      <c r="AJ9" s="100"/>
-      <c r="AK9" s="98"/>
-      <c r="AL9" s="99"/>
-      <c r="AM9" s="99"/>
-      <c r="AN9" s="99"/>
-      <c r="AO9" s="99"/>
-      <c r="AP9" s="100"/>
+      <c r="AI9" s="166"/>
+      <c r="AJ9" s="167"/>
+      <c r="AK9" s="165"/>
+      <c r="AL9" s="166"/>
+      <c r="AM9" s="166"/>
+      <c r="AN9" s="166"/>
+      <c r="AO9" s="166"/>
+      <c r="AP9" s="167"/>
     </row>
     <row r="10" spans="1:42" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="20">
         <v>2</v>
       </c>
-      <c r="D10" s="112"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="114"/>
-      <c r="H10" s="114"/>
-      <c r="I10" s="114"/>
-      <c r="J10" s="113"/>
-      <c r="K10" s="112"/>
-      <c r="L10" s="114"/>
-      <c r="M10" s="114"/>
-      <c r="N10" s="114"/>
-      <c r="O10" s="114"/>
-      <c r="P10" s="114"/>
-      <c r="Q10" s="113"/>
-      <c r="R10" s="98" t="s">
+      <c r="D10" s="162"/>
+      <c r="E10" s="163"/>
+      <c r="F10" s="162"/>
+      <c r="G10" s="164"/>
+      <c r="H10" s="164"/>
+      <c r="I10" s="164"/>
+      <c r="J10" s="163"/>
+      <c r="K10" s="162"/>
+      <c r="L10" s="164"/>
+      <c r="M10" s="164"/>
+      <c r="N10" s="164"/>
+      <c r="O10" s="164"/>
+      <c r="P10" s="164"/>
+      <c r="Q10" s="163"/>
+      <c r="R10" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="S10" s="100"/>
-      <c r="T10" s="98" t="s">
+      <c r="S10" s="167"/>
+      <c r="T10" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="U10" s="99"/>
-      <c r="V10" s="99"/>
-      <c r="W10" s="99"/>
-      <c r="X10" s="99"/>
-      <c r="Y10" s="100"/>
-      <c r="Z10" s="98" t="s">
+      <c r="U10" s="166"/>
+      <c r="V10" s="166"/>
+      <c r="W10" s="166"/>
+      <c r="X10" s="166"/>
+      <c r="Y10" s="167"/>
+      <c r="Z10" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="AA10" s="99"/>
-      <c r="AB10" s="99"/>
-      <c r="AC10" s="99"/>
-      <c r="AD10" s="99"/>
-      <c r="AE10" s="99"/>
-      <c r="AF10" s="99"/>
-      <c r="AG10" s="100"/>
-      <c r="AH10" s="98" t="s">
+      <c r="AA10" s="166"/>
+      <c r="AB10" s="166"/>
+      <c r="AC10" s="166"/>
+      <c r="AD10" s="166"/>
+      <c r="AE10" s="166"/>
+      <c r="AF10" s="166"/>
+      <c r="AG10" s="167"/>
+      <c r="AH10" s="165" t="s">
         <v>15</v>
       </c>
-      <c r="AI10" s="99"/>
-      <c r="AJ10" s="100"/>
-      <c r="AK10" s="98"/>
-      <c r="AL10" s="99"/>
-      <c r="AM10" s="99"/>
-      <c r="AN10" s="99"/>
-      <c r="AO10" s="99"/>
-      <c r="AP10" s="100"/>
+      <c r="AI10" s="166"/>
+      <c r="AJ10" s="167"/>
+      <c r="AK10" s="165"/>
+      <c r="AL10" s="166"/>
+      <c r="AM10" s="166"/>
+      <c r="AN10" s="166"/>
+      <c r="AO10" s="166"/>
+      <c r="AP10" s="167"/>
     </row>
     <row r="11" spans="1:42" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="21">
         <v>3</v>
       </c>
-      <c r="D11" s="112"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="112"/>
-      <c r="G11" s="114"/>
-      <c r="H11" s="114"/>
-      <c r="I11" s="114"/>
-      <c r="J11" s="113"/>
-      <c r="K11" s="112"/>
-      <c r="L11" s="114"/>
-      <c r="M11" s="114"/>
-      <c r="N11" s="114"/>
-      <c r="O11" s="114"/>
-      <c r="P11" s="114"/>
-      <c r="Q11" s="113"/>
-      <c r="R11" s="96" t="s">
+      <c r="D11" s="162"/>
+      <c r="E11" s="163"/>
+      <c r="F11" s="162"/>
+      <c r="G11" s="164"/>
+      <c r="H11" s="164"/>
+      <c r="I11" s="164"/>
+      <c r="J11" s="163"/>
+      <c r="K11" s="162"/>
+      <c r="L11" s="164"/>
+      <c r="M11" s="164"/>
+      <c r="N11" s="164"/>
+      <c r="O11" s="164"/>
+      <c r="P11" s="164"/>
+      <c r="Q11" s="163"/>
+      <c r="R11" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="S11" s="97"/>
-      <c r="T11" s="96" t="s">
+      <c r="S11" s="169"/>
+      <c r="T11" s="168" t="s">
         <v>20</v>
       </c>
-      <c r="U11" s="101"/>
-      <c r="V11" s="101"/>
-      <c r="W11" s="101"/>
-      <c r="X11" s="101"/>
-      <c r="Y11" s="97"/>
-      <c r="Z11" s="98" t="s">
+      <c r="U11" s="170"/>
+      <c r="V11" s="170"/>
+      <c r="W11" s="170"/>
+      <c r="X11" s="170"/>
+      <c r="Y11" s="169"/>
+      <c r="Z11" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="AA11" s="99"/>
-      <c r="AB11" s="99"/>
-      <c r="AC11" s="99"/>
-      <c r="AD11" s="99"/>
-      <c r="AE11" s="99"/>
-      <c r="AF11" s="99"/>
-      <c r="AG11" s="100"/>
-      <c r="AH11" s="98" t="s">
+      <c r="AA11" s="166"/>
+      <c r="AB11" s="166"/>
+      <c r="AC11" s="166"/>
+      <c r="AD11" s="166"/>
+      <c r="AE11" s="166"/>
+      <c r="AF11" s="166"/>
+      <c r="AG11" s="167"/>
+      <c r="AH11" s="165" t="s">
         <v>15</v>
       </c>
-      <c r="AI11" s="99"/>
-      <c r="AJ11" s="100"/>
-      <c r="AK11" s="98"/>
-      <c r="AL11" s="99"/>
-      <c r="AM11" s="99"/>
-      <c r="AN11" s="99"/>
-      <c r="AO11" s="99"/>
-      <c r="AP11" s="100"/>
+      <c r="AI11" s="166"/>
+      <c r="AJ11" s="167"/>
+      <c r="AK11" s="165"/>
+      <c r="AL11" s="166"/>
+      <c r="AM11" s="166"/>
+      <c r="AN11" s="166"/>
+      <c r="AO11" s="166"/>
+      <c r="AP11" s="167"/>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12" s="22"/>
@@ -6726,24 +6724,22 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="K10:Q10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="K11:Q11"/>
-    <mergeCell ref="AK10:AP10"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="T11:Y11"/>
-    <mergeCell ref="Z11:AG11"/>
-    <mergeCell ref="AH11:AJ11"/>
-    <mergeCell ref="AK11:AP11"/>
-    <mergeCell ref="Z7:AG8"/>
-    <mergeCell ref="AH7:AJ8"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="T10:Y10"/>
-    <mergeCell ref="Z10:AG10"/>
-    <mergeCell ref="AH10:AJ10"/>
+    <mergeCell ref="K7:Q8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="AK7:AP8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="AH9:AJ9"/>
+    <mergeCell ref="O1:R3"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="T9:Y9"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="K9:Q9"/>
+    <mergeCell ref="E1:N1"/>
+    <mergeCell ref="E2:N2"/>
+    <mergeCell ref="E3:N3"/>
     <mergeCell ref="D7:E8"/>
     <mergeCell ref="F7:J8"/>
     <mergeCell ref="AK9:AP9"/>
@@ -6760,22 +6756,24 @@
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="R7:S8"/>
     <mergeCell ref="T7:Y8"/>
-    <mergeCell ref="K7:Q8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="AK7:AP8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="AH9:AJ9"/>
-    <mergeCell ref="O1:R3"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="T9:Y9"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="K9:Q9"/>
-    <mergeCell ref="E1:N1"/>
-    <mergeCell ref="E2:N2"/>
-    <mergeCell ref="E3:N3"/>
+    <mergeCell ref="Z7:AG8"/>
+    <mergeCell ref="AH7:AJ8"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="T10:Y10"/>
+    <mergeCell ref="Z10:AG10"/>
+    <mergeCell ref="AH10:AJ10"/>
+    <mergeCell ref="AK10:AP10"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="T11:Y11"/>
+    <mergeCell ref="Z11:AG11"/>
+    <mergeCell ref="AH11:AJ11"/>
+    <mergeCell ref="AK11:AP11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="K10:Q10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:J11"/>
+    <mergeCell ref="K11:Q11"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>

</xml_diff>